<commit_message>
Shows the loop for facilities correctly now
</commit_message>
<xml_diff>
--- a/Anand_Work/FallWork2018/OUTPUT.xlsx
+++ b/Anand_Work/FallWork2018/OUTPUT.xlsx
@@ -911,7 +911,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AW17"/>
+  <dimension ref="A1:AW15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1217,6 +1217,7 @@
         <v>0</v>
       </c>
       <c r="AV5" s="1"/>
+      <c r="AW5" s="1"/>
     </row>
     <row r="6" spans="1:49">
       <c r="AN6" s="1"/>
@@ -1224,71 +1225,225 @@
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
       <c r="AR6" s="1"/>
-      <c r="AS6" s="1"/>
+      <c r="AS6" s="1">
+        <v>0</v>
+      </c>
       <c r="AT6" s="1">
         <v>0</v>
       </c>
       <c r="AU6" s="1">
         <v>0</v>
       </c>
-      <c r="AV6" s="1">
-        <v>0</v>
-      </c>
+      <c r="AV6" s="1"/>
     </row>
     <row r="7" spans="1:49">
-      <c r="AN7" s="1"/>
-      <c r="AO7" s="1"/>
-      <c r="AP7" s="1"/>
-      <c r="AQ7" s="1"/>
-      <c r="AR7" s="1"/>
-      <c r="AS7" s="1"/>
-      <c r="AT7" s="1"/>
-      <c r="AU7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV7" s="1">
-        <v>0</v>
+      <c r="A7">
+        <v>43381.70964120371</v>
+      </c>
+      <c r="B7">
+        <v>43381.71162037037</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>171</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>43381.71163194445</v>
+      </c>
+      <c r="I7" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7">
+        <v>40.7180023193359</v>
+      </c>
+      <c r="O7">
+        <v>-74.0754013061523</v>
+      </c>
+      <c r="P7" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" t="s">
+        <v>61</v>
+      </c>
+      <c r="S7" t="s">
+        <v>62</v>
+      </c>
+      <c r="U7" t="s">
+        <v>63</v>
+      </c>
+      <c r="V7" t="s">
+        <v>64</v>
+      </c>
+      <c r="W7" t="s">
+        <v>65</v>
+      </c>
+      <c r="X7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:49">
-      <c r="AN8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO8" s="1"/>
+      <c r="A8">
+        <v>43381.71248842592</v>
+      </c>
+      <c r="B8">
+        <v>43381.715</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>216</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>43381.715</v>
+      </c>
+      <c r="I8" t="s">
+        <v>71</v>
+      </c>
+      <c r="N8">
+        <v>45.5653076171875</v>
+      </c>
+      <c r="O8">
+        <v>-122.644798278808</v>
+      </c>
+      <c r="P8" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>52</v>
+      </c>
+      <c r="R8" t="s">
+        <v>72</v>
+      </c>
+      <c r="S8" t="s">
+        <v>73</v>
+      </c>
+      <c r="U8" t="s">
+        <v>74</v>
+      </c>
+      <c r="V8" t="s">
+        <v>75</v>
+      </c>
+      <c r="W8" t="s">
+        <v>76</v>
+      </c>
+      <c r="X8" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE8">
+        <v>97055</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:49">
       <c r="A9">
-        <v>43381.70964120371</v>
+        <v>43381.71474537037</v>
       </c>
       <c r="B9">
-        <v>43381.71162037037</v>
+        <v>43381.71667824074</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="E9">
         <v>100</v>
       </c>
       <c r="F9">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
-        <v>43381.71163194445</v>
+        <v>43381.71667824074</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="N9">
-        <v>40.7180023193359</v>
+        <v>44.0682067871093</v>
       </c>
       <c r="O9">
-        <v>-74.0754013061523</v>
+        <v>-123.081901550292</v>
       </c>
       <c r="P9" t="s">
         <v>60</v>
@@ -1297,34 +1452,49 @@
         <v>52</v>
       </c>
       <c r="R9" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="S9" t="s">
-        <v>62</v>
-      </c>
-      <c r="U9" t="s">
-        <v>63</v>
+        <v>89</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="V9" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="W9" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="X9" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="Y9" t="s">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="Z9" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="AA9" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="AB9" t="s">
-        <v>69</v>
+        <v>96</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE9">
+        <v>97419</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>99</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>100</v>
       </c>
       <c r="AH9" t="s">
         <v>54</v>
@@ -1333,42 +1503,42 @@
         <v>55</v>
       </c>
       <c r="AL9" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:49">
       <c r="A10">
-        <v>43381.71248842592</v>
+        <v>43381.71635416667</v>
       </c>
       <c r="B10">
-        <v>43381.715</v>
+        <v>43381.72159722223</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="E10">
         <v>100</v>
       </c>
       <c r="F10">
-        <v>216</v>
+        <v>452</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>43381.715</v>
+        <v>43381.72159722223</v>
       </c>
       <c r="I10" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="N10">
-        <v>45.5653076171875</v>
+        <v>45.3726959228515</v>
       </c>
       <c r="O10">
-        <v>-122.644798278808</v>
+        <v>-122.76309967041</v>
       </c>
       <c r="P10" t="s">
         <v>60</v>
@@ -1377,49 +1547,46 @@
         <v>52</v>
       </c>
       <c r="R10" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="S10" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="U10" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="V10" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="W10" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="X10" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="Y10" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="AA10" t="s">
         <v>80</v>
       </c>
       <c r="AB10" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="AC10" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="AD10" t="s">
         <v>83</v>
       </c>
       <c r="AE10">
-        <v>97055</v>
+        <v>97064</v>
       </c>
       <c r="AF10" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="AG10" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="AH10" t="s">
         <v>54</v>
@@ -1433,37 +1600,37 @@
     </row>
     <row r="11" spans="1:49">
       <c r="A11">
-        <v>43381.71474537037</v>
+        <v>43381.74771990741</v>
       </c>
       <c r="B11">
-        <v>43381.71667824074</v>
+        <v>43381.75016203704</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="E11">
         <v>100</v>
       </c>
       <c r="F11">
-        <v>166</v>
+        <v>211</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
-        <v>43381.71667824074</v>
+        <v>43381.75016203704</v>
       </c>
       <c r="I11" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="N11">
-        <v>44.0682067871093</v>
+        <v>45.3493957519531</v>
       </c>
       <c r="O11">
-        <v>-123.081901550292</v>
+        <v>-117.212799072265</v>
       </c>
       <c r="P11" t="s">
         <v>60</v>
@@ -1472,93 +1639,81 @@
         <v>52</v>
       </c>
       <c r="R11" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="S11" t="s">
-        <v>89</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>90</v>
+        <v>117</v>
+      </c>
+      <c r="U11" t="s">
+        <v>118</v>
       </c>
       <c r="V11" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="W11" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="X11" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="Y11" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="Z11" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="AA11" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="AB11" t="s">
-        <v>96</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>98</v>
-      </c>
-      <c r="AE11">
-        <v>97419</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>99</v>
-      </c>
-      <c r="AG11" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="AH11" t="s">
-        <v>54</v>
+        <v>124</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>125</v>
       </c>
       <c r="AJ11" t="s">
         <v>55</v>
       </c>
       <c r="AL11" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:49">
       <c r="A12">
-        <v>43381.71635416667</v>
+        <v>43381.7379050926</v>
       </c>
       <c r="B12">
-        <v>43381.72159722223</v>
+        <v>43381.75645833334</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="E12">
         <v>100</v>
       </c>
       <c r="F12">
-        <v>452</v>
+        <v>1603</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12">
-        <v>43381.72159722223</v>
+        <v>43381.75645833334</v>
       </c>
       <c r="I12" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="N12">
-        <v>45.3726959228515</v>
+        <v>38.4797058105468</v>
       </c>
       <c r="O12">
-        <v>-122.76309967041</v>
+        <v>-121.443801879882</v>
       </c>
       <c r="P12" t="s">
         <v>60</v>
@@ -1567,46 +1722,37 @@
         <v>52</v>
       </c>
       <c r="R12" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="S12" t="s">
-        <v>105</v>
+        <v>130</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
       </c>
       <c r="U12" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="V12" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="W12" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="X12" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="Y12" t="s">
-        <v>110</v>
+        <v>129</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>135</v>
       </c>
       <c r="AA12" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="AB12" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>112</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>83</v>
-      </c>
-      <c r="AE12">
-        <v>97064</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>113</v>
-      </c>
-      <c r="AG12" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="AH12" t="s">
         <v>54</v>
@@ -1615,42 +1761,69 @@
         <v>55</v>
       </c>
       <c r="AL12" t="s">
-        <v>56</v>
+        <v>126</v>
+      </c>
+      <c r="AN12" t="s">
+        <v>137</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>138</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>139</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS12">
+        <v>40</v>
+      </c>
+      <c r="AT12">
+        <v>40</v>
+      </c>
+      <c r="AU12">
+        <v>20</v>
+      </c>
+      <c r="AV12">
+        <v>1500</v>
+      </c>
+      <c r="AW12">
+        <v>1700</v>
       </c>
     </row>
     <row r="13" spans="1:49">
       <c r="A13">
-        <v>43381.74771990741</v>
+        <v>43381.87571759259</v>
       </c>
       <c r="B13">
-        <v>43381.75016203704</v>
+        <v>43381.88489583333</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="E13">
         <v>100</v>
       </c>
       <c r="F13">
-        <v>211</v>
+        <v>793</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13">
-        <v>43381.75016203704</v>
+        <v>43381.88489583333</v>
       </c>
       <c r="I13" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="N13">
-        <v>45.3493957519531</v>
+        <v>45.5440979003906</v>
       </c>
       <c r="O13">
-        <v>-117.212799072265</v>
+        <v>-122.642303466796</v>
       </c>
       <c r="P13" t="s">
         <v>60</v>
@@ -1659,81 +1832,93 @@
         <v>52</v>
       </c>
       <c r="R13" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="S13" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="U13" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="V13" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="W13" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="X13" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="Y13" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="Z13" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="AA13" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="AB13" t="s">
-        <v>123</v>
+        <v>150</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>151</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>152</v>
+      </c>
+      <c r="AE13">
+        <v>98671</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>151</v>
       </c>
       <c r="AH13" t="s">
-        <v>124</v>
-      </c>
-      <c r="AI13" t="s">
-        <v>125</v>
+        <v>154</v>
       </c>
       <c r="AJ13" t="s">
         <v>55</v>
       </c>
       <c r="AL13" t="s">
-        <v>126</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:49">
       <c r="A14">
-        <v>43381.7379050926</v>
+        <v>43382.01947916667</v>
       </c>
       <c r="B14">
-        <v>43381.75645833334</v>
+        <v>43382.02648148148</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
       <c r="E14">
         <v>100</v>
       </c>
       <c r="F14">
-        <v>1603</v>
+        <v>604</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
-        <v>43381.75645833334</v>
+        <v>43382.02648148148</v>
       </c>
       <c r="I14" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="N14">
-        <v>38.4797058105468</v>
+        <v>48.465103149414</v>
       </c>
       <c r="O14">
-        <v>-121.443801879882</v>
+        <v>7.95590209960937</v>
       </c>
       <c r="P14" t="s">
         <v>60</v>
@@ -1742,37 +1927,31 @@
         <v>52</v>
       </c>
       <c r="R14" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="S14" t="s">
-        <v>130</v>
-      </c>
-      <c r="T14">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c r="U14" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="V14" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="W14" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="X14" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="Y14" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="Z14" t="s">
-        <v>135</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>68</v>
+        <v>164</v>
       </c>
       <c r="AB14" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="AH14" t="s">
         <v>54</v>
@@ -1782,68 +1961,41 @@
       </c>
       <c r="AL14" t="s">
         <v>126</v>
-      </c>
-      <c r="AN14" t="s">
-        <v>137</v>
-      </c>
-      <c r="AO14" t="s">
-        <v>138</v>
-      </c>
-      <c r="AP14" t="s">
-        <v>139</v>
-      </c>
-      <c r="AQ14" t="s">
-        <v>54</v>
-      </c>
-      <c r="AS14">
-        <v>40</v>
-      </c>
-      <c r="AT14">
-        <v>40</v>
-      </c>
-      <c r="AU14">
-        <v>20</v>
-      </c>
-      <c r="AV14">
-        <v>1500</v>
-      </c>
-      <c r="AW14">
-        <v>1700</v>
       </c>
     </row>
     <row r="15" spans="1:49">
       <c r="A15">
-        <v>43381.87571759259</v>
+        <v>43382.42454861111</v>
       </c>
       <c r="B15">
-        <v>43381.88489583333</v>
+        <v>43382.44295138889</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="E15">
         <v>100</v>
       </c>
       <c r="F15">
-        <v>793</v>
+        <v>1590</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15">
-        <v>43381.88489583333</v>
+        <v>43382.44296296296</v>
       </c>
       <c r="I15" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
       <c r="N15">
-        <v>45.5440979003906</v>
+        <v>45.0897064208984</v>
       </c>
       <c r="O15">
-        <v>-122.642303466796</v>
+        <v>-123.400299072265</v>
       </c>
       <c r="P15" t="s">
         <v>60</v>
@@ -1852,52 +2004,55 @@
         <v>52</v>
       </c>
       <c r="R15" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="S15" t="s">
-        <v>143</v>
+        <v>169</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
       </c>
       <c r="U15" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
       <c r="V15" t="s">
-        <v>145</v>
+        <v>171</v>
       </c>
       <c r="W15" t="s">
-        <v>146</v>
+        <v>172</v>
       </c>
       <c r="X15" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="Y15" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="Z15" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="AA15" t="s">
         <v>80</v>
       </c>
       <c r="AB15" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="AC15" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="AD15" t="s">
-        <v>152</v>
+        <v>83</v>
       </c>
       <c r="AE15">
-        <v>98671</v>
+        <v>97367</v>
       </c>
       <c r="AF15" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="AG15" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="AH15" t="s">
-        <v>154</v>
+        <v>54</v>
       </c>
       <c r="AJ15" t="s">
         <v>55</v>
@@ -1905,206 +2060,31 @@
       <c r="AL15" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:49">
-      <c r="A16">
-        <v>43382.01947916667</v>
-      </c>
-      <c r="B16">
-        <v>43382.02648148148</v>
-      </c>
-      <c r="C16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E16">
-        <v>100</v>
-      </c>
-      <c r="F16">
-        <v>604</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>43382.02648148148</v>
-      </c>
-      <c r="I16" t="s">
-        <v>156</v>
-      </c>
-      <c r="N16">
-        <v>48.465103149414</v>
-      </c>
-      <c r="O16">
-        <v>7.95590209960937</v>
-      </c>
-      <c r="P16" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>52</v>
-      </c>
-      <c r="R16" t="s">
-        <v>157</v>
-      </c>
-      <c r="S16" t="s">
-        <v>158</v>
-      </c>
-      <c r="U16" t="s">
-        <v>159</v>
-      </c>
-      <c r="V16" t="s">
-        <v>160</v>
-      </c>
-      <c r="W16" t="s">
-        <v>161</v>
-      </c>
-      <c r="X16" t="s">
-        <v>162</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>163</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>164</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>165</v>
-      </c>
-      <c r="AH16" t="s">
+      <c r="AN15" t="s">
+        <v>169</v>
+      </c>
+      <c r="AO15" t="s">
+        <v>178</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>178</v>
+      </c>
+      <c r="AQ15" t="s">
         <v>54</v>
       </c>
-      <c r="AJ16" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:47">
-      <c r="A17">
-        <v>43382.42454861111</v>
-      </c>
-      <c r="B17">
-        <v>43382.44295138889</v>
-      </c>
-      <c r="C17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E17">
-        <v>100</v>
-      </c>
-      <c r="F17">
-        <v>1590</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>43382.44296296296</v>
-      </c>
-      <c r="I17" t="s">
-        <v>167</v>
-      </c>
-      <c r="N17">
-        <v>45.0897064208984</v>
-      </c>
-      <c r="O17">
-        <v>-123.400299072265</v>
-      </c>
-      <c r="P17" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>52</v>
-      </c>
-      <c r="R17" t="s">
-        <v>168</v>
-      </c>
-      <c r="S17" t="s">
-        <v>169</v>
-      </c>
-      <c r="T17">
-        <v>1</v>
-      </c>
-      <c r="U17" t="s">
-        <v>170</v>
-      </c>
-      <c r="V17" t="s">
-        <v>171</v>
-      </c>
-      <c r="W17" t="s">
-        <v>172</v>
-      </c>
-      <c r="X17" t="s">
-        <v>173</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>168</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>174</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>175</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>176</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>83</v>
-      </c>
-      <c r="AE17">
-        <v>97367</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>177</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>176</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>56</v>
-      </c>
-      <c r="AN17" t="s">
-        <v>169</v>
-      </c>
-      <c r="AO17" t="s">
-        <v>178</v>
-      </c>
-      <c r="AP17" t="s">
-        <v>178</v>
-      </c>
-      <c r="AQ17" t="s">
-        <v>54</v>
-      </c>
-      <c r="AS17">
+      <c r="AS15">
         <v>0</v>
       </c>
-      <c r="AT17">
+      <c r="AT15">
         <v>0</v>
       </c>
-      <c r="AU17">
+      <c r="AU15">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U11" r:id="rId1"/>
+    <hyperlink ref="U9" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added code to display next set of headings
</commit_message>
<xml_diff>
--- a/Anand_Work/FallWork2018/OUTPUT.xlsx
+++ b/Anand_Work/FallWork2018/OUTPUT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="200">
   <si>
     <t>Start Date</t>
   </si>
@@ -164,6 +164,70 @@
   <si>
     <t>1 - How many 5th/6th grade students do you expect to attend your outdoor school program this
 current/upcoming school year?</t>
+  </si>
+  <si>
+    <t>1 - Please describe your facility's emergency communication infrastructure.</t>
+  </si>
+  <si>
+    <t>What kind of communication connectivity is available at your site? - 1 - Cell Service</t>
+  </si>
+  <si>
+    <t>What kind of communication connectivity is available at your site? - 1 - Wi-Fi/Internet</t>
+  </si>
+  <si>
+    <t>What kind of communication connectivity is available at your site? - 1 - Land Line</t>
+  </si>
+  <si>
+    <t>Camp access: (check all that apply) - 1 - Camp access: (check all that apply) - Selected Choice</t>
+  </si>
+  <si>
+    <t>Camp access: (check all that apply) - 1 - Other - Text</t>
+  </si>
+  <si>
+    <t>1 - Location's acreage (if unknown please state unknown)</t>
+  </si>
+  <si>
+    <t>1 - What natural resources exist for study? Forest, Savanna, Stream, Pond? Special features such as salmon spawning location or wildfire evidence or unique geological features for study? Please describe.</t>
+  </si>
+  <si>
+    <t>At (insert facility name), what food service aspects are provided? - 1 - At (insert facility name), what food service aspects are provided? - Selected Choice</t>
+  </si>
+  <si>
+    <t>At (insert facility name), what food service aspects are provided? - 1 - Other - Text</t>
+  </si>
+  <si>
+    <t>If food is provided, can menus accommodate special dietary needs? (check all that apply) - 1 - If food is provided, can menus accommodate special dietary needs? (check all that apply) - Selected Choice</t>
+  </si>
+  <si>
+    <t>If food is provided, can menus accommodate special dietary needs? (check all that apply) - 1 - Other - Text</t>
+  </si>
+  <si>
+    <t>1 - Maximum inside dining capacity? (if unknown please state unknown)</t>
+  </si>
+  <si>
+    <t>1 - Maximum outside dining capacity?  (if unknown please state unknown)</t>
+  </si>
+  <si>
+    <t>Are there covered or indoor meeting areas? - 1 - Are there covered or indoor meeting areas? - Selected Choice</t>
+  </si>
+  <si>
+    <t>Are there covered or indoor meeting areas? - 1 - If Yes, How many and what capacity? - Text</t>
+  </si>
+  <si>
+    <t>1 - Maximum overnight indoor sleeping capacity (please describe accommodations)</t>
+  </si>
+  <si>
+    <t>1 - Maximum overnight outside sleeping capacity (please describe accomodations)</t>
+  </si>
+  <si>
+    <t>1 - Does your facility offer universally accessible sleeping facilities to accommodate students with limited mobility? If so, please describe.</t>
+  </si>
+  <si>
+    <t>1 - What are the biggest unmet facility and material needs for your outdoor school?</t>
+  </si>
+  <si>
+    <t>1 - Is there any additional information that you would like to provide regarding facilities and 
+materials?</t>
   </si>
   <si>
     <t>Survey Preview</t>
@@ -911,13 +975,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AW15"/>
+  <dimension ref="A1:BR15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:70">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1065,8 +1129,71 @@
       <c r="AW1" t="s">
         <v>48</v>
       </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="2" spans="1:49">
+    <row r="2" spans="1:70">
       <c r="A2">
         <v>43378.46934027778</v>
       </c>
@@ -1074,7 +1201,7 @@
         <v>43378.47023148148</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -1089,7 +1216,7 @@
         <v>43378.47024305556</v>
       </c>
       <c r="I2" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="N2">
         <v>44.5641937255859</v>
@@ -1098,13 +1225,13 @@
         <v>-123.278999328613</v>
       </c>
       <c r="P2" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="Q2" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:49">
+    <row r="3" spans="1:70">
       <c r="A3">
         <v>43378.47028935186</v>
       </c>
@@ -1112,7 +1239,7 @@
         <v>43378.47060185186</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -1127,7 +1254,7 @@
         <v>43378.47060185186</v>
       </c>
       <c r="I3" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="N3">
         <v>44.5641937255859</v>
@@ -1136,22 +1263,22 @@
         <v>-123.278999328613</v>
       </c>
       <c r="P3" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="Q3" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="AH3" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="AJ3" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="AL3" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:49">
+    <row r="4" spans="1:70">
       <c r="A4">
         <v>43380.91150462963</v>
       </c>
@@ -1159,7 +1286,7 @@
         <v>43380.91293981481</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -1174,7 +1301,7 @@
         <v>43380.91295138889</v>
       </c>
       <c r="I4" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="N4">
         <v>44.5637969970703</v>
@@ -1183,10 +1310,10 @@
         <v>-123.2779006958</v>
       </c>
       <c r="P4" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="Q4" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="T4">
         <v>3</v>
@@ -1201,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:49">
+    <row r="5" spans="1:70">
       <c r="AN5" s="1"/>
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
@@ -1219,7 +1346,7 @@
       <c r="AV5" s="1"/>
       <c r="AW5" s="1"/>
     </row>
-    <row r="6" spans="1:49">
+    <row r="6" spans="1:70">
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
       <c r="AP6" s="1"/>
@@ -1236,7 +1363,7 @@
       </c>
       <c r="AV6" s="1"/>
     </row>
-    <row r="7" spans="1:49">
+    <row r="7" spans="1:70">
       <c r="A7">
         <v>43381.70964120371</v>
       </c>
@@ -1247,7 +1374,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="E7">
         <v>100</v>
@@ -1262,7 +1389,7 @@
         <v>43381.71163194445</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="N7">
         <v>40.7180023193359</v>
@@ -1271,52 +1398,52 @@
         <v>-74.0754013061523</v>
       </c>
       <c r="P7" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="Q7" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="R7" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="S7" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="U7" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="V7" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="W7" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="X7" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="Y7" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="Z7" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="AA7" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="AB7" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="AH7" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="AJ7" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="AL7" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:49">
+    <row r="8" spans="1:70">
       <c r="A8">
         <v>43381.71248842592</v>
       </c>
@@ -1327,7 +1454,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="E8">
         <v>100</v>
@@ -1342,7 +1469,7 @@
         <v>43381.715</v>
       </c>
       <c r="I8" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="N8">
         <v>45.5653076171875</v>
@@ -1351,67 +1478,67 @@
         <v>-122.644798278808</v>
       </c>
       <c r="P8" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="Q8" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="R8" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="S8" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="U8" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="V8" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="W8" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="X8" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="Y8" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="Z8" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="AA8" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="AB8" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="AC8" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="AD8" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="AE8">
         <v>97055</v>
       </c>
       <c r="AF8" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="AG8" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="AH8" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="AJ8" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="AL8" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:49">
+    <row r="9" spans="1:70">
       <c r="A9">
         <v>43381.71474537037</v>
       </c>
@@ -1422,7 +1549,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -1437,7 +1564,7 @@
         <v>43381.71667824074</v>
       </c>
       <c r="I9" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="N9">
         <v>44.0682067871093</v>
@@ -1446,67 +1573,67 @@
         <v>-123.081901550292</v>
       </c>
       <c r="P9" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="Q9" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="R9" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="S9" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="V9" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="W9" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="X9" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="Y9" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="Z9" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AA9" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="AB9" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="AC9" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="AD9" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="AE9">
         <v>97419</v>
       </c>
       <c r="AF9" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="AG9" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="AH9" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="AJ9" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="AL9" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:49">
+    <row r="10" spans="1:70">
       <c r="A10">
         <v>43381.71635416667</v>
       </c>
@@ -1517,7 +1644,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="E10">
         <v>100</v>
@@ -1532,7 +1659,7 @@
         <v>43381.72159722223</v>
       </c>
       <c r="I10" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="N10">
         <v>45.3726959228515</v>
@@ -1541,64 +1668,64 @@
         <v>-122.76309967041</v>
       </c>
       <c r="P10" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="Q10" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="R10" t="s">
+        <v>125</v>
+      </c>
+      <c r="S10" t="s">
+        <v>126</v>
+      </c>
+      <c r="U10" t="s">
+        <v>127</v>
+      </c>
+      <c r="V10" t="s">
+        <v>128</v>
+      </c>
+      <c r="W10" t="s">
+        <v>129</v>
+      </c>
+      <c r="X10" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>132</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>133</v>
+      </c>
+      <c r="AD10" t="s">
         <v>104</v>
-      </c>
-      <c r="S10" t="s">
-        <v>105</v>
-      </c>
-      <c r="U10" t="s">
-        <v>106</v>
-      </c>
-      <c r="V10" t="s">
-        <v>107</v>
-      </c>
-      <c r="W10" t="s">
-        <v>108</v>
-      </c>
-      <c r="X10" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>112</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>83</v>
       </c>
       <c r="AE10">
         <v>97064</v>
       </c>
       <c r="AF10" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="AG10" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="AH10" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="AJ10" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="AL10" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:49">
+    <row r="11" spans="1:70">
       <c r="A11">
         <v>43381.74771990741</v>
       </c>
@@ -1609,7 +1736,7 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="E11">
         <v>100</v>
@@ -1624,7 +1751,7 @@
         <v>43381.75016203704</v>
       </c>
       <c r="I11" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="N11">
         <v>45.3493957519531</v>
@@ -1633,55 +1760,55 @@
         <v>-117.212799072265</v>
       </c>
       <c r="P11" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="Q11" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="R11" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="S11" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="U11" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="V11" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="W11" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="X11" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="Y11" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="Z11" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="AA11" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="AB11" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="AH11" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="AI11" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="AJ11" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="AL11" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:49">
+    <row r="12" spans="1:70">
       <c r="A12">
         <v>43381.7379050926</v>
       </c>
@@ -1692,7 +1819,7 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="E12">
         <v>100</v>
@@ -1707,7 +1834,7 @@
         <v>43381.75645833334</v>
       </c>
       <c r="I12" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="N12">
         <v>38.4797058105468</v>
@@ -1716,64 +1843,64 @@
         <v>-121.443801879882</v>
       </c>
       <c r="P12" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="Q12" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="R12" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="S12" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="T12">
         <v>1</v>
       </c>
       <c r="U12" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="V12" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="W12" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="X12" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="Y12" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="Z12" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="AA12" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="AB12" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="AH12" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="AJ12" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="AL12" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="AN12" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="AO12" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="AP12" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="AQ12" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="AS12">
         <v>40</v>
@@ -1791,7 +1918,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="13" spans="1:49">
+    <row r="13" spans="1:70">
       <c r="A13">
         <v>43381.87571759259</v>
       </c>
@@ -1802,7 +1929,7 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="E13">
         <v>100</v>
@@ -1817,7 +1944,7 @@
         <v>43381.88489583333</v>
       </c>
       <c r="I13" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="N13">
         <v>45.5440979003906</v>
@@ -1826,67 +1953,67 @@
         <v>-122.642303466796</v>
       </c>
       <c r="P13" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="Q13" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="R13" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="S13" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="U13" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="V13" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="W13" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="X13" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="Y13" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="Z13" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="AA13" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="AB13" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="AC13" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="AD13" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="AE13">
         <v>98671</v>
       </c>
       <c r="AF13" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="AG13" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="AH13" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="AJ13" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="AL13" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:49">
+    <row r="14" spans="1:70">
       <c r="A14">
         <v>43382.01947916667</v>
       </c>
@@ -1897,7 +2024,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="E14">
         <v>100</v>
@@ -1912,7 +2039,7 @@
         <v>43382.02648148148</v>
       </c>
       <c r="I14" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="N14">
         <v>48.465103149414</v>
@@ -1921,49 +2048,49 @@
         <v>7.95590209960937</v>
       </c>
       <c r="P14" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="Q14" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="R14" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="S14" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="U14" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="V14" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="W14" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="X14" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="Y14" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="Z14" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
       <c r="AB14" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="AH14" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="AJ14" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="AL14" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:49">
+    <row r="15" spans="1:70">
       <c r="A15">
         <v>43382.42454861111</v>
       </c>
@@ -1974,7 +2101,7 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="E15">
         <v>100</v>
@@ -1989,7 +2116,7 @@
         <v>43382.44296296296</v>
       </c>
       <c r="I15" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="N15">
         <v>45.0897064208984</v>
@@ -1998,79 +2125,79 @@
         <v>-123.400299072265</v>
       </c>
       <c r="P15" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="Q15" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="R15" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="S15" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="T15">
         <v>1</v>
       </c>
       <c r="U15" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="V15" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="W15" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="X15" t="s">
-        <v>173</v>
+        <v>194</v>
       </c>
       <c r="Y15" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="Z15" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
       <c r="AA15" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="AB15" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="AC15" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="AD15" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="AE15">
         <v>97367</v>
       </c>
       <c r="AF15" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
       <c r="AG15" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="AH15" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="AJ15" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="AL15" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="AN15" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="AO15" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="AP15" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="AQ15" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="AS15">
         <v>0</v>

</xml_diff>

<commit_message>
Started Working on Section4
</commit_message>
<xml_diff>
--- a/Anand_Work/FallWork2018/OUTPUT.xlsx
+++ b/Anand_Work/FallWork2018/OUTPUT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="219">
   <si>
     <t>Start Date</t>
   </si>
@@ -622,6 +622,63 @@
   </si>
   <si>
     <t>varies</t>
+  </si>
+  <si>
+    <t>We have an emergency action plan written up. Speed dial set to 911, AED system for facility, walker talkies on staff leaders.</t>
+  </si>
+  <si>
+    <t>Gravel/dirt road,Forestry road,Private access/limited access road,Extra large vehicle (Such semi-tuck with trailer, standard bus, class A RV),Large vehicles (such as semi without trailer, short bus length, Class C RV, truck with trailer),Standard vehicle (Such as truck without trailer, SUV, sedan),Small vehicle (Such as motorcycle, hybrid, smart car)</t>
+  </si>
+  <si>
+    <t>104 acres</t>
+  </si>
+  <si>
+    <t>Stream, river, marsh, forest, reptile and amphibians habitat, wildlife, gold beds, fossil beds</t>
+  </si>
+  <si>
+    <t>Food service facility, kitchen staff, and food</t>
+  </si>
+  <si>
+    <t>Yes (if yes, please check all that apply),Vegetarian,Vegan,Kosher,Diabetic Meal plan,Gluten/wheat allergies,Dairy allergies (milk and/or egg),Soy, peanut, or tree nut allergies,Seafood or shellfish allergies</t>
+  </si>
+  <si>
+    <t>If Yes, How many and what capacity?</t>
+  </si>
+  <si>
+    <t>Yes, we have sidewalks to all buildings with 2 ADA accessible cabins, and ADA accessible batthroom facilities.</t>
+  </si>
+  <si>
+    <t>More bathroom facilities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are located in the Siusalaw National Forest and are "off the grid". However, we do have a satellite communication system that provides both telephone service and internet access. The local hospital, Pac West and Life Flight all have our coordinates and are familiar with our location in case of an emergency. </t>
+  </si>
+  <si>
+    <t>Paved road,Gravel/dirt road,Extra large vehicle (Such semi-tuck with trailer, standard bus, class A RV),Large vehicles (such as semi without trailer, short bus length, Class C RV, truck with trailer),Standard vehicle (Such as truck without trailer, SUV, sedan),Small vehicle (Such as motorcycle, hybrid, smart car),Horse/Pack animal</t>
+  </si>
+  <si>
+    <t>25 acres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forest (old growth forest including Sitka Spruce and many nurse logs); pristine mountain stream (including salmon spawning location); many ferns and wild plants and countless mushrooms.  </t>
+  </si>
+  <si>
+    <t>Programs can choose to provide their own food service or hire DCC's staff to provide meals.</t>
+  </si>
+  <si>
+    <t>Yes (if yes, please check all that apply),Vegetarian,Gluten/wheat allergies,Dairy allergies (milk and/or egg),Soy, peanut, or tree nut allergies</t>
+  </si>
+  <si>
+    <t>Depends on the weather.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have a meeting area that can seat 100 and a craft room that can seat about 12. There is also an outdoor covered Activity Center that could seat 100+. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The main lodge can sleep up to 120. This would include upper bunks. Rooms are chalet-style with common restrooms at each end of the hallway. In addition to the 3-floor lodge, we also have 5 cabins that each sleep 12-14 in bunk beds and a yurt that sleeps 14. A central bathhouse is available for cabin campers. The total capacity is about 190. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, we have two main floor rooms available in the lodge that are accessible and the Alsea cabin is also accessible. </t>
   </si>
 </sst>
 </file>
@@ -1809,53 +1866,59 @@
       </c>
     </row>
     <row r="12" spans="1:70">
-      <c r="A12">
-        <v>43381.7379050926</v>
-      </c>
-      <c r="B12">
-        <v>43381.75645833334</v>
+      <c r="A12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" t="s">
+        <v>175</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E12">
-        <v>100</v>
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>201</v>
       </c>
       <c r="F12">
         <v>1603</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>43381.75645833334</v>
+      <c r="G12" t="s">
+        <v>202</v>
+      </c>
+      <c r="H12" t="s">
+        <v>203</v>
       </c>
       <c r="I12" t="s">
-        <v>149</v>
+        <v>204</v>
+      </c>
+      <c r="K12" t="s">
+        <v>205</v>
+      </c>
+      <c r="M12">
+        <v>240</v>
       </c>
       <c r="N12">
-        <v>38.4797058105468</v>
-      </c>
-      <c r="O12">
-        <v>-121.443801879882</v>
-      </c>
-      <c r="P12" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>73</v>
-      </c>
-      <c r="R12" t="s">
-        <v>150</v>
+        <v>300</v>
+      </c>
+      <c r="O12" t="s">
+        <v>206</v>
+      </c>
+      <c r="P12">
+        <v>5</v>
+      </c>
+      <c r="Q12">
+        <v>180</v>
+      </c>
+      <c r="R12">
+        <v>500</v>
       </c>
       <c r="S12" t="s">
-        <v>151</v>
-      </c>
-      <c r="T12">
-        <v>1</v>
+        <v>207</v>
+      </c>
+      <c r="T12" t="s">
+        <v>208</v>
       </c>
       <c r="U12" t="s">
         <v>152</v>
@@ -2091,50 +2154,59 @@
       </c>
     </row>
     <row r="15" spans="1:70">
-      <c r="A15">
-        <v>43382.42454861111</v>
-      </c>
-      <c r="B15">
-        <v>43382.44295138889</v>
+      <c r="A15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B15" t="s">
+        <v>175</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>187</v>
-      </c>
-      <c r="E15">
-        <v>100</v>
+        <v>175</v>
+      </c>
+      <c r="E15" t="s">
+        <v>210</v>
       </c>
       <c r="F15">
         <v>1590</v>
       </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>43382.44296296296</v>
+      <c r="G15" t="s">
+        <v>211</v>
+      </c>
+      <c r="H15" t="s">
+        <v>212</v>
       </c>
       <c r="I15" t="s">
-        <v>188</v>
-      </c>
-      <c r="N15">
-        <v>45.0897064208984</v>
-      </c>
-      <c r="O15">
-        <v>-123.400299072265</v>
+        <v>145</v>
+      </c>
+      <c r="J15" t="s">
+        <v>213</v>
+      </c>
+      <c r="K15" t="s">
+        <v>214</v>
+      </c>
+      <c r="M15">
+        <v>150</v>
+      </c>
+      <c r="N15" t="s">
+        <v>215</v>
+      </c>
+      <c r="O15" t="s">
+        <v>206</v>
       </c>
       <c r="P15" t="s">
-        <v>81</v>
+        <v>216</v>
       </c>
       <c r="Q15" t="s">
-        <v>73</v>
+        <v>217</v>
       </c>
       <c r="R15" t="s">
         <v>189</v>
       </c>
       <c r="S15" t="s">
-        <v>190</v>
+        <v>218</v>
       </c>
       <c r="T15">
         <v>1</v>

</xml_diff>

<commit_message>
Need to work on loop of section 4
</commit_message>
<xml_diff>
--- a/Anand_Work/FallWork2018/OUTPUT.xlsx
+++ b/Anand_Work/FallWork2018/OUTPUT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="220">
   <si>
     <t>Start Date</t>
   </si>
@@ -649,6 +649,9 @@
   </si>
   <si>
     <t>More bathroom facilities.</t>
+  </si>
+  <si>
+    <t>We are currently providing curriculum and turn key outdoor school for schools with limited resources to plan their own.</t>
   </si>
   <si>
     <t xml:space="preserve">We are located in the Siusalaw National Forest and are "off the grid". However, we do have a satellite communication system that provides both telephone service and internet access. The local hospital, Pac West and Life Flight all have our coordinates and are familiar with our location in case of an emergency. </t>
@@ -1781,6 +1784,60 @@
       <c r="AL10" t="s">
         <v>77</v>
       </c>
+      <c r="AX10" t="s">
+        <v>200</v>
+      </c>
+      <c r="AY10" t="s">
+        <v>175</v>
+      </c>
+      <c r="AZ10" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA10" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB10" t="s">
+        <v>201</v>
+      </c>
+      <c r="BD10" t="s">
+        <v>202</v>
+      </c>
+      <c r="BE10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BF10" t="s">
+        <v>204</v>
+      </c>
+      <c r="BH10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BJ10">
+        <v>240</v>
+      </c>
+      <c r="BK10">
+        <v>300</v>
+      </c>
+      <c r="BL10" t="s">
+        <v>206</v>
+      </c>
+      <c r="BM10">
+        <v>5</v>
+      </c>
+      <c r="BN10">
+        <v>180</v>
+      </c>
+      <c r="BO10">
+        <v>500</v>
+      </c>
+      <c r="BP10" t="s">
+        <v>207</v>
+      </c>
+      <c r="BQ10" t="s">
+        <v>208</v>
+      </c>
+      <c r="BR10" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="11" spans="1:70">
       <c r="A11">
@@ -1866,59 +1923,53 @@
       </c>
     </row>
     <row r="12" spans="1:70">
-      <c r="A12" t="s">
-        <v>200</v>
-      </c>
-      <c r="B12" t="s">
-        <v>175</v>
+      <c r="A12">
+        <v>43381.7379050926</v>
+      </c>
+      <c r="B12">
+        <v>43381.75645833334</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" t="s">
-        <v>201</v>
+        <v>148</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
       </c>
       <c r="F12">
         <v>1603</v>
       </c>
-      <c r="G12" t="s">
-        <v>202</v>
-      </c>
-      <c r="H12" t="s">
-        <v>203</v>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>43381.75645833334</v>
       </c>
       <c r="I12" t="s">
-        <v>204</v>
-      </c>
-      <c r="K12" t="s">
-        <v>205</v>
-      </c>
-      <c r="M12">
-        <v>240</v>
+        <v>149</v>
       </c>
       <c r="N12">
-        <v>300</v>
-      </c>
-      <c r="O12" t="s">
-        <v>206</v>
-      </c>
-      <c r="P12">
-        <v>5</v>
-      </c>
-      <c r="Q12">
-        <v>180</v>
-      </c>
-      <c r="R12">
-        <v>500</v>
+        <v>38.4797058105468</v>
+      </c>
+      <c r="O12">
+        <v>-121.443801879882</v>
+      </c>
+      <c r="P12" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>73</v>
+      </c>
+      <c r="R12" t="s">
+        <v>150</v>
       </c>
       <c r="S12" t="s">
-        <v>207</v>
-      </c>
-      <c r="T12" t="s">
-        <v>208</v>
+        <v>151</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
       </c>
       <c r="U12" t="s">
         <v>152</v>
@@ -2075,6 +2126,54 @@
       <c r="AL13" t="s">
         <v>77</v>
       </c>
+      <c r="AX13" t="s">
+        <v>210</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>175</v>
+      </c>
+      <c r="AZ13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA13" t="s">
+        <v>175</v>
+      </c>
+      <c r="BB13" t="s">
+        <v>211</v>
+      </c>
+      <c r="BD13" t="s">
+        <v>212</v>
+      </c>
+      <c r="BE13" t="s">
+        <v>213</v>
+      </c>
+      <c r="BF13" t="s">
+        <v>145</v>
+      </c>
+      <c r="BG13" t="s">
+        <v>214</v>
+      </c>
+      <c r="BH13" t="s">
+        <v>215</v>
+      </c>
+      <c r="BJ13">
+        <v>150</v>
+      </c>
+      <c r="BK13" t="s">
+        <v>216</v>
+      </c>
+      <c r="BL13" t="s">
+        <v>206</v>
+      </c>
+      <c r="BM13" t="s">
+        <v>217</v>
+      </c>
+      <c r="BN13" t="s">
+        <v>218</v>
+      </c>
+      <c r="BP13" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="14" spans="1:70">
       <c r="A14">
@@ -2154,59 +2253,50 @@
       </c>
     </row>
     <row r="15" spans="1:70">
-      <c r="A15" t="s">
-        <v>209</v>
-      </c>
-      <c r="B15" t="s">
-        <v>175</v>
+      <c r="A15">
+        <v>43382.42454861111</v>
+      </c>
+      <c r="B15">
+        <v>43382.44295138889</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>175</v>
-      </c>
-      <c r="E15" t="s">
-        <v>210</v>
+        <v>187</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
       </c>
       <c r="F15">
         <v>1590</v>
       </c>
-      <c r="G15" t="s">
-        <v>211</v>
-      </c>
-      <c r="H15" t="s">
-        <v>212</v>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>43382.44296296296</v>
       </c>
       <c r="I15" t="s">
-        <v>145</v>
-      </c>
-      <c r="J15" t="s">
-        <v>213</v>
-      </c>
-      <c r="K15" t="s">
-        <v>214</v>
-      </c>
-      <c r="M15">
-        <v>150</v>
-      </c>
-      <c r="N15" t="s">
-        <v>215</v>
-      </c>
-      <c r="O15" t="s">
-        <v>206</v>
+        <v>188</v>
+      </c>
+      <c r="N15">
+        <v>45.0897064208984</v>
+      </c>
+      <c r="O15">
+        <v>-123.400299072265</v>
       </c>
       <c r="P15" t="s">
-        <v>216</v>
+        <v>81</v>
       </c>
       <c r="Q15" t="s">
-        <v>217</v>
+        <v>73</v>
       </c>
       <c r="R15" t="s">
         <v>189</v>
       </c>
       <c r="S15" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="T15">
         <v>1</v>

</xml_diff>

<commit_message>
Done with section 4 need to make changes in comments
</commit_message>
<xml_diff>
--- a/Anand_Work/FallWork2018/OUTPUT.xlsx
+++ b/Anand_Work/FallWork2018/OUTPUT.xlsx
@@ -1405,6 +1405,27 @@
       </c>
       <c r="AV5" s="1"/>
       <c r="AW5" s="1"/>
+      <c r="AX5" s="1"/>
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1"/>
+      <c r="BA5" s="1"/>
+      <c r="BB5" s="1"/>
+      <c r="BC5" s="1"/>
+      <c r="BD5" s="1"/>
+      <c r="BE5" s="1"/>
+      <c r="BF5" s="1"/>
+      <c r="BG5" s="1"/>
+      <c r="BH5" s="1"/>
+      <c r="BI5" s="1"/>
+      <c r="BJ5" s="1"/>
+      <c r="BK5" s="1"/>
+      <c r="BL5" s="1"/>
+      <c r="BM5" s="1"/>
+      <c r="BN5" s="1"/>
+      <c r="BO5" s="1"/>
+      <c r="BP5" s="1"/>
+      <c r="BQ5" s="1"/>
+      <c r="BR5" s="1"/>
     </row>
     <row r="6" spans="1:70">
       <c r="AN6" s="1"/>
@@ -1422,6 +1443,26 @@
         <v>0</v>
       </c>
       <c r="AV6" s="1"/>
+      <c r="AX6" s="1"/>
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+      <c r="BA6" s="1"/>
+      <c r="BB6" s="1"/>
+      <c r="BC6" s="1"/>
+      <c r="BD6" s="1"/>
+      <c r="BE6" s="1"/>
+      <c r="BF6" s="1"/>
+      <c r="BG6" s="1"/>
+      <c r="BH6" s="1"/>
+      <c r="BI6" s="1"/>
+      <c r="BJ6" s="1"/>
+      <c r="BK6" s="1"/>
+      <c r="BL6" s="1"/>
+      <c r="BM6" s="1"/>
+      <c r="BN6" s="1"/>
+      <c r="BO6" s="1"/>
+      <c r="BP6" s="1"/>
+      <c r="BQ6" s="1"/>
     </row>
     <row r="7" spans="1:70">
       <c r="A7">
@@ -1784,60 +1825,6 @@
       <c r="AL10" t="s">
         <v>77</v>
       </c>
-      <c r="AX10" t="s">
-        <v>200</v>
-      </c>
-      <c r="AY10" t="s">
-        <v>175</v>
-      </c>
-      <c r="AZ10" t="s">
-        <v>75</v>
-      </c>
-      <c r="BA10" t="s">
-        <v>75</v>
-      </c>
-      <c r="BB10" t="s">
-        <v>201</v>
-      </c>
-      <c r="BD10" t="s">
-        <v>202</v>
-      </c>
-      <c r="BE10" t="s">
-        <v>203</v>
-      </c>
-      <c r="BF10" t="s">
-        <v>204</v>
-      </c>
-      <c r="BH10" t="s">
-        <v>205</v>
-      </c>
-      <c r="BJ10">
-        <v>240</v>
-      </c>
-      <c r="BK10">
-        <v>300</v>
-      </c>
-      <c r="BL10" t="s">
-        <v>206</v>
-      </c>
-      <c r="BM10">
-        <v>5</v>
-      </c>
-      <c r="BN10">
-        <v>180</v>
-      </c>
-      <c r="BO10">
-        <v>500</v>
-      </c>
-      <c r="BP10" t="s">
-        <v>207</v>
-      </c>
-      <c r="BQ10" t="s">
-        <v>208</v>
-      </c>
-      <c r="BR10" t="s">
-        <v>209</v>
-      </c>
     </row>
     <row r="11" spans="1:70">
       <c r="A11">
@@ -2031,6 +2018,60 @@
       <c r="AW12">
         <v>1700</v>
       </c>
+      <c r="AX12" t="s">
+        <v>200</v>
+      </c>
+      <c r="AY12" t="s">
+        <v>175</v>
+      </c>
+      <c r="AZ12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB12" t="s">
+        <v>201</v>
+      </c>
+      <c r="BD12" t="s">
+        <v>202</v>
+      </c>
+      <c r="BE12" t="s">
+        <v>203</v>
+      </c>
+      <c r="BF12" t="s">
+        <v>204</v>
+      </c>
+      <c r="BH12" t="s">
+        <v>205</v>
+      </c>
+      <c r="BJ12">
+        <v>240</v>
+      </c>
+      <c r="BK12">
+        <v>300</v>
+      </c>
+      <c r="BL12" t="s">
+        <v>206</v>
+      </c>
+      <c r="BM12">
+        <v>5</v>
+      </c>
+      <c r="BN12">
+        <v>180</v>
+      </c>
+      <c r="BO12">
+        <v>500</v>
+      </c>
+      <c r="BP12" t="s">
+        <v>207</v>
+      </c>
+      <c r="BQ12" t="s">
+        <v>208</v>
+      </c>
+      <c r="BR12" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="13" spans="1:70">
       <c r="A13">
@@ -2126,54 +2167,6 @@
       <c r="AL13" t="s">
         <v>77</v>
       </c>
-      <c r="AX13" t="s">
-        <v>210</v>
-      </c>
-      <c r="AY13" t="s">
-        <v>175</v>
-      </c>
-      <c r="AZ13" t="s">
-        <v>75</v>
-      </c>
-      <c r="BA13" t="s">
-        <v>175</v>
-      </c>
-      <c r="BB13" t="s">
-        <v>211</v>
-      </c>
-      <c r="BD13" t="s">
-        <v>212</v>
-      </c>
-      <c r="BE13" t="s">
-        <v>213</v>
-      </c>
-      <c r="BF13" t="s">
-        <v>145</v>
-      </c>
-      <c r="BG13" t="s">
-        <v>214</v>
-      </c>
-      <c r="BH13" t="s">
-        <v>215</v>
-      </c>
-      <c r="BJ13">
-        <v>150</v>
-      </c>
-      <c r="BK13" t="s">
-        <v>216</v>
-      </c>
-      <c r="BL13" t="s">
-        <v>206</v>
-      </c>
-      <c r="BM13" t="s">
-        <v>217</v>
-      </c>
-      <c r="BN13" t="s">
-        <v>218</v>
-      </c>
-      <c r="BP13" t="s">
-        <v>219</v>
-      </c>
     </row>
     <row r="14" spans="1:70">
       <c r="A14">
@@ -2369,6 +2362,54 @@
       </c>
       <c r="AU15">
         <v>0</v>
+      </c>
+      <c r="AX15" t="s">
+        <v>210</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>175</v>
+      </c>
+      <c r="AZ15" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA15" t="s">
+        <v>175</v>
+      </c>
+      <c r="BB15" t="s">
+        <v>211</v>
+      </c>
+      <c r="BD15" t="s">
+        <v>212</v>
+      </c>
+      <c r="BE15" t="s">
+        <v>213</v>
+      </c>
+      <c r="BF15" t="s">
+        <v>145</v>
+      </c>
+      <c r="BG15" t="s">
+        <v>214</v>
+      </c>
+      <c r="BH15" t="s">
+        <v>215</v>
+      </c>
+      <c r="BJ15">
+        <v>150</v>
+      </c>
+      <c r="BK15" t="s">
+        <v>216</v>
+      </c>
+      <c r="BL15" t="s">
+        <v>206</v>
+      </c>
+      <c r="BM15" t="s">
+        <v>217</v>
+      </c>
+      <c r="BN15" t="s">
+        <v>218</v>
+      </c>
+      <c r="BP15" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes to section4 and sectio5 so that it prints right data with a line space after the loop
</commit_message>
<xml_diff>
--- a/Anand_Work/FallWork2018/OUTPUT.xlsx
+++ b/Anand_Work/FallWork2018/OUTPUT.xlsx
@@ -688,16 +688,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -731,15 +723,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1035,7 +1026,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BR15"/>
+  <dimension ref="A1:BR16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1389,194 +1380,60 @@
       </c>
     </row>
     <row r="5" spans="1:70">
-      <c r="AN5" s="1"/>
-      <c r="AO5" s="1"/>
-      <c r="AP5" s="1"/>
-      <c r="AQ5" s="1"/>
-      <c r="AR5" s="1"/>
-      <c r="AS5" s="1">
+      <c r="AS5">
         <v>0</v>
       </c>
-      <c r="AT5" s="1">
+      <c r="AT5">
         <v>0</v>
       </c>
-      <c r="AU5" s="1">
+      <c r="AU5">
         <v>0</v>
       </c>
-      <c r="AV5" s="1"/>
-      <c r="AW5" s="1"/>
-      <c r="AX5" s="1"/>
-      <c r="AY5" s="1"/>
-      <c r="AZ5" s="1"/>
-      <c r="BA5" s="1"/>
-      <c r="BB5" s="1"/>
-      <c r="BC5" s="1"/>
-      <c r="BD5" s="1"/>
-      <c r="BE5" s="1"/>
-      <c r="BF5" s="1"/>
-      <c r="BG5" s="1"/>
-      <c r="BH5" s="1"/>
-      <c r="BI5" s="1"/>
-      <c r="BJ5" s="1"/>
-      <c r="BK5" s="1"/>
-      <c r="BL5" s="1"/>
-      <c r="BM5" s="1"/>
-      <c r="BN5" s="1"/>
-      <c r="BO5" s="1"/>
-      <c r="BP5" s="1"/>
-      <c r="BQ5" s="1"/>
-      <c r="BR5" s="1"/>
     </row>
     <row r="6" spans="1:70">
-      <c r="AN6" s="1"/>
-      <c r="AO6" s="1"/>
-      <c r="AP6" s="1"/>
-      <c r="AQ6" s="1"/>
-      <c r="AR6" s="1"/>
-      <c r="AS6" s="1">
+      <c r="AS6">
         <v>0</v>
       </c>
-      <c r="AT6" s="1">
+      <c r="AT6">
         <v>0</v>
       </c>
-      <c r="AU6" s="1">
+      <c r="AU6">
         <v>0</v>
-      </c>
-      <c r="AV6" s="1"/>
-      <c r="AX6" s="1"/>
-      <c r="AY6" s="1"/>
-      <c r="AZ6" s="1"/>
-      <c r="BA6" s="1"/>
-      <c r="BB6" s="1"/>
-      <c r="BC6" s="1"/>
-      <c r="BD6" s="1"/>
-      <c r="BE6" s="1"/>
-      <c r="BF6" s="1"/>
-      <c r="BG6" s="1"/>
-      <c r="BH6" s="1"/>
-      <c r="BI6" s="1"/>
-      <c r="BJ6" s="1"/>
-      <c r="BK6" s="1"/>
-      <c r="BL6" s="1"/>
-      <c r="BM6" s="1"/>
-      <c r="BN6" s="1"/>
-      <c r="BO6" s="1"/>
-      <c r="BP6" s="1"/>
-      <c r="BQ6" s="1"/>
-    </row>
-    <row r="7" spans="1:70">
-      <c r="A7">
-        <v>43381.70964120371</v>
-      </c>
-      <c r="B7">
-        <v>43381.71162037037</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7">
-        <v>100</v>
-      </c>
-      <c r="F7">
-        <v>171</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>43381.71163194445</v>
-      </c>
-      <c r="I7" t="s">
-        <v>80</v>
-      </c>
-      <c r="N7">
-        <v>40.7180023193359</v>
-      </c>
-      <c r="O7">
-        <v>-74.0754013061523</v>
-      </c>
-      <c r="P7" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>73</v>
-      </c>
-      <c r="R7" t="s">
-        <v>82</v>
-      </c>
-      <c r="S7" t="s">
-        <v>83</v>
-      </c>
-      <c r="U7" t="s">
-        <v>84</v>
-      </c>
-      <c r="V7" t="s">
-        <v>85</v>
-      </c>
-      <c r="W7" t="s">
-        <v>86</v>
-      </c>
-      <c r="X7" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>75</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>76</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:70">
       <c r="A8">
-        <v>43381.71248842592</v>
+        <v>43381.70964120371</v>
       </c>
       <c r="B8">
-        <v>43381.715</v>
+        <v>43381.71162037037</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E8">
         <v>100</v>
       </c>
       <c r="F8">
-        <v>216</v>
+        <v>171</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
-        <v>43381.715</v>
+        <v>43381.71163194445</v>
       </c>
       <c r="I8" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="N8">
-        <v>45.5653076171875</v>
+        <v>40.7180023193359</v>
       </c>
       <c r="O8">
-        <v>-122.644798278808</v>
+        <v>-74.0754013061523</v>
       </c>
       <c r="P8" t="s">
         <v>81</v>
@@ -1585,49 +1442,34 @@
         <v>73</v>
       </c>
       <c r="R8" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="S8" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="U8" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="V8" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="W8" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="X8" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="Y8" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="Z8" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="AA8" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="AB8" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>103</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>104</v>
-      </c>
-      <c r="AE8">
-        <v>97055</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>105</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="AH8" t="s">
         <v>75</v>
@@ -1641,37 +1483,37 @@
     </row>
     <row r="9" spans="1:70">
       <c r="A9">
-        <v>43381.71474537037</v>
+        <v>43381.71248842592</v>
       </c>
       <c r="B9">
-        <v>43381.71667824074</v>
+        <v>43381.715</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="E9">
         <v>100</v>
       </c>
       <c r="F9">
-        <v>166</v>
+        <v>216</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
-        <v>43381.71667824074</v>
+        <v>43381.715</v>
       </c>
       <c r="I9" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="N9">
-        <v>44.0682067871093</v>
+        <v>45.5653076171875</v>
       </c>
       <c r="O9">
-        <v>-123.081901550292</v>
+        <v>-122.644798278808</v>
       </c>
       <c r="P9" t="s">
         <v>81</v>
@@ -1680,49 +1522,49 @@
         <v>73</v>
       </c>
       <c r="R9" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="S9" t="s">
-        <v>110</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>111</v>
+        <v>94</v>
+      </c>
+      <c r="U9" t="s">
+        <v>95</v>
       </c>
       <c r="V9" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="W9" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="X9" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="Y9" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="Z9" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="AA9" t="s">
         <v>101</v>
       </c>
       <c r="AB9" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="AC9" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="AD9" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="AE9">
-        <v>97419</v>
+        <v>97055</v>
       </c>
       <c r="AF9" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="AG9" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="AH9" t="s">
         <v>75</v>
@@ -1731,42 +1573,42 @@
         <v>76</v>
       </c>
       <c r="AL9" t="s">
-        <v>122</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:70">
       <c r="A10">
-        <v>43381.71635416667</v>
+        <v>43381.71474537037</v>
       </c>
       <c r="B10">
-        <v>43381.72159722223</v>
+        <v>43381.71667824074</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="E10">
         <v>100</v>
       </c>
       <c r="F10">
-        <v>452</v>
+        <v>166</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>43381.72159722223</v>
+        <v>43381.71667824074</v>
       </c>
       <c r="I10" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="N10">
-        <v>45.3726959228515</v>
+        <v>44.0682067871093</v>
       </c>
       <c r="O10">
-        <v>-122.76309967041</v>
+        <v>-123.081901550292</v>
       </c>
       <c r="P10" t="s">
         <v>81</v>
@@ -1775,46 +1617,49 @@
         <v>73</v>
       </c>
       <c r="R10" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="S10" t="s">
-        <v>126</v>
-      </c>
-      <c r="U10" t="s">
-        <v>127</v>
+        <v>110</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="V10" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="W10" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="X10" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="Y10" t="s">
-        <v>131</v>
+        <v>115</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>116</v>
       </c>
       <c r="AA10" t="s">
         <v>101</v>
       </c>
       <c r="AB10" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="AC10" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="AD10" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="AE10">
-        <v>97064</v>
+        <v>97419</v>
       </c>
       <c r="AF10" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="AG10" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="AH10" t="s">
         <v>75</v>
@@ -1823,42 +1668,42 @@
         <v>76</v>
       </c>
       <c r="AL10" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:70">
       <c r="A11">
-        <v>43381.74771990741</v>
+        <v>43381.71635416667</v>
       </c>
       <c r="B11">
-        <v>43381.75016203704</v>
+        <v>43381.72159722223</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="E11">
         <v>100</v>
       </c>
       <c r="F11">
-        <v>211</v>
+        <v>452</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
-        <v>43381.75016203704</v>
+        <v>43381.72159722223</v>
       </c>
       <c r="I11" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="N11">
-        <v>45.3493957519531</v>
+        <v>45.3726959228515</v>
       </c>
       <c r="O11">
-        <v>-117.212799072265</v>
+        <v>-122.76309967041</v>
       </c>
       <c r="P11" t="s">
         <v>81</v>
@@ -1867,81 +1712,90 @@
         <v>73</v>
       </c>
       <c r="R11" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="S11" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="U11" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="V11" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="W11" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="X11" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="Y11" t="s">
-        <v>137</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="AA11" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="AB11" t="s">
-        <v>144</v>
+        <v>132</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>133</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE11">
+        <v>97064</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>133</v>
       </c>
       <c r="AH11" t="s">
-        <v>145</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>146</v>
+        <v>75</v>
       </c>
       <c r="AJ11" t="s">
         <v>76</v>
       </c>
       <c r="AL11" t="s">
-        <v>147</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:70">
       <c r="A12">
-        <v>43381.7379050926</v>
+        <v>43381.74771990741</v>
       </c>
       <c r="B12">
-        <v>43381.75645833334</v>
+        <v>43381.75016203704</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="E12">
         <v>100</v>
       </c>
       <c r="F12">
-        <v>1603</v>
+        <v>211</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12">
-        <v>43381.75645833334</v>
+        <v>43381.75016203704</v>
       </c>
       <c r="I12" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="N12">
-        <v>38.4797058105468</v>
+        <v>45.3493957519531</v>
       </c>
       <c r="O12">
-        <v>-121.443801879882</v>
+        <v>-117.212799072265</v>
       </c>
       <c r="P12" t="s">
         <v>81</v>
@@ -1950,162 +1804,81 @@
         <v>73</v>
       </c>
       <c r="R12" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="S12" t="s">
-        <v>151</v>
-      </c>
-      <c r="T12">
-        <v>1</v>
+        <v>138</v>
       </c>
       <c r="U12" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="V12" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="W12" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="X12" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="Y12" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="Z12" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="AA12" t="s">
         <v>89</v>
       </c>
       <c r="AB12" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="AH12" t="s">
-        <v>75</v>
+        <v>145</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>146</v>
       </c>
       <c r="AJ12" t="s">
         <v>76</v>
       </c>
       <c r="AL12" t="s">
         <v>147</v>
-      </c>
-      <c r="AN12" t="s">
-        <v>158</v>
-      </c>
-      <c r="AO12" t="s">
-        <v>159</v>
-      </c>
-      <c r="AP12" t="s">
-        <v>160</v>
-      </c>
-      <c r="AQ12" t="s">
-        <v>75</v>
-      </c>
-      <c r="AS12">
-        <v>40</v>
-      </c>
-      <c r="AT12">
-        <v>40</v>
-      </c>
-      <c r="AU12">
-        <v>20</v>
-      </c>
-      <c r="AV12">
-        <v>1500</v>
-      </c>
-      <c r="AW12">
-        <v>1700</v>
-      </c>
-      <c r="AX12" t="s">
-        <v>200</v>
-      </c>
-      <c r="AY12" t="s">
-        <v>175</v>
-      </c>
-      <c r="AZ12" t="s">
-        <v>75</v>
-      </c>
-      <c r="BA12" t="s">
-        <v>75</v>
-      </c>
-      <c r="BB12" t="s">
-        <v>201</v>
-      </c>
-      <c r="BD12" t="s">
-        <v>202</v>
-      </c>
-      <c r="BE12" t="s">
-        <v>203</v>
-      </c>
-      <c r="BF12" t="s">
-        <v>204</v>
-      </c>
-      <c r="BH12" t="s">
-        <v>205</v>
-      </c>
-      <c r="BJ12">
-        <v>240</v>
-      </c>
-      <c r="BK12">
-        <v>300</v>
-      </c>
-      <c r="BL12" t="s">
-        <v>206</v>
-      </c>
-      <c r="BM12">
-        <v>5</v>
-      </c>
-      <c r="BN12">
-        <v>180</v>
-      </c>
-      <c r="BO12">
-        <v>500</v>
-      </c>
-      <c r="BP12" t="s">
-        <v>207</v>
-      </c>
-      <c r="BQ12" t="s">
-        <v>208</v>
-      </c>
-      <c r="BR12" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:70">
       <c r="A13">
-        <v>43381.87571759259</v>
+        <v>43381.7379050926</v>
       </c>
       <c r="B13">
-        <v>43381.88489583333</v>
+        <v>43381.75645833334</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="E13">
         <v>100</v>
       </c>
       <c r="F13">
-        <v>793</v>
+        <v>1603</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13">
-        <v>43381.88489583333</v>
+        <v>43381.75645833334</v>
       </c>
       <c r="I13" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="N13">
-        <v>45.5440979003906</v>
+        <v>38.4797058105468</v>
       </c>
       <c r="O13">
-        <v>-122.642303466796</v>
+        <v>-121.443801879882</v>
       </c>
       <c r="P13" t="s">
         <v>81</v>
@@ -2114,93 +1887,162 @@
         <v>73</v>
       </c>
       <c r="R13" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="S13" t="s">
-        <v>164</v>
+        <v>151</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
       </c>
       <c r="U13" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="V13" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="W13" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="X13" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="Y13" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="Z13" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="AA13" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="AB13" t="s">
-        <v>171</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>172</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>173</v>
-      </c>
-      <c r="AE13">
-        <v>98671</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>174</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="AH13" t="s">
-        <v>175</v>
+        <v>75</v>
       </c>
       <c r="AJ13" t="s">
         <v>76</v>
       </c>
       <c r="AL13" t="s">
-        <v>77</v>
+        <v>147</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>158</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>159</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>160</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS13">
+        <v>40</v>
+      </c>
+      <c r="AT13">
+        <v>40</v>
+      </c>
+      <c r="AU13">
+        <v>20</v>
+      </c>
+      <c r="AV13">
+        <v>1500</v>
+      </c>
+      <c r="AW13">
+        <v>1700</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>200</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>175</v>
+      </c>
+      <c r="AZ13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA13" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB13" t="s">
+        <v>201</v>
+      </c>
+      <c r="BD13" t="s">
+        <v>202</v>
+      </c>
+      <c r="BE13" t="s">
+        <v>203</v>
+      </c>
+      <c r="BF13" t="s">
+        <v>204</v>
+      </c>
+      <c r="BH13" t="s">
+        <v>205</v>
+      </c>
+      <c r="BJ13">
+        <v>240</v>
+      </c>
+      <c r="BK13">
+        <v>300</v>
+      </c>
+      <c r="BL13" t="s">
+        <v>206</v>
+      </c>
+      <c r="BM13">
+        <v>5</v>
+      </c>
+      <c r="BN13">
+        <v>180</v>
+      </c>
+      <c r="BO13">
+        <v>500</v>
+      </c>
+      <c r="BP13" t="s">
+        <v>207</v>
+      </c>
+      <c r="BQ13" t="s">
+        <v>208</v>
+      </c>
+      <c r="BR13" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:70">
       <c r="A14">
-        <v>43382.01947916667</v>
+        <v>43381.87571759259</v>
       </c>
       <c r="B14">
-        <v>43382.02648148148</v>
+        <v>43381.88489583333</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="E14">
         <v>100</v>
       </c>
       <c r="F14">
-        <v>604</v>
+        <v>793</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
-        <v>43382.02648148148</v>
+        <v>43381.88489583333</v>
       </c>
       <c r="I14" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="N14">
-        <v>48.465103149414</v>
+        <v>45.5440979003906</v>
       </c>
       <c r="O14">
-        <v>7.95590209960937</v>
+        <v>-122.642303466796</v>
       </c>
       <c r="P14" t="s">
         <v>81</v>
@@ -2209,75 +2051,93 @@
         <v>73</v>
       </c>
       <c r="R14" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="S14" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="U14" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="V14" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="W14" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="X14" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="Y14" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="Z14" t="s">
-        <v>185</v>
+        <v>170</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>101</v>
       </c>
       <c r="AB14" t="s">
-        <v>186</v>
+        <v>171</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>173</v>
+      </c>
+      <c r="AE14">
+        <v>98671</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>174</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>172</v>
       </c>
       <c r="AH14" t="s">
-        <v>75</v>
+        <v>175</v>
       </c>
       <c r="AJ14" t="s">
         <v>76</v>
       </c>
       <c r="AL14" t="s">
-        <v>147</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:70">
       <c r="A15">
-        <v>43382.42454861111</v>
+        <v>43382.01947916667</v>
       </c>
       <c r="B15">
-        <v>43382.44295138889</v>
+        <v>43382.02648148148</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="E15">
         <v>100</v>
       </c>
       <c r="F15">
-        <v>1590</v>
+        <v>604</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15">
-        <v>43382.44296296296</v>
+        <v>43382.02648148148</v>
       </c>
       <c r="I15" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="N15">
-        <v>45.0897064208984</v>
+        <v>48.465103149414</v>
       </c>
       <c r="O15">
-        <v>-123.400299072265</v>
+        <v>7.95590209960937</v>
       </c>
       <c r="P15" t="s">
         <v>81</v>
@@ -2286,52 +2146,31 @@
         <v>73</v>
       </c>
       <c r="R15" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="S15" t="s">
-        <v>190</v>
-      </c>
-      <c r="T15">
-        <v>1</v>
+        <v>179</v>
       </c>
       <c r="U15" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="V15" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="W15" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="X15" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="Y15" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="Z15" t="s">
-        <v>195</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>101</v>
+        <v>185</v>
       </c>
       <c r="AB15" t="s">
-        <v>196</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>197</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>104</v>
-      </c>
-      <c r="AE15">
-        <v>97367</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>198</v>
-      </c>
-      <c r="AG15" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="AH15" t="s">
         <v>75</v>
@@ -2340,81 +2179,179 @@
         <v>76</v>
       </c>
       <c r="AL15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:70">
+      <c r="A16">
+        <v>43382.42454861111</v>
+      </c>
+      <c r="B16">
+        <v>43382.44295138889</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>187</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+      <c r="F16">
+        <v>1590</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>43382.44296296296</v>
+      </c>
+      <c r="I16" t="s">
+        <v>188</v>
+      </c>
+      <c r="N16">
+        <v>45.0897064208984</v>
+      </c>
+      <c r="O16">
+        <v>-123.400299072265</v>
+      </c>
+      <c r="P16" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>73</v>
+      </c>
+      <c r="R16" t="s">
+        <v>189</v>
+      </c>
+      <c r="S16" t="s">
+        <v>190</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16" t="s">
+        <v>191</v>
+      </c>
+      <c r="V16" t="s">
+        <v>192</v>
+      </c>
+      <c r="W16" t="s">
+        <v>193</v>
+      </c>
+      <c r="X16" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>197</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE16">
+        <v>97367</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>198</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>197</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL16" t="s">
         <v>77</v>
       </c>
-      <c r="AN15" t="s">
+      <c r="AN16" t="s">
         <v>190</v>
       </c>
-      <c r="AO15" t="s">
+      <c r="AO16" t="s">
         <v>199</v>
       </c>
-      <c r="AP15" t="s">
+      <c r="AP16" t="s">
         <v>199</v>
       </c>
-      <c r="AQ15" t="s">
+      <c r="AQ16" t="s">
         <v>75</v>
       </c>
-      <c r="AS15">
+      <c r="AS16">
         <v>0</v>
       </c>
-      <c r="AT15">
+      <c r="AT16">
         <v>0</v>
       </c>
-      <c r="AU15">
+      <c r="AU16">
         <v>0</v>
       </c>
-      <c r="AX15" t="s">
+      <c r="AX16" t="s">
         <v>210</v>
       </c>
-      <c r="AY15" t="s">
+      <c r="AY16" t="s">
         <v>175</v>
       </c>
-      <c r="AZ15" t="s">
+      <c r="AZ16" t="s">
         <v>75</v>
       </c>
-      <c r="BA15" t="s">
+      <c r="BA16" t="s">
         <v>175</v>
       </c>
-      <c r="BB15" t="s">
+      <c r="BB16" t="s">
         <v>211</v>
       </c>
-      <c r="BD15" t="s">
+      <c r="BD16" t="s">
         <v>212</v>
       </c>
-      <c r="BE15" t="s">
+      <c r="BE16" t="s">
         <v>213</v>
       </c>
-      <c r="BF15" t="s">
+      <c r="BF16" t="s">
         <v>145</v>
       </c>
-      <c r="BG15" t="s">
+      <c r="BG16" t="s">
         <v>214</v>
       </c>
-      <c r="BH15" t="s">
+      <c r="BH16" t="s">
         <v>215</v>
       </c>
-      <c r="BJ15">
+      <c r="BJ16">
         <v>150</v>
       </c>
-      <c r="BK15" t="s">
+      <c r="BK16" t="s">
         <v>216</v>
       </c>
-      <c r="BL15" t="s">
+      <c r="BL16" t="s">
         <v>206</v>
       </c>
-      <c r="BM15" t="s">
+      <c r="BM16" t="s">
         <v>217</v>
       </c>
-      <c r="BN15" t="s">
+      <c r="BN16" t="s">
         <v>218</v>
       </c>
-      <c r="BP15" t="s">
+      <c r="BP16" t="s">
         <v>219</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="U9" r:id="rId1"/>
+    <hyperlink ref="U10" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added heading for a new section
</commit_message>
<xml_diff>
--- a/Anand_Work/FallWork2018/OUTPUT.xlsx
+++ b/Anand_Work/FallWork2018/OUTPUT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="230">
   <si>
     <t>Start Date</t>
   </si>
@@ -228,6 +228,46 @@
   <si>
     <t>1 - Is there any additional information that you would like to provide regarding facilities and 
 materials?</t>
+  </si>
+  <si>
+    <t>Please indicate who provides instruction to students while at outdoor school:
+ (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - adult volunteers</t>
+  </si>
+  <si>
+    <t>Please indicate who provides instruction to students while at outdoor school:
+ (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - parents</t>
+  </si>
+  <si>
+    <t>Please indicate who provides instruction to students while at outdoor school:
+ (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - college volunteers</t>
+  </si>
+  <si>
+    <t>Please indicate who provides instruction to students while at outdoor school:
+ (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - school teachers</t>
+  </si>
+  <si>
+    <t>Please indicate who provides instruction to students while at outdoor school:
+ (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - school administration</t>
+  </si>
+  <si>
+    <t>Please indicate who provides instruction to students while at outdoor school:
+ (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - high school volunteers</t>
+  </si>
+  <si>
+    <t>Please indicate who provides instruction to students while at outdoor school:
+ (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - trained staff</t>
+  </si>
+  <si>
+    <t>Please indicate who provides instruction to students while at outdoor school:
+ (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - natural resource professionals</t>
+  </si>
+  <si>
+    <t>Please indicate who provides instruction to students while at outdoor school:
+ (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - other</t>
+  </si>
+  <si>
+    <t>Please indicate who provides instruction to students while at outdoor school:
+ (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - other - Text</t>
   </si>
   <si>
     <t>Survey Preview</t>
@@ -1026,13 +1066,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BR16"/>
+  <dimension ref="A1:CF16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:70">
+    <row r="1" spans="1:84">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1243,8 +1283,50 @@
       <c r="BR1" t="s">
         <v>69</v>
       </c>
+      <c r="BS1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="2" spans="1:70">
+    <row r="2" spans="1:84">
       <c r="A2">
         <v>43378.46934027778</v>
       </c>
@@ -1252,7 +1334,7 @@
         <v>43378.47023148148</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -1267,7 +1349,7 @@
         <v>43378.47024305556</v>
       </c>
       <c r="I2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="N2">
         <v>44.5641937255859</v>
@@ -1276,13 +1358,13 @@
         <v>-123.278999328613</v>
       </c>
       <c r="P2" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="Q2" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:70">
+    <row r="3" spans="1:84">
       <c r="A3">
         <v>43378.47028935186</v>
       </c>
@@ -1290,7 +1372,7 @@
         <v>43378.47060185186</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -1305,7 +1387,7 @@
         <v>43378.47060185186</v>
       </c>
       <c r="I3" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="N3">
         <v>44.5641937255859</v>
@@ -1314,22 +1396,22 @@
         <v>-123.278999328613</v>
       </c>
       <c r="P3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="Q3" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="AH3" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="AJ3" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="AL3" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:70">
+    <row r="4" spans="1:84">
       <c r="A4">
         <v>43380.91150462963</v>
       </c>
@@ -1337,7 +1419,7 @@
         <v>43380.91293981481</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -1352,7 +1434,7 @@
         <v>43380.91295138889</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="N4">
         <v>44.5637969970703</v>
@@ -1361,10 +1443,10 @@
         <v>-123.2779006958</v>
       </c>
       <c r="P4" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="Q4" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="T4">
         <v>3</v>
@@ -1379,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:70">
+    <row r="5" spans="1:84">
       <c r="AS5">
         <v>0</v>
       </c>
@@ -1390,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:70">
+    <row r="6" spans="1:84">
       <c r="AS6">
         <v>0</v>
       </c>
@@ -1401,7 +1483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:70">
+    <row r="8" spans="1:84">
       <c r="A8">
         <v>43381.70964120371</v>
       </c>
@@ -1412,7 +1494,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="E8">
         <v>100</v>
@@ -1427,7 +1509,7 @@
         <v>43381.71163194445</v>
       </c>
       <c r="I8" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="N8">
         <v>40.7180023193359</v>
@@ -1436,52 +1518,52 @@
         <v>-74.0754013061523</v>
       </c>
       <c r="P8" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="Q8" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="R8" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="S8" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="U8" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="V8" t="s">
+        <v>95</v>
+      </c>
+      <c r="W8" t="s">
+        <v>96</v>
+      </c>
+      <c r="X8" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH8" t="s">
         <v>85</v>
       </c>
-      <c r="W8" t="s">
+      <c r="AJ8" t="s">
         <v>86</v>
       </c>
-      <c r="X8" t="s">
+      <c r="AL8" t="s">
         <v>87</v>
       </c>
-      <c r="Y8" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>75</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>76</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>77</v>
-      </c>
     </row>
-    <row r="9" spans="1:70">
+    <row r="9" spans="1:84">
       <c r="A9">
         <v>43381.71248842592</v>
       </c>
@@ -1492,7 +1574,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -1507,7 +1589,7 @@
         <v>43381.715</v>
       </c>
       <c r="I9" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="N9">
         <v>45.5653076171875</v>
@@ -1516,67 +1598,67 @@
         <v>-122.644798278808</v>
       </c>
       <c r="P9" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="Q9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="R9" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="S9" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="U9" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="V9" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="W9" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="X9" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="Y9" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="Z9" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AA9" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AB9" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="AC9" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="AD9" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="AE9">
         <v>97055</v>
       </c>
       <c r="AF9" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="AG9" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="AH9" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="AJ9" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="AL9" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:70">
+    <row r="10" spans="1:84">
       <c r="A10">
         <v>43381.71474537037</v>
       </c>
@@ -1587,7 +1669,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E10">
         <v>100</v>
@@ -1602,7 +1684,7 @@
         <v>43381.71667824074</v>
       </c>
       <c r="I10" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="N10">
         <v>44.0682067871093</v>
@@ -1611,67 +1693,67 @@
         <v>-123.081901550292</v>
       </c>
       <c r="P10" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="Q10" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="R10" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="S10" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="U10" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="V10" t="s">
+        <v>122</v>
+      </c>
+      <c r="W10" t="s">
+        <v>123</v>
+      </c>
+      <c r="X10" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA10" t="s">
         <v>111</v>
       </c>
-      <c r="V10" t="s">
-        <v>112</v>
-      </c>
-      <c r="W10" t="s">
-        <v>113</v>
-      </c>
-      <c r="X10" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>101</v>
-      </c>
       <c r="AB10" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="AC10" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="AD10" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="AE10">
         <v>97419</v>
       </c>
       <c r="AF10" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="AG10" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="AH10" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="AJ10" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="AL10" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:70">
+    <row r="11" spans="1:84">
       <c r="A11">
         <v>43381.71635416667</v>
       </c>
@@ -1682,7 +1764,7 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="E11">
         <v>100</v>
@@ -1697,7 +1779,7 @@
         <v>43381.72159722223</v>
       </c>
       <c r="I11" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="N11">
         <v>45.3726959228515</v>
@@ -1706,64 +1788,64 @@
         <v>-122.76309967041</v>
       </c>
       <c r="P11" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="Q11" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="R11" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="S11" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="U11" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="V11" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="W11" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="X11" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="Y11" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="AA11" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AB11" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="AC11" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="AD11" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="AE11">
         <v>97064</v>
       </c>
       <c r="AF11" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="AG11" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="AH11" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="AJ11" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="AL11" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:70">
+    <row r="12" spans="1:84">
       <c r="A12">
         <v>43381.74771990741</v>
       </c>
@@ -1774,7 +1856,7 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="E12">
         <v>100</v>
@@ -1789,7 +1871,7 @@
         <v>43381.75016203704</v>
       </c>
       <c r="I12" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="N12">
         <v>45.3493957519531</v>
@@ -1798,55 +1880,55 @@
         <v>-117.212799072265</v>
       </c>
       <c r="P12" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="Q12" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="R12" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="S12" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="U12" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="V12" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="W12" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="X12" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="Y12" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="Z12" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="AA12" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="AB12" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="AH12" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="AI12" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="AJ12" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="AL12" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:70">
+    <row r="13" spans="1:84">
       <c r="A13">
         <v>43381.7379050926</v>
       </c>
@@ -1857,7 +1939,7 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="E13">
         <v>100</v>
@@ -1872,7 +1954,7 @@
         <v>43381.75645833334</v>
       </c>
       <c r="I13" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="N13">
         <v>38.4797058105468</v>
@@ -1881,64 +1963,64 @@
         <v>-121.443801879882</v>
       </c>
       <c r="P13" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="Q13" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="R13" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="S13" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="T13">
         <v>1</v>
       </c>
       <c r="U13" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="V13" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="W13" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="X13" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Y13" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="Z13" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="AA13" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="AB13" t="s">
+        <v>167</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL13" t="s">
         <v>157</v>
       </c>
-      <c r="AH13" t="s">
-        <v>75</v>
-      </c>
-      <c r="AJ13" t="s">
-        <v>76</v>
-      </c>
-      <c r="AL13" t="s">
-        <v>147</v>
-      </c>
       <c r="AN13" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="AO13" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="AP13" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="AQ13" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="AS13">
         <v>40</v>
@@ -1956,31 +2038,31 @@
         <v>1700</v>
       </c>
       <c r="AX13" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="AY13" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="AZ13" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="BA13" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="BB13" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="BD13" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="BE13" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="BF13" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="BH13" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="BJ13">
         <v>240</v>
@@ -1989,7 +2071,7 @@
         <v>300</v>
       </c>
       <c r="BL13" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="BM13">
         <v>5</v>
@@ -2001,16 +2083,16 @@
         <v>500</v>
       </c>
       <c r="BP13" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="BQ13" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="BR13" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:70">
+    <row r="14" spans="1:84">
       <c r="A14">
         <v>43381.87571759259</v>
       </c>
@@ -2021,7 +2103,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="E14">
         <v>100</v>
@@ -2036,7 +2118,7 @@
         <v>43381.88489583333</v>
       </c>
       <c r="I14" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="N14">
         <v>45.5440979003906</v>
@@ -2045,67 +2127,67 @@
         <v>-122.642303466796</v>
       </c>
       <c r="P14" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="Q14" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="R14" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="S14" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="U14" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="V14" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="W14" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="X14" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="Y14" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="Z14" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="AA14" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AB14" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="AC14" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="AD14" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="AE14">
         <v>98671</v>
       </c>
       <c r="AF14" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="AG14" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="AH14" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="AJ14" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="AL14" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:70">
+    <row r="15" spans="1:84">
       <c r="A15">
         <v>43382.01947916667</v>
       </c>
@@ -2116,7 +2198,7 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="E15">
         <v>100</v>
@@ -2131,7 +2213,7 @@
         <v>43382.02648148148</v>
       </c>
       <c r="I15" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="N15">
         <v>48.465103149414</v>
@@ -2140,49 +2222,49 @@
         <v>7.95590209960937</v>
       </c>
       <c r="P15" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="Q15" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="R15" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="S15" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="U15" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="V15" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="W15" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="X15" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="Y15" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="Z15" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="AB15" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="AH15" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="AJ15" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="AL15" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:70">
+    <row r="16" spans="1:84">
       <c r="A16">
         <v>43382.42454861111</v>
       </c>
@@ -2193,7 +2275,7 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="E16">
         <v>100</v>
@@ -2208,7 +2290,7 @@
         <v>43382.44296296296</v>
       </c>
       <c r="I16" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="N16">
         <v>45.0897064208984</v>
@@ -2217,79 +2299,79 @@
         <v>-123.400299072265</v>
       </c>
       <c r="P16" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="Q16" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="R16" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="S16" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="T16">
         <v>1</v>
       </c>
       <c r="U16" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="V16" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="W16" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="X16" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="Y16" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="Z16" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="AA16" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AB16" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="AC16" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="AD16" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="AE16">
         <v>97367</v>
       </c>
       <c r="AF16" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="AG16" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="AH16" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="AJ16" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="AL16" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="AN16" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="AO16" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="AP16" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="AQ16" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="AS16">
         <v>0</v>
@@ -2301,52 +2383,52 @@
         <v>0</v>
       </c>
       <c r="AX16" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="AY16" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="AZ16" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="BA16" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="BB16" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="BD16" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="BE16" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="BF16" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="BG16" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="BH16" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="BJ16">
         <v>150</v>
       </c>
       <c r="BK16" t="s">
+        <v>226</v>
+      </c>
+      <c r="BL16" t="s">
         <v>216</v>
       </c>
-      <c r="BL16" t="s">
-        <v>206</v>
-      </c>
       <c r="BM16" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="BN16" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="BP16" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed sections appropriately, done with section 5
</commit_message>
<xml_diff>
--- a/Anand_Work/FallWork2018/OUTPUT.xlsx
+++ b/Anand_Work/FallWork2018/OUTPUT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="363">
   <si>
     <t>Start Date</t>
   </si>
@@ -151,18 +151,18 @@
     <t>What is the percentage of â€˜awakeâ€™ time that youth spend engaged in instruction? (Instructional Activities: structured or unstructured activities with explicit learning objectives) - 1 - % of time</t>
   </si>
   <si>
-    <t>What is the percentage of â€˜awakeâ€™ time that youth spend engaged in other activities?
+    <t>What is the percentage of â€˜awakeâ€™ time that youth spend engaged in other activities?_x000D_
 (Other Activities: structured time without explicit learning objectives) - 1 - % of time</t>
   </si>
   <si>
-    <t>What is the percentage of â€˜awakeâ€™ time that youth spend engaged in free-time?
+    <t>What is the percentage of â€˜awakeâ€™ time that youth spend engaged in free-time?_x000D_
 (Free activities: unstructured time without explicit learning objectives) - 1 - % of time</t>
   </si>
   <si>
     <t>1 - How many 5th/6th grade students attended your outdoor school program last school year?</t>
   </si>
   <si>
-    <t>1 - How many 5th/6th grade students do you expect to attend your outdoor school program this
+    <t>1 - How many 5th/6th grade students do you expect to attend your outdoor school program this_x000D_
 current/upcoming school year?</t>
   </si>
   <si>
@@ -226,47 +226,47 @@
     <t>1 - What are the biggest unmet facility and material needs for your outdoor school?</t>
   </si>
   <si>
-    <t>1 - Is there any additional information that you would like to provide regarding facilities and 
+    <t>1 - Is there any additional information that you would like to provide regarding facilities and _x000D_
 materials?</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - adult volunteers</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - parents</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - college volunteers</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - school teachers</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - school administration</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - high school volunteers</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - trained staff</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - natural resource professionals</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - other</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - other - Text</t>
   </si>
   <si>
@@ -360,7 +360,7 @@
     <t>afreeberg@campfireclolumbia.org</t>
   </si>
   <si>
-    <t>1411 SW Morrison St #300
+    <t>1411 SW Morrison St #300_x000D_
 Portland, O 97205</t>
   </si>
   <si>
@@ -409,7 +409,7 @@
     <t>matt@wholeearthschool.com</t>
   </si>
   <si>
-    <t>150 Shelton McMurphy Blvd Suite 206
+    <t>150 Shelton McMurphy Blvd Suite 206_x000D_
 Eugene, OR 97401</t>
   </si>
   <si>
@@ -530,7 +530,7 @@
     <t>Young</t>
   </si>
   <si>
-    <t>37028 Shoreview Dr.
+    <t>37028 Shoreview Dr._x000D_
 Dorena, OR 97434</t>
   </si>
   <si>
@@ -648,7 +648,7 @@
     <t>Kauffman</t>
   </si>
   <si>
-    <t>22455 Finn Road
+    <t>22455 Finn Road_x000D_
 Sheridan, OR 97378</t>
   </si>
   <si>
@@ -664,6 +664,227 @@
     <t>varies</t>
   </si>
   <si>
+    <t>66.228.26.105</t>
+  </si>
+  <si>
+    <t>R_1ovtwrJr01IjYRu</t>
+  </si>
+  <si>
+    <t>office@campmorrow.org</t>
+  </si>
+  <si>
+    <t>Camp Morrow</t>
+  </si>
+  <si>
+    <t>www.campmorrow.org</t>
+  </si>
+  <si>
+    <t>541-544-2971</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>Birman</t>
+  </si>
+  <si>
+    <t>jason@campmorrow.org</t>
+  </si>
+  <si>
+    <t>79551 Morrow Rd. Wamic, OR 97063</t>
+  </si>
+  <si>
+    <t>September-May (traditional school year calendar)</t>
+  </si>
+  <si>
+    <t>Camp Morrow Lake Camp</t>
+  </si>
+  <si>
+    <t>Currently we have one school that comes and does there own programming/teaching.  They come for 3 days, but we could go up to 5 days.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The current school stays 2 nights, but we can accommodate up to 4 nights.  </t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>72.173.163.86</t>
+  </si>
+  <si>
+    <t>R_DiQdJ5rTP5VjUwF</t>
+  </si>
+  <si>
+    <t>fortin@awsp.org</t>
+  </si>
+  <si>
+    <t>Assocaition of Washington School Principals Learning Centers</t>
+  </si>
+  <si>
+    <t>http://www.awsplearningcenters.org/</t>
+  </si>
+  <si>
+    <t>360-497-7131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin </t>
+  </si>
+  <si>
+    <t>Fortin</t>
+  </si>
+  <si>
+    <t>2142 Cispus Rd _x000D_
+Randle WA 98377</t>
+  </si>
+  <si>
+    <t>Cispus Learning Center</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>We provide the facilities, schools bring their program</t>
+  </si>
+  <si>
+    <t>Chwelah Peak Learning Center</t>
+  </si>
+  <si>
+    <t>We ptrovide the facilty, the schools bring the program</t>
+  </si>
+  <si>
+    <t>73.96.218.63</t>
+  </si>
+  <si>
+    <t>R_Tpcop4aL1x25mXD</t>
+  </si>
+  <si>
+    <t>camp@taloali.org</t>
+  </si>
+  <si>
+    <t>Camp Taloali</t>
+  </si>
+  <si>
+    <t>www.taloali.org</t>
+  </si>
+  <si>
+    <t>503-400-6437</t>
+  </si>
+  <si>
+    <t>Janet</t>
+  </si>
+  <si>
+    <t>Johanson</t>
+  </si>
+  <si>
+    <t>PO Box 32 Stayton, OR 97383</t>
+  </si>
+  <si>
+    <t>School Year</t>
+  </si>
+  <si>
+    <t>Stayton</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>Marion</t>
+  </si>
+  <si>
+    <t>Stayton, Oregon</t>
+  </si>
+  <si>
+    <t>76.2.16.81</t>
+  </si>
+  <si>
+    <t>R_3kukFuaEHldBjUj</t>
+  </si>
+  <si>
+    <t>Erynne@cascademountainschool.org</t>
+  </si>
+  <si>
+    <t>Mt. Adams Institute's Cascade Mountain School</t>
+  </si>
+  <si>
+    <t>www.cascademountainschool.org &amp; www.mtadamsinstitute.org</t>
+  </si>
+  <si>
+    <t>541-740-9951</t>
+  </si>
+  <si>
+    <t>Erynne</t>
+  </si>
+  <si>
+    <t>VanZee</t>
+  </si>
+  <si>
+    <t>erynne@cascademountainschool.org</t>
+  </si>
+  <si>
+    <t>2453 Highway 141, Trout Lake, Washington 98650</t>
+  </si>
+  <si>
+    <t>April to October</t>
+  </si>
+  <si>
+    <t>Full service outdoor school (both facility and provider)</t>
+  </si>
+  <si>
+    <t>50.76.96.250</t>
+  </si>
+  <si>
+    <t>R_1OHPeQk238fuNz3</t>
+  </si>
+  <si>
+    <t>bo.henderson@scouting.org</t>
+  </si>
+  <si>
+    <t>Cascade Pacific Council, BSA</t>
+  </si>
+  <si>
+    <t>www.cpcbsa.org</t>
+  </si>
+  <si>
+    <t>503-225-5744</t>
+  </si>
+  <si>
+    <t>Bo</t>
+  </si>
+  <si>
+    <t>Henderson</t>
+  </si>
+  <si>
+    <t>2145 SW Naito Pkwy_x000D_
+Portland, OR 97201</t>
+  </si>
+  <si>
+    <t>September 1 - May 31</t>
+  </si>
+  <si>
+    <t>Cloverdale</t>
+  </si>
+  <si>
+    <t>Tillamook</t>
+  </si>
+  <si>
+    <t>Pacific City</t>
+  </si>
+  <si>
+    <t>Camp Meriwether</t>
+  </si>
+  <si>
+    <t>set by provider</t>
+  </si>
+  <si>
+    <t>Camp Clark</t>
+  </si>
+  <si>
+    <t>Camp Baldwin</t>
+  </si>
+  <si>
+    <t>Butte Creek Scout Ranch</t>
+  </si>
+  <si>
     <t>We have an emergency action plan written up. Speed dial set to 911, AED system for facility, walker talkies on staff leaders.</t>
   </si>
   <si>
@@ -722,6 +943,187 @@
   </si>
   <si>
     <t xml:space="preserve">Yes, we have two main floor rooms available in the lodge that are accessible and the Alsea cabin is also accessible. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">80 acres </t>
+  </si>
+  <si>
+    <t xml:space="preserve">creek, lake, high desert climate, forest (mostly pine and oak trees).  </t>
+  </si>
+  <si>
+    <t>Schools have the option of us providing food service or they can provide food service.</t>
+  </si>
+  <si>
+    <t>Yes (if yes, please check all that apply),Gluten/wheat allergies,Dairy allergies (milk and/or egg),Soy, peanut, or tree nut allergies,Seafood or shellfish allergies</t>
+  </si>
+  <si>
+    <t>150 in a multi purpose room.  Audio/visual and chairs provided.  A/C and heated building. There is also a small heated room for smaller group of 15.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150  Mostly bunk-bed style housing in heated cabins.  There are a few queen beds.   Bathrooms are located in separate buildings. </t>
+  </si>
+  <si>
+    <t>We have areas that tents can be set up and we have RV sites (both full hook ups and partial hook ups).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most of our facility is wheelchair accessible.  There would only be a few cabins not accessible. </t>
+  </si>
+  <si>
+    <t>WE have mobile radios that are tied to the local Fire Department/EMT</t>
+  </si>
+  <si>
+    <t>Paved road,Extra large vehicle (Such semi-tuck with trailer, standard bus, class A RV)</t>
+  </si>
+  <si>
+    <t>Forst, creek, river, pond</t>
+  </si>
+  <si>
+    <t>Yes (if yes, please check all that apply),Vegetarian,Vegan,Kosher,Hallal,Diabetic Meal plan,Gluten/wheat allergies,Dairy allergies (milk and/or egg),Soy, peanut, or tree nut allergies,Seafood or shellfish allergies</t>
+  </si>
+  <si>
+    <t>20 rooms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">364 Bunk bed in dorms </t>
+  </si>
+  <si>
+    <t>350 in tents of the group brings them</t>
+  </si>
+  <si>
+    <t>yes, wheelchair ramps, accesible rest rooms and showers</t>
+  </si>
+  <si>
+    <t>More private type rooms for adults</t>
+  </si>
+  <si>
+    <t>We have a huge challenge course- 45+ low events, plus 6 high elements.</t>
+  </si>
+  <si>
+    <t>Land lines and cell service to call for help</t>
+  </si>
+  <si>
+    <t>Gravel/dirt road,Extra large vehicle (Such semi-tuck with trailer, standard bus, class A RV)</t>
+  </si>
+  <si>
+    <t>20 acres</t>
+  </si>
+  <si>
+    <t>Forest, creek, logged area</t>
+  </si>
+  <si>
+    <t>200 if schools bring tents</t>
+  </si>
+  <si>
+    <t>yes, wheelchair ramps, accessible showers and toliets</t>
+  </si>
+  <si>
+    <t>more beds needed</t>
+  </si>
+  <si>
+    <t>we have an artificial stream to teach panning techniques</t>
+  </si>
+  <si>
+    <t>VHF radio system with repeater</t>
+  </si>
+  <si>
+    <t>Gravel/dirt road,Extra large vehicle (Such semi-tuck with trailer, standard bus, class A RV),Large vehicles (such as semi without trailer, short bus length, Class C RV, truck with trailer),Standard vehicle (Such as truck without trailer, SUV, sedan),Small vehicle (Such as motorcycle, hybrid, smart car),Horse/Pack animal</t>
+  </si>
+  <si>
+    <t>several coastal biomes, tide pools, 2.5 miles of Pacific Ocean exclusive beach access, cape lookout and several salmon streams</t>
+  </si>
+  <si>
+    <t>Food Service is available.  We can provide or district can provide</t>
+  </si>
+  <si>
+    <t>9/600</t>
+  </si>
+  <si>
+    <t>Currently 96 housed in 6 duplex cabins that can accommodate 8 persons per side._x000D_
+  We are however running a capital campaign to expand this offering by an additional 192 persons in similarly sized cabins.  Expected completion in 2020.</t>
+  </si>
+  <si>
+    <t>542 housed in 3 walled structures with custom canvas doors, lighting and heat.  These structures sleep 6 and are grouped together in units of 5-7.</t>
+  </si>
+  <si>
+    <t>Various locations at the facility can be used by folks with assessiblity needs.  To fully accomodate everyone, dialogue would need to occur with the provider so we can be sure to fully understand the needs of specific individuals and work to accommodate them on a case by case basis..</t>
+  </si>
+  <si>
+    <t>Indoor Housing</t>
+  </si>
+  <si>
+    <t>Currently OMSI is using this facility as an additional location to their Newport Facility for Outdoor School beginning Spring of 2019.</t>
+  </si>
+  <si>
+    <t>same as Facility 1</t>
+  </si>
+  <si>
+    <t>Yes (if yes, please check all that apply),Vegetarian,Vegan,Kosher,Hallal,Gluten/wheat allergies,Dairy allergies (milk and/or egg),Soy, peanut, or tree nut allergies,Seafood or shellfish allergies</t>
+  </si>
+  <si>
+    <t>1 / 257</t>
+  </si>
+  <si>
+    <t>capacity of 44 in 9 rustic cabins and 2 recently constructed cabins.</t>
+  </si>
+  <si>
+    <t>250 capacity in small two person structures with canvas doors grouped in units of 12-16</t>
+  </si>
+  <si>
+    <t>UHF Radio System</t>
+  </si>
+  <si>
+    <t>Timberline bordering Eastern Oregon Savanna, shaded creeks and marsh</t>
+  </si>
+  <si>
+    <t>4/100</t>
+  </si>
+  <si>
+    <t>68 in 9 cabins constructed in 2015.  each cabin is one room that houses 8.  Cabins are heated, have electricity and insulated.</t>
+  </si>
+  <si>
+    <t>0 unless groups wanted to bring tents then closer to 350</t>
+  </si>
+  <si>
+    <t>Indoor housing and eating capacity are to double within the next 3 years.</t>
+  </si>
+  <si>
+    <t>UHF Radios</t>
+  </si>
+  <si>
+    <t>This facility is a working ranch.  property stadles Butte Creek (the border of Marion and Clackamas Counties</t>
+  </si>
+  <si>
+    <t>1/250  the Barn and Riding Arenas can be used as well</t>
+  </si>
+  <si>
+    <t>Same as Facility 2</t>
+  </si>
+  <si>
+    <t>We are working on designs for dormitory cabins to house around 256.  Facilities 1, 2, and 3 take priority.  A set construction date has not been determined.</t>
+  </si>
+  <si>
+    <t>Extremely Responsible</t>
+  </si>
+  <si>
+    <t>Somewhat responsible</t>
+  </si>
+  <si>
+    <t>Responsible</t>
+  </si>
+  <si>
+    <t>Not at all responsible</t>
+  </si>
+  <si>
+    <t>Forest service</t>
+  </si>
+  <si>
+    <t>Fish and wildlife</t>
+  </si>
+  <si>
+    <t>Other professionals</t>
+  </si>
+  <si>
+    <t>we are not the instructional providers</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1468,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CF16"/>
+  <dimension ref="A1:CF26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2038,7 +2440,7 @@
         <v>1700</v>
       </c>
       <c r="AX13" t="s">
-        <v>210</v>
+        <v>283</v>
       </c>
       <c r="AY13" t="s">
         <v>185</v>
@@ -2050,19 +2452,19 @@
         <v>85</v>
       </c>
       <c r="BB13" t="s">
-        <v>211</v>
+        <v>284</v>
       </c>
       <c r="BD13" t="s">
-        <v>212</v>
+        <v>285</v>
       </c>
       <c r="BE13" t="s">
-        <v>213</v>
+        <v>286</v>
       </c>
       <c r="BF13" t="s">
-        <v>214</v>
+        <v>287</v>
       </c>
       <c r="BH13" t="s">
-        <v>215</v>
+        <v>288</v>
       </c>
       <c r="BJ13">
         <v>240</v>
@@ -2071,7 +2473,7 @@
         <v>300</v>
       </c>
       <c r="BL13" t="s">
-        <v>216</v>
+        <v>289</v>
       </c>
       <c r="BM13">
         <v>5</v>
@@ -2083,13 +2485,52 @@
         <v>500</v>
       </c>
       <c r="BP13" t="s">
-        <v>217</v>
+        <v>290</v>
       </c>
       <c r="BQ13" t="s">
-        <v>218</v>
+        <v>291</v>
       </c>
       <c r="BR13" t="s">
-        <v>219</v>
+        <v>292</v>
+      </c>
+      <c r="BS13" t="s">
+        <v>355</v>
+      </c>
+      <c r="BT13" t="s">
+        <v>356</v>
+      </c>
+      <c r="BU13" t="s">
+        <v>355</v>
+      </c>
+      <c r="BV13" t="s">
+        <v>357</v>
+      </c>
+      <c r="BW13" t="s">
+        <v>358</v>
+      </c>
+      <c r="BX13" t="s">
+        <v>358</v>
+      </c>
+      <c r="BY13" t="s">
+        <v>357</v>
+      </c>
+      <c r="CA13" t="s">
+        <v>355</v>
+      </c>
+      <c r="CB13" t="s">
+        <v>359</v>
+      </c>
+      <c r="CC13" t="s">
+        <v>355</v>
+      </c>
+      <c r="CD13" t="s">
+        <v>360</v>
+      </c>
+      <c r="CE13" t="s">
+        <v>355</v>
+      </c>
+      <c r="CF13" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="14" spans="1:84">
@@ -2383,7 +2824,7 @@
         <v>0</v>
       </c>
       <c r="AX16" t="s">
-        <v>220</v>
+        <v>293</v>
       </c>
       <c r="AY16" t="s">
         <v>185</v>
@@ -2395,45 +2836,1261 @@
         <v>185</v>
       </c>
       <c r="BB16" t="s">
-        <v>221</v>
+        <v>294</v>
       </c>
       <c r="BD16" t="s">
-        <v>222</v>
+        <v>295</v>
       </c>
       <c r="BE16" t="s">
-        <v>223</v>
+        <v>296</v>
       </c>
       <c r="BF16" t="s">
         <v>155</v>
       </c>
       <c r="BG16" t="s">
-        <v>224</v>
+        <v>297</v>
       </c>
       <c r="BH16" t="s">
-        <v>225</v>
+        <v>298</v>
       </c>
       <c r="BJ16">
         <v>150</v>
       </c>
       <c r="BK16" t="s">
+        <v>299</v>
+      </c>
+      <c r="BL16" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM16" t="s">
+        <v>300</v>
+      </c>
+      <c r="BN16" t="s">
+        <v>301</v>
+      </c>
+      <c r="BP16" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:84">
+      <c r="A17">
+        <v>43382.4278125</v>
+      </c>
+      <c r="B17">
+        <v>43382.45159722222</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>210</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="F17">
+        <v>2055</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>43382.4516087963</v>
+      </c>
+      <c r="I17" t="s">
+        <v>211</v>
+      </c>
+      <c r="N17">
+        <v>45.222900390625</v>
+      </c>
+      <c r="O17">
+        <v>-121.292701721191</v>
+      </c>
+      <c r="P17" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>83</v>
+      </c>
+      <c r="R17" t="s">
+        <v>212</v>
+      </c>
+      <c r="S17" t="s">
+        <v>213</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17" t="s">
+        <v>214</v>
+      </c>
+      <c r="V17" t="s">
+        <v>215</v>
+      </c>
+      <c r="W17" t="s">
+        <v>216</v>
+      </c>
+      <c r="X17" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>218</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>220</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>221</v>
+      </c>
+      <c r="AO17" t="s">
+        <v>222</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>223</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>224</v>
+      </c>
+      <c r="AS17">
+        <v>0</v>
+      </c>
+      <c r="AT17">
+        <v>0</v>
+      </c>
+      <c r="AU17">
+        <v>0</v>
+      </c>
+      <c r="AV17">
+        <v>20</v>
+      </c>
+      <c r="AW17">
+        <v>20</v>
+      </c>
+      <c r="AY17" t="s">
+        <v>85</v>
+      </c>
+      <c r="AZ17" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA17" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB17" t="s">
+        <v>294</v>
+      </c>
+      <c r="BD17" t="s">
+        <v>303</v>
+      </c>
+      <c r="BE17" t="s">
+        <v>304</v>
+      </c>
+      <c r="BF17" t="s">
+        <v>155</v>
+      </c>
+      <c r="BG17" t="s">
+        <v>305</v>
+      </c>
+      <c r="BH17" t="s">
+        <v>306</v>
+      </c>
+      <c r="BJ17">
+        <v>150</v>
+      </c>
+      <c r="BK17">
+        <v>50</v>
+      </c>
+      <c r="BL17" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM17" t="s">
+        <v>307</v>
+      </c>
+      <c r="BN17" t="s">
+        <v>308</v>
+      </c>
+      <c r="BO17" t="s">
+        <v>309</v>
+      </c>
+      <c r="BP17" t="s">
+        <v>310</v>
+      </c>
+      <c r="BS17" t="s">
+        <v>355</v>
+      </c>
+      <c r="BT17" t="s">
+        <v>355</v>
+      </c>
+      <c r="BV17" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="18" spans="1:84">
+      <c r="A18">
+        <v>43382.50405092593</v>
+      </c>
+      <c r="B18">
+        <v>43382.5228125</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>225</v>
+      </c>
+      <c r="E18">
+        <v>100</v>
+      </c>
+      <c r="F18">
+        <v>1621</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>43382.52282407408</v>
+      </c>
+      <c r="I18" t="s">
         <v>226</v>
       </c>
-      <c r="BL16" t="s">
-        <v>216</v>
-      </c>
-      <c r="BM16" t="s">
+      <c r="N18">
+        <v>46.5491943359375</v>
+      </c>
+      <c r="O18">
+        <v>-121.855499267578</v>
+      </c>
+      <c r="P18" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>83</v>
+      </c>
+      <c r="R18" t="s">
         <v>227</v>
       </c>
-      <c r="BN16" t="s">
+      <c r="S18" t="s">
         <v>228</v>
       </c>
-      <c r="BP16" t="s">
+      <c r="T18">
+        <v>2</v>
+      </c>
+      <c r="U18" s="1" t="s">
         <v>229</v>
+      </c>
+      <c r="V18" t="s">
+        <v>230</v>
+      </c>
+      <c r="W18" t="s">
+        <v>231</v>
+      </c>
+      <c r="X18" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>233</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>167</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN18" t="s">
+        <v>234</v>
+      </c>
+      <c r="AO18" t="s">
+        <v>235</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>235</v>
+      </c>
+      <c r="AQ18" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>236</v>
+      </c>
+      <c r="AS18">
+        <v>0</v>
+      </c>
+      <c r="AT18">
+        <v>0</v>
+      </c>
+      <c r="AU18">
+        <v>0</v>
+      </c>
+      <c r="AV18">
+        <v>2900</v>
+      </c>
+      <c r="AW18">
+        <v>2900</v>
+      </c>
+      <c r="AX18" t="s">
+        <v>311</v>
+      </c>
+      <c r="AY18" t="s">
+        <v>185</v>
+      </c>
+      <c r="AZ18" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA18" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB18" t="s">
+        <v>312</v>
+      </c>
+      <c r="BD18">
+        <v>68</v>
+      </c>
+      <c r="BE18" t="s">
+        <v>313</v>
+      </c>
+      <c r="BF18" t="s">
+        <v>287</v>
+      </c>
+      <c r="BH18" t="s">
+        <v>314</v>
+      </c>
+      <c r="BJ18">
+        <v>350</v>
+      </c>
+      <c r="BK18">
+        <v>350</v>
+      </c>
+      <c r="BL18" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM18" t="s">
+        <v>315</v>
+      </c>
+      <c r="BN18" t="s">
+        <v>316</v>
+      </c>
+      <c r="BO18" t="s">
+        <v>317</v>
+      </c>
+      <c r="BP18" t="s">
+        <v>318</v>
+      </c>
+      <c r="BQ18" t="s">
+        <v>319</v>
+      </c>
+      <c r="BR18" t="s">
+        <v>320</v>
+      </c>
+      <c r="BS18" t="s">
+        <v>357</v>
+      </c>
+      <c r="BT18" t="s">
+        <v>357</v>
+      </c>
+      <c r="BV18" t="s">
+        <v>355</v>
+      </c>
+      <c r="BW18" t="s">
+        <v>356</v>
+      </c>
+      <c r="BX18" t="s">
+        <v>357</v>
+      </c>
+      <c r="BY18" t="s">
+        <v>358</v>
+      </c>
+      <c r="BZ18" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="19" spans="1:84">
+      <c r="AN19" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO19" t="s">
+        <v>235</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>235</v>
+      </c>
+      <c r="AQ19" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR19" t="s">
+        <v>238</v>
+      </c>
+      <c r="AS19">
+        <v>0</v>
+      </c>
+      <c r="AT19">
+        <v>0</v>
+      </c>
+      <c r="AU19">
+        <v>0</v>
+      </c>
+      <c r="AV19">
+        <v>693</v>
+      </c>
+      <c r="AW19">
+        <v>700</v>
+      </c>
+      <c r="AX19" t="s">
+        <v>321</v>
+      </c>
+      <c r="AY19" t="s">
+        <v>85</v>
+      </c>
+      <c r="AZ19" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA19" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB19" t="s">
+        <v>322</v>
+      </c>
+      <c r="BD19" t="s">
+        <v>323</v>
+      </c>
+      <c r="BE19" t="s">
+        <v>324</v>
+      </c>
+      <c r="BF19" t="s">
+        <v>287</v>
+      </c>
+      <c r="BH19" t="s">
+        <v>314</v>
+      </c>
+      <c r="BJ19">
+        <v>200</v>
+      </c>
+      <c r="BK19">
+        <v>200</v>
+      </c>
+      <c r="BL19" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM19">
+        <v>10</v>
+      </c>
+      <c r="BN19">
+        <v>196</v>
+      </c>
+      <c r="BO19" t="s">
+        <v>325</v>
+      </c>
+      <c r="BP19" t="s">
+        <v>326</v>
+      </c>
+      <c r="BQ19" t="s">
+        <v>327</v>
+      </c>
+      <c r="BR19" t="s">
+        <v>328</v>
+      </c>
+      <c r="BS19" t="s">
+        <v>357</v>
+      </c>
+      <c r="BT19" t="s">
+        <v>357</v>
+      </c>
+      <c r="BU19" t="s">
+        <v>356</v>
+      </c>
+      <c r="BV19" t="s">
+        <v>355</v>
+      </c>
+      <c r="BW19" t="s">
+        <v>356</v>
+      </c>
+      <c r="BX19" t="s">
+        <v>357</v>
+      </c>
+      <c r="BY19" t="s">
+        <v>358</v>
+      </c>
+      <c r="BZ19" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="21" spans="1:84">
+      <c r="A21">
+        <v>43382.63195601852</v>
+      </c>
+      <c r="B21">
+        <v>43382.63358796296</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>239</v>
+      </c>
+      <c r="E21">
+        <v>100</v>
+      </c>
+      <c r="F21">
+        <v>140</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>43382.63358796296</v>
+      </c>
+      <c r="I21" t="s">
+        <v>240</v>
+      </c>
+      <c r="N21">
+        <v>44.9490051269531</v>
+      </c>
+      <c r="O21">
+        <v>-123.003997802734</v>
+      </c>
+      <c r="P21" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>83</v>
+      </c>
+      <c r="R21" t="s">
+        <v>241</v>
+      </c>
+      <c r="S21" t="s">
+        <v>242</v>
+      </c>
+      <c r="U21" t="s">
+        <v>243</v>
+      </c>
+      <c r="V21" t="s">
+        <v>244</v>
+      </c>
+      <c r="W21" t="s">
+        <v>245</v>
+      </c>
+      <c r="X21" t="s">
+        <v>246</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>247</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>248</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>249</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>250</v>
+      </c>
+      <c r="AE21">
+        <v>97383</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>252</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:84">
+      <c r="A22">
+        <v>43383.43930555556</v>
+      </c>
+      <c r="B22">
+        <v>43383.45842592593</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>253</v>
+      </c>
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>1651</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>43383.45842592593</v>
+      </c>
+      <c r="I22" t="s">
+        <v>254</v>
+      </c>
+      <c r="N22">
+        <v>45.9828033447265</v>
+      </c>
+      <c r="O22">
+        <v>-121.516296386718</v>
+      </c>
+      <c r="P22" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>83</v>
+      </c>
+      <c r="R22" t="s">
+        <v>255</v>
+      </c>
+      <c r="S22" t="s">
+        <v>256</v>
+      </c>
+      <c r="U22" t="s">
+        <v>257</v>
+      </c>
+      <c r="V22" t="s">
+        <v>258</v>
+      </c>
+      <c r="W22" t="s">
+        <v>259</v>
+      </c>
+      <c r="X22" t="s">
+        <v>260</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>261</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>262</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>263</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:84">
+      <c r="A23">
+        <v>43383.49253472222</v>
+      </c>
+      <c r="B23">
+        <v>43383.52399305555</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>265</v>
+      </c>
+      <c r="E23">
+        <v>100</v>
+      </c>
+      <c r="F23">
+        <v>2717</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>43383.52400462963</v>
+      </c>
+      <c r="I23" t="s">
+        <v>266</v>
+      </c>
+      <c r="N23">
+        <v>45.5077972412109</v>
+      </c>
+      <c r="O23">
+        <v>-122.689697265625</v>
+      </c>
+      <c r="P23" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>83</v>
+      </c>
+      <c r="R23" t="s">
+        <v>267</v>
+      </c>
+      <c r="S23" t="s">
+        <v>268</v>
+      </c>
+      <c r="T23">
+        <v>4</v>
+      </c>
+      <c r="U23" t="s">
+        <v>269</v>
+      </c>
+      <c r="V23" t="s">
+        <v>270</v>
+      </c>
+      <c r="W23" t="s">
+        <v>271</v>
+      </c>
+      <c r="X23" t="s">
+        <v>272</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>267</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>273</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>274</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>275</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>129</v>
+      </c>
+      <c r="AE23">
+        <v>97112</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>276</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>277</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL23" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN23" t="s">
+        <v>278</v>
+      </c>
+      <c r="AO23" t="s">
+        <v>279</v>
+      </c>
+      <c r="AP23" t="s">
+        <v>279</v>
+      </c>
+      <c r="AQ23" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR23" t="s">
+        <v>279</v>
+      </c>
+      <c r="AS23">
+        <v>0</v>
+      </c>
+      <c r="AT23">
+        <v>0</v>
+      </c>
+      <c r="AU23">
+        <v>0</v>
+      </c>
+      <c r="AV23">
+        <v>220</v>
+      </c>
+      <c r="AW23">
+        <v>2000</v>
+      </c>
+      <c r="AX23" t="s">
+        <v>329</v>
+      </c>
+      <c r="AY23" t="s">
+        <v>85</v>
+      </c>
+      <c r="AZ23" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA23" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB23" t="s">
+        <v>330</v>
+      </c>
+      <c r="BD23">
+        <v>790</v>
+      </c>
+      <c r="BE23" t="s">
+        <v>331</v>
+      </c>
+      <c r="BF23" t="s">
+        <v>155</v>
+      </c>
+      <c r="BG23" t="s">
+        <v>332</v>
+      </c>
+      <c r="BH23" t="s">
+        <v>314</v>
+      </c>
+      <c r="BJ23">
+        <v>600</v>
+      </c>
+      <c r="BK23">
+        <v>0</v>
+      </c>
+      <c r="BL23" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM23" t="s">
+        <v>333</v>
+      </c>
+      <c r="BN23" t="s">
+        <v>334</v>
+      </c>
+      <c r="BO23" t="s">
+        <v>335</v>
+      </c>
+      <c r="BP23" t="s">
+        <v>336</v>
+      </c>
+      <c r="BQ23" t="s">
+        <v>337</v>
+      </c>
+      <c r="BR23" t="s">
+        <v>338</v>
+      </c>
+      <c r="BS23" t="s">
+        <v>355</v>
+      </c>
+      <c r="BT23" t="s">
+        <v>355</v>
+      </c>
+      <c r="BU23" t="s">
+        <v>355</v>
+      </c>
+      <c r="BV23" t="s">
+        <v>355</v>
+      </c>
+      <c r="BW23" t="s">
+        <v>355</v>
+      </c>
+      <c r="BX23" t="s">
+        <v>355</v>
+      </c>
+      <c r="BY23" t="s">
+        <v>355</v>
+      </c>
+      <c r="BZ23" t="s">
+        <v>355</v>
+      </c>
+      <c r="CB23" t="s">
+        <v>362</v>
+      </c>
+      <c r="CD23" t="s">
+        <v>362</v>
+      </c>
+      <c r="CF23" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="24" spans="1:84">
+      <c r="AN24" t="s">
+        <v>280</v>
+      </c>
+      <c r="AO24" t="s">
+        <v>279</v>
+      </c>
+      <c r="AP24" t="s">
+        <v>279</v>
+      </c>
+      <c r="AR24" t="s">
+        <v>279</v>
+      </c>
+      <c r="AS24">
+        <v>0</v>
+      </c>
+      <c r="AT24">
+        <v>0</v>
+      </c>
+      <c r="AU24">
+        <v>0</v>
+      </c>
+      <c r="AV24">
+        <v>0</v>
+      </c>
+      <c r="AW24">
+        <v>0</v>
+      </c>
+      <c r="AX24" t="s">
+        <v>339</v>
+      </c>
+      <c r="AY24" t="s">
+        <v>85</v>
+      </c>
+      <c r="AZ24" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA24" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB24" t="s">
+        <v>330</v>
+      </c>
+      <c r="BD24" t="s">
+        <v>339</v>
+      </c>
+      <c r="BE24" t="s">
+        <v>339</v>
+      </c>
+      <c r="BF24" t="s">
+        <v>155</v>
+      </c>
+      <c r="BG24" t="s">
+        <v>339</v>
+      </c>
+      <c r="BH24" t="s">
+        <v>340</v>
+      </c>
+      <c r="BJ24">
+        <v>257</v>
+      </c>
+      <c r="BK24">
+        <v>0</v>
+      </c>
+      <c r="BL24" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM24" t="s">
+        <v>341</v>
+      </c>
+      <c r="BN24" t="s">
+        <v>342</v>
+      </c>
+      <c r="BO24" t="s">
+        <v>343</v>
+      </c>
+      <c r="BP24" t="s">
+        <v>339</v>
+      </c>
+      <c r="BQ24" t="s">
+        <v>337</v>
+      </c>
+      <c r="BS24" t="s">
+        <v>355</v>
+      </c>
+      <c r="BT24" t="s">
+        <v>355</v>
+      </c>
+      <c r="BU24" t="s">
+        <v>355</v>
+      </c>
+      <c r="BV24" t="s">
+        <v>355</v>
+      </c>
+      <c r="BW24" t="s">
+        <v>355</v>
+      </c>
+      <c r="BX24" t="s">
+        <v>355</v>
+      </c>
+      <c r="BZ24" t="s">
+        <v>355</v>
+      </c>
+      <c r="CB24" t="s">
+        <v>362</v>
+      </c>
+      <c r="CD24" t="s">
+        <v>362</v>
+      </c>
+      <c r="CF24" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="25" spans="1:84">
+      <c r="AN25" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO25" t="s">
+        <v>279</v>
+      </c>
+      <c r="AP25" t="s">
+        <v>279</v>
+      </c>
+      <c r="AQ25" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR25" t="s">
+        <v>279</v>
+      </c>
+      <c r="AS25">
+        <v>0</v>
+      </c>
+      <c r="AT25">
+        <v>0</v>
+      </c>
+      <c r="AU25">
+        <v>0</v>
+      </c>
+      <c r="AV25">
+        <v>0</v>
+      </c>
+      <c r="AW25">
+        <v>0</v>
+      </c>
+      <c r="AX25" t="s">
+        <v>344</v>
+      </c>
+      <c r="AZ25" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA25" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB25" t="s">
+        <v>330</v>
+      </c>
+      <c r="BD25">
+        <v>640</v>
+      </c>
+      <c r="BE25" t="s">
+        <v>345</v>
+      </c>
+      <c r="BF25" t="s">
+        <v>155</v>
+      </c>
+      <c r="BG25" t="s">
+        <v>339</v>
+      </c>
+      <c r="BH25" t="s">
+        <v>314</v>
+      </c>
+      <c r="BJ25">
+        <v>60</v>
+      </c>
+      <c r="BK25">
+        <v>0</v>
+      </c>
+      <c r="BL25" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM25" t="s">
+        <v>346</v>
+      </c>
+      <c r="BN25" t="s">
+        <v>347</v>
+      </c>
+      <c r="BO25" t="s">
+        <v>348</v>
+      </c>
+      <c r="BP25" t="s">
+        <v>339</v>
+      </c>
+      <c r="BQ25" t="s">
+        <v>337</v>
+      </c>
+      <c r="BR25" t="s">
+        <v>349</v>
+      </c>
+      <c r="BS25" t="s">
+        <v>355</v>
+      </c>
+      <c r="BT25" t="s">
+        <v>355</v>
+      </c>
+      <c r="BU25" t="s">
+        <v>355</v>
+      </c>
+      <c r="BV25" t="s">
+        <v>355</v>
+      </c>
+      <c r="BW25" t="s">
+        <v>355</v>
+      </c>
+      <c r="BX25" t="s">
+        <v>355</v>
+      </c>
+      <c r="BY25" t="s">
+        <v>355</v>
+      </c>
+      <c r="BZ25" t="s">
+        <v>355</v>
+      </c>
+      <c r="CB25" t="s">
+        <v>362</v>
+      </c>
+      <c r="CD25" t="s">
+        <v>362</v>
+      </c>
+      <c r="CF25" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="26" spans="1:84">
+      <c r="AN26" t="s">
+        <v>282</v>
+      </c>
+      <c r="AO26" t="s">
+        <v>279</v>
+      </c>
+      <c r="AP26" t="s">
+        <v>279</v>
+      </c>
+      <c r="AQ26" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR26" t="s">
+        <v>279</v>
+      </c>
+      <c r="AS26">
+        <v>0</v>
+      </c>
+      <c r="AT26">
+        <v>0</v>
+      </c>
+      <c r="AU26">
+        <v>0</v>
+      </c>
+      <c r="AV26">
+        <v>0</v>
+      </c>
+      <c r="AW26">
+        <v>0</v>
+      </c>
+      <c r="AX26" t="s">
+        <v>350</v>
+      </c>
+      <c r="AZ26" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA26" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB26" t="s">
+        <v>330</v>
+      </c>
+      <c r="BD26">
+        <v>640</v>
+      </c>
+      <c r="BE26" t="s">
+        <v>351</v>
+      </c>
+      <c r="BF26" t="s">
+        <v>155</v>
+      </c>
+      <c r="BG26" t="s">
+        <v>339</v>
+      </c>
+      <c r="BH26" t="s">
+        <v>314</v>
+      </c>
+      <c r="BJ26">
+        <v>250</v>
+      </c>
+      <c r="BK26">
+        <v>0</v>
+      </c>
+      <c r="BL26" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM26" t="s">
+        <v>352</v>
+      </c>
+      <c r="BN26">
+        <v>0</v>
+      </c>
+      <c r="BO26" t="s">
+        <v>353</v>
+      </c>
+      <c r="BP26" t="s">
+        <v>339</v>
+      </c>
+      <c r="BQ26" t="s">
+        <v>337</v>
+      </c>
+      <c r="BR26" t="s">
+        <v>354</v>
+      </c>
+      <c r="BS26" t="s">
+        <v>355</v>
+      </c>
+      <c r="BT26" t="s">
+        <v>355</v>
+      </c>
+      <c r="BU26" t="s">
+        <v>355</v>
+      </c>
+      <c r="BV26" t="s">
+        <v>355</v>
+      </c>
+      <c r="BW26" t="s">
+        <v>355</v>
+      </c>
+      <c r="BX26" t="s">
+        <v>355</v>
+      </c>
+      <c r="BY26" t="s">
+        <v>355</v>
+      </c>
+      <c r="BZ26" t="s">
+        <v>355</v>
+      </c>
+      <c r="CA26" t="s">
+        <v>355</v>
+      </c>
+      <c r="CB26" t="s">
+        <v>362</v>
+      </c>
+      <c r="CD26" t="s">
+        <v>362</v>
+      </c>
+      <c r="CF26" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="U10" r:id="rId1"/>
+    <hyperlink ref="U18" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Made the loop data bold again
</commit_message>
<xml_diff>
--- a/Anand_Work/FallWork2018/OUTPUT.xlsx
+++ b/Anand_Work/FallWork2018/OUTPUT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="363">
   <si>
     <t>Start Date</t>
   </si>
@@ -151,18 +151,18 @@
     <t>What is the percentage of â€˜awakeâ€™ time that youth spend engaged in instruction? (Instructional Activities: structured or unstructured activities with explicit learning objectives) - 1 - % of time</t>
   </si>
   <si>
-    <t>What is the percentage of â€˜awakeâ€™ time that youth spend engaged in other activities?
+    <t>What is the percentage of â€˜awakeâ€™ time that youth spend engaged in other activities?_x000D_
 (Other Activities: structured time without explicit learning objectives) - 1 - % of time</t>
   </si>
   <si>
-    <t>What is the percentage of â€˜awakeâ€™ time that youth spend engaged in free-time?
+    <t>What is the percentage of â€˜awakeâ€™ time that youth spend engaged in free-time?_x000D_
 (Free activities: unstructured time without explicit learning objectives) - 1 - % of time</t>
   </si>
   <si>
     <t>1 - How many 5th/6th grade students attended your outdoor school program last school year?</t>
   </si>
   <si>
-    <t>1 - How many 5th/6th grade students do you expect to attend your outdoor school program this
+    <t>1 - How many 5th/6th grade students do you expect to attend your outdoor school program this_x000D_
 current/upcoming school year?</t>
   </si>
   <si>
@@ -226,47 +226,47 @@
     <t>1 - What are the biggest unmet facility and material needs for your outdoor school?</t>
   </si>
   <si>
-    <t>1 - Is there any additional information that you would like to provide regarding facilities and 
+    <t>1 - Is there any additional information that you would like to provide regarding facilities and _x000D_
 materials?</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - adult volunteers</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - parents</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - college volunteers</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - school teachers</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - school administration</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - high school volunteers</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - trained staff</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - natural resource professionals</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - other</t>
   </si>
   <si>
-    <t>Please indicate who provides instruction to students while at outdoor school:
+    <t>Please indicate who provides instruction to students while at outdoor school:_x000D_
  (Instruction: structured or unstructured activities with explicit learning objectives) - 1 - other - Text</t>
   </si>
   <si>
@@ -360,7 +360,7 @@
     <t>afreeberg@campfireclolumbia.org</t>
   </si>
   <si>
-    <t>1411 SW Morrison St #300
+    <t>1411 SW Morrison St #300_x000D_
 Portland, O 97205</t>
   </si>
   <si>
@@ -409,7 +409,7 @@
     <t>matt@wholeearthschool.com</t>
   </si>
   <si>
-    <t>150 Shelton McMurphy Blvd Suite 206
+    <t>150 Shelton McMurphy Blvd Suite 206_x000D_
 Eugene, OR 97401</t>
   </si>
   <si>
@@ -530,7 +530,7 @@
     <t>Young</t>
   </si>
   <si>
-    <t>37028 Shoreview Dr.
+    <t>37028 Shoreview Dr._x000D_
 Dorena, OR 97434</t>
   </si>
   <si>
@@ -648,7 +648,7 @@
     <t>Kauffman</t>
   </si>
   <si>
-    <t>22455 Finn Road
+    <t>22455 Finn Road_x000D_
 Sheridan, OR 97378</t>
   </si>
   <si>
@@ -664,6 +664,227 @@
     <t>varies</t>
   </si>
   <si>
+    <t>66.228.26.105</t>
+  </si>
+  <si>
+    <t>R_1ovtwrJr01IjYRu</t>
+  </si>
+  <si>
+    <t>office@campmorrow.org</t>
+  </si>
+  <si>
+    <t>Camp Morrow</t>
+  </si>
+  <si>
+    <t>www.campmorrow.org</t>
+  </si>
+  <si>
+    <t>541-544-2971</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>Birman</t>
+  </si>
+  <si>
+    <t>jason@campmorrow.org</t>
+  </si>
+  <si>
+    <t>79551 Morrow Rd. Wamic, OR 97063</t>
+  </si>
+  <si>
+    <t>September-May (traditional school year calendar)</t>
+  </si>
+  <si>
+    <t>Camp Morrow Lake Camp</t>
+  </si>
+  <si>
+    <t>Currently we have one school that comes and does there own programming/teaching.  They come for 3 days, but we could go up to 5 days.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The current school stays 2 nights, but we can accommodate up to 4 nights.  </t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>72.173.163.86</t>
+  </si>
+  <si>
+    <t>R_DiQdJ5rTP5VjUwF</t>
+  </si>
+  <si>
+    <t>fortin@awsp.org</t>
+  </si>
+  <si>
+    <t>Assocaition of Washington School Principals Learning Centers</t>
+  </si>
+  <si>
+    <t>http://www.awsplearningcenters.org/</t>
+  </si>
+  <si>
+    <t>360-497-7131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin </t>
+  </si>
+  <si>
+    <t>Fortin</t>
+  </si>
+  <si>
+    <t>2142 Cispus Rd _x000D_
+Randle WA 98377</t>
+  </si>
+  <si>
+    <t>Cispus Learning Center</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>We provide the facilities, schools bring their program</t>
+  </si>
+  <si>
+    <t>Chwelah Peak Learning Center</t>
+  </si>
+  <si>
+    <t>We ptrovide the facilty, the schools bring the program</t>
+  </si>
+  <si>
+    <t>73.96.218.63</t>
+  </si>
+  <si>
+    <t>R_Tpcop4aL1x25mXD</t>
+  </si>
+  <si>
+    <t>camp@taloali.org</t>
+  </si>
+  <si>
+    <t>Camp Taloali</t>
+  </si>
+  <si>
+    <t>www.taloali.org</t>
+  </si>
+  <si>
+    <t>503-400-6437</t>
+  </si>
+  <si>
+    <t>Janet</t>
+  </si>
+  <si>
+    <t>Johanson</t>
+  </si>
+  <si>
+    <t>PO Box 32 Stayton, OR 97383</t>
+  </si>
+  <si>
+    <t>School Year</t>
+  </si>
+  <si>
+    <t>Stayton</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>Marion</t>
+  </si>
+  <si>
+    <t>Stayton, Oregon</t>
+  </si>
+  <si>
+    <t>76.2.16.81</t>
+  </si>
+  <si>
+    <t>R_3kukFuaEHldBjUj</t>
+  </si>
+  <si>
+    <t>Erynne@cascademountainschool.org</t>
+  </si>
+  <si>
+    <t>Mt. Adams Institute's Cascade Mountain School</t>
+  </si>
+  <si>
+    <t>www.cascademountainschool.org &amp; www.mtadamsinstitute.org</t>
+  </si>
+  <si>
+    <t>541-740-9951</t>
+  </si>
+  <si>
+    <t>Erynne</t>
+  </si>
+  <si>
+    <t>VanZee</t>
+  </si>
+  <si>
+    <t>erynne@cascademountainschool.org</t>
+  </si>
+  <si>
+    <t>2453 Highway 141, Trout Lake, Washington 98650</t>
+  </si>
+  <si>
+    <t>April to October</t>
+  </si>
+  <si>
+    <t>Full service outdoor school (both facility and provider)</t>
+  </si>
+  <si>
+    <t>50.76.96.250</t>
+  </si>
+  <si>
+    <t>R_1OHPeQk238fuNz3</t>
+  </si>
+  <si>
+    <t>bo.henderson@scouting.org</t>
+  </si>
+  <si>
+    <t>Cascade Pacific Council, BSA</t>
+  </si>
+  <si>
+    <t>www.cpcbsa.org</t>
+  </si>
+  <si>
+    <t>503-225-5744</t>
+  </si>
+  <si>
+    <t>Bo</t>
+  </si>
+  <si>
+    <t>Henderson</t>
+  </si>
+  <si>
+    <t>2145 SW Naito Pkwy_x000D_
+Portland, OR 97201</t>
+  </si>
+  <si>
+    <t>September 1 - May 31</t>
+  </si>
+  <si>
+    <t>Cloverdale</t>
+  </si>
+  <si>
+    <t>Tillamook</t>
+  </si>
+  <si>
+    <t>Pacific City</t>
+  </si>
+  <si>
+    <t>Camp Meriwether</t>
+  </si>
+  <si>
+    <t>set by provider</t>
+  </si>
+  <si>
+    <t>Camp Clark</t>
+  </si>
+  <si>
+    <t>Camp Baldwin</t>
+  </si>
+  <si>
+    <t>Butte Creek Scout Ranch</t>
+  </si>
+  <si>
     <t>We have an emergency action plan written up. Speed dial set to 911, AED system for facility, walker talkies on staff leaders.</t>
   </si>
   <si>
@@ -722,14 +943,203 @@
   </si>
   <si>
     <t xml:space="preserve">Yes, we have two main floor rooms available in the lodge that are accessible and the Alsea cabin is also accessible. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">80 acres </t>
+  </si>
+  <si>
+    <t xml:space="preserve">creek, lake, high desert climate, forest (mostly pine and oak trees).  </t>
+  </si>
+  <si>
+    <t>Schools have the option of us providing food service or they can provide food service.</t>
+  </si>
+  <si>
+    <t>Yes (if yes, please check all that apply),Gluten/wheat allergies,Dairy allergies (milk and/or egg),Soy, peanut, or tree nut allergies,Seafood or shellfish allergies</t>
+  </si>
+  <si>
+    <t>150 in a multi purpose room.  Audio/visual and chairs provided.  A/C and heated building. There is also a small heated room for smaller group of 15.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150  Mostly bunk-bed style housing in heated cabins.  There are a few queen beds.   Bathrooms are located in separate buildings. </t>
+  </si>
+  <si>
+    <t>We have areas that tents can be set up and we have RV sites (both full hook ups and partial hook ups).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most of our facility is wheelchair accessible.  There would only be a few cabins not accessible. </t>
+  </si>
+  <si>
+    <t>WE have mobile radios that are tied to the local Fire Department/EMT</t>
+  </si>
+  <si>
+    <t>Paved road,Extra large vehicle (Such semi-tuck with trailer, standard bus, class A RV)</t>
+  </si>
+  <si>
+    <t>Forst, creek, river, pond</t>
+  </si>
+  <si>
+    <t>Yes (if yes, please check all that apply),Vegetarian,Vegan,Kosher,Hallal,Diabetic Meal plan,Gluten/wheat allergies,Dairy allergies (milk and/or egg),Soy, peanut, or tree nut allergies,Seafood or shellfish allergies</t>
+  </si>
+  <si>
+    <t>20 rooms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">364 Bunk bed in dorms </t>
+  </si>
+  <si>
+    <t>350 in tents of the group brings them</t>
+  </si>
+  <si>
+    <t>yes, wheelchair ramps, accesible rest rooms and showers</t>
+  </si>
+  <si>
+    <t>More private type rooms for adults</t>
+  </si>
+  <si>
+    <t>We have a huge challenge course- 45+ low events, plus 6 high elements.</t>
+  </si>
+  <si>
+    <t>Land lines and cell service to call for help</t>
+  </si>
+  <si>
+    <t>Gravel/dirt road,Extra large vehicle (Such semi-tuck with trailer, standard bus, class A RV)</t>
+  </si>
+  <si>
+    <t>20 acres</t>
+  </si>
+  <si>
+    <t>Forest, creek, logged area</t>
+  </si>
+  <si>
+    <t>200 if schools bring tents</t>
+  </si>
+  <si>
+    <t>yes, wheelchair ramps, accessible showers and toliets</t>
+  </si>
+  <si>
+    <t>more beds needed</t>
+  </si>
+  <si>
+    <t>we have an artificial stream to teach panning techniques</t>
+  </si>
+  <si>
+    <t>VHF radio system with repeater</t>
+  </si>
+  <si>
+    <t>Gravel/dirt road,Extra large vehicle (Such semi-tuck with trailer, standard bus, class A RV),Large vehicles (such as semi without trailer, short bus length, Class C RV, truck with trailer),Standard vehicle (Such as truck without trailer, SUV, sedan),Small vehicle (Such as motorcycle, hybrid, smart car),Horse/Pack animal</t>
+  </si>
+  <si>
+    <t>several coastal biomes, tide pools, 2.5 miles of Pacific Ocean exclusive beach access, cape lookout and several salmon streams</t>
+  </si>
+  <si>
+    <t>Food Service is available.  We can provide or district can provide</t>
+  </si>
+  <si>
+    <t>9/600</t>
+  </si>
+  <si>
+    <t>Currently 96 housed in 6 duplex cabins that can accommodate 8 persons per side._x000D_
+  We are however running a capital campaign to expand this offering by an additional 192 persons in similarly sized cabins.  Expected completion in 2020.</t>
+  </si>
+  <si>
+    <t>542 housed in 3 walled structures with custom canvas doors, lighting and heat.  These structures sleep 6 and are grouped together in units of 5-7.</t>
+  </si>
+  <si>
+    <t>Various locations at the facility can be used by folks with assessiblity needs.  To fully accomodate everyone, dialogue would need to occur with the provider so we can be sure to fully understand the needs of specific individuals and work to accommodate them on a case by case basis..</t>
+  </si>
+  <si>
+    <t>Indoor Housing</t>
+  </si>
+  <si>
+    <t>Currently OMSI is using this facility as an additional location to their Newport Facility for Outdoor School beginning Spring of 2019.</t>
+  </si>
+  <si>
+    <t>same as Facility 1</t>
+  </si>
+  <si>
+    <t>Yes (if yes, please check all that apply),Vegetarian,Vegan,Kosher,Hallal,Gluten/wheat allergies,Dairy allergies (milk and/or egg),Soy, peanut, or tree nut allergies,Seafood or shellfish allergies</t>
+  </si>
+  <si>
+    <t>1 / 257</t>
+  </si>
+  <si>
+    <t>capacity of 44 in 9 rustic cabins and 2 recently constructed cabins.</t>
+  </si>
+  <si>
+    <t>250 capacity in small two person structures with canvas doors grouped in units of 12-16</t>
+  </si>
+  <si>
+    <t>UHF Radio System</t>
+  </si>
+  <si>
+    <t>Timberline bordering Eastern Oregon Savanna, shaded creeks and marsh</t>
+  </si>
+  <si>
+    <t>4/100</t>
+  </si>
+  <si>
+    <t>68 in 9 cabins constructed in 2015.  each cabin is one room that houses 8.  Cabins are heated, have electricity and insulated.</t>
+  </si>
+  <si>
+    <t>0 unless groups wanted to bring tents then closer to 350</t>
+  </si>
+  <si>
+    <t>Indoor housing and eating capacity are to double within the next 3 years.</t>
+  </si>
+  <si>
+    <t>UHF Radios</t>
+  </si>
+  <si>
+    <t>This facility is a working ranch.  property stadles Butte Creek (the border of Marion and Clackamas Counties</t>
+  </si>
+  <si>
+    <t>1/250  the Barn and Riding Arenas can be used as well</t>
+  </si>
+  <si>
+    <t>Same as Facility 2</t>
+  </si>
+  <si>
+    <t>We are working on designs for dormitory cabins to house around 256.  Facilities 1, 2, and 3 take priority.  A set construction date has not been determined.</t>
+  </si>
+  <si>
+    <t>Extremely Responsible</t>
+  </si>
+  <si>
+    <t>Somewhat responsible</t>
+  </si>
+  <si>
+    <t>Responsible</t>
+  </si>
+  <si>
+    <t>Not at all responsible</t>
+  </si>
+  <si>
+    <t>Forest service</t>
+  </si>
+  <si>
+    <t>Fish and wildlife</t>
+  </si>
+  <si>
+    <t>Other professionals</t>
+  </si>
+  <si>
+    <t>we are not the instructional providers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -763,14 +1173,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1066,7 +1477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CF16"/>
+  <dimension ref="A1:CF26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1462,26 +1873,110 @@
       </c>
     </row>
     <row r="5" spans="1:84">
-      <c r="AS5">
-        <v>0</v>
-      </c>
-      <c r="AT5">
-        <v>0</v>
-      </c>
-      <c r="AU5">
-        <v>0</v>
-      </c>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="1"/>
+      <c r="AR5" s="1"/>
+      <c r="AS5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="1"/>
+      <c r="AW5" s="1"/>
+      <c r="AX5" s="1"/>
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1"/>
+      <c r="BA5" s="1"/>
+      <c r="BB5" s="1"/>
+      <c r="BC5" s="1"/>
+      <c r="BD5" s="1"/>
+      <c r="BE5" s="1"/>
+      <c r="BF5" s="1"/>
+      <c r="BG5" s="1"/>
+      <c r="BH5" s="1"/>
+      <c r="BI5" s="1"/>
+      <c r="BJ5" s="1"/>
+      <c r="BK5" s="1"/>
+      <c r="BL5" s="1"/>
+      <c r="BM5" s="1"/>
+      <c r="BN5" s="1"/>
+      <c r="BO5" s="1"/>
+      <c r="BP5" s="1"/>
+      <c r="BQ5" s="1"/>
+      <c r="BR5" s="1"/>
+      <c r="BS5" s="1"/>
+      <c r="BT5" s="1"/>
+      <c r="BU5" s="1"/>
+      <c r="BV5" s="1"/>
+      <c r="BW5" s="1"/>
+      <c r="BX5" s="1"/>
+      <c r="BY5" s="1"/>
+      <c r="BZ5" s="1"/>
+      <c r="CA5" s="1"/>
+      <c r="CB5" s="1"/>
+      <c r="CC5" s="1"/>
+      <c r="CD5" s="1"/>
+      <c r="CE5" s="1"/>
+      <c r="CF5" s="1"/>
     </row>
     <row r="6" spans="1:84">
-      <c r="AS6">
-        <v>0</v>
-      </c>
-      <c r="AT6">
-        <v>0</v>
-      </c>
-      <c r="AU6">
-        <v>0</v>
-      </c>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
+      <c r="AQ6" s="1"/>
+      <c r="AR6" s="1"/>
+      <c r="AS6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="1"/>
+      <c r="AW6" s="1"/>
+      <c r="AX6" s="1"/>
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+      <c r="BA6" s="1"/>
+      <c r="BB6" s="1"/>
+      <c r="BC6" s="1"/>
+      <c r="BD6" s="1"/>
+      <c r="BE6" s="1"/>
+      <c r="BF6" s="1"/>
+      <c r="BG6" s="1"/>
+      <c r="BH6" s="1"/>
+      <c r="BI6" s="1"/>
+      <c r="BJ6" s="1"/>
+      <c r="BK6" s="1"/>
+      <c r="BL6" s="1"/>
+      <c r="BM6" s="1"/>
+      <c r="BN6" s="1"/>
+      <c r="BO6" s="1"/>
+      <c r="BP6" s="1"/>
+      <c r="BQ6" s="1"/>
+      <c r="BR6" s="1"/>
+      <c r="BS6" s="1"/>
+      <c r="BT6" s="1"/>
+      <c r="BU6" s="1"/>
+      <c r="BV6" s="1"/>
+      <c r="BW6" s="1"/>
+      <c r="BX6" s="1"/>
+      <c r="BY6" s="1"/>
+      <c r="BZ6" s="1"/>
+      <c r="CA6" s="1"/>
+      <c r="CB6" s="1"/>
+      <c r="CC6" s="1"/>
+      <c r="CD6" s="1"/>
+      <c r="CE6" s="1"/>
+      <c r="CF6" s="1"/>
     </row>
     <row r="8" spans="1:84">
       <c r="A8">
@@ -1704,7 +2199,7 @@
       <c r="S10" t="s">
         <v>120</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="U10" s="2" t="s">
         <v>121</v>
       </c>
       <c r="V10" t="s">
@@ -2038,7 +2533,7 @@
         <v>1700</v>
       </c>
       <c r="AX13" t="s">
-        <v>210</v>
+        <v>283</v>
       </c>
       <c r="AY13" t="s">
         <v>185</v>
@@ -2050,19 +2545,19 @@
         <v>85</v>
       </c>
       <c r="BB13" t="s">
-        <v>211</v>
+        <v>284</v>
       </c>
       <c r="BD13" t="s">
-        <v>212</v>
+        <v>285</v>
       </c>
       <c r="BE13" t="s">
-        <v>213</v>
+        <v>286</v>
       </c>
       <c r="BF13" t="s">
-        <v>214</v>
+        <v>287</v>
       </c>
       <c r="BH13" t="s">
-        <v>215</v>
+        <v>288</v>
       </c>
       <c r="BJ13">
         <v>240</v>
@@ -2071,7 +2566,7 @@
         <v>300</v>
       </c>
       <c r="BL13" t="s">
-        <v>216</v>
+        <v>289</v>
       </c>
       <c r="BM13">
         <v>5</v>
@@ -2083,13 +2578,52 @@
         <v>500</v>
       </c>
       <c r="BP13" t="s">
-        <v>217</v>
+        <v>290</v>
       </c>
       <c r="BQ13" t="s">
-        <v>218</v>
+        <v>291</v>
       </c>
       <c r="BR13" t="s">
-        <v>219</v>
+        <v>292</v>
+      </c>
+      <c r="BS13" t="s">
+        <v>355</v>
+      </c>
+      <c r="BT13" t="s">
+        <v>356</v>
+      </c>
+      <c r="BU13" t="s">
+        <v>355</v>
+      </c>
+      <c r="BV13" t="s">
+        <v>357</v>
+      </c>
+      <c r="BW13" t="s">
+        <v>358</v>
+      </c>
+      <c r="BX13" t="s">
+        <v>358</v>
+      </c>
+      <c r="BY13" t="s">
+        <v>357</v>
+      </c>
+      <c r="CA13" t="s">
+        <v>355</v>
+      </c>
+      <c r="CB13" t="s">
+        <v>359</v>
+      </c>
+      <c r="CC13" t="s">
+        <v>355</v>
+      </c>
+      <c r="CD13" t="s">
+        <v>360</v>
+      </c>
+      <c r="CE13" t="s">
+        <v>355</v>
+      </c>
+      <c r="CF13" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="14" spans="1:84">
@@ -2383,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="AX16" t="s">
-        <v>220</v>
+        <v>293</v>
       </c>
       <c r="AY16" t="s">
         <v>185</v>
@@ -2395,45 +2929,1289 @@
         <v>185</v>
       </c>
       <c r="BB16" t="s">
-        <v>221</v>
+        <v>294</v>
       </c>
       <c r="BD16" t="s">
-        <v>222</v>
+        <v>295</v>
       </c>
       <c r="BE16" t="s">
-        <v>223</v>
+        <v>296</v>
       </c>
       <c r="BF16" t="s">
         <v>155</v>
       </c>
       <c r="BG16" t="s">
-        <v>224</v>
+        <v>297</v>
       </c>
       <c r="BH16" t="s">
-        <v>225</v>
+        <v>298</v>
       </c>
       <c r="BJ16">
         <v>150</v>
       </c>
       <c r="BK16" t="s">
+        <v>299</v>
+      </c>
+      <c r="BL16" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM16" t="s">
+        <v>300</v>
+      </c>
+      <c r="BN16" t="s">
+        <v>301</v>
+      </c>
+      <c r="BP16" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:84">
+      <c r="A17">
+        <v>43382.4278125</v>
+      </c>
+      <c r="B17">
+        <v>43382.45159722222</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>210</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="F17">
+        <v>2055</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>43382.4516087963</v>
+      </c>
+      <c r="I17" t="s">
+        <v>211</v>
+      </c>
+      <c r="N17">
+        <v>45.222900390625</v>
+      </c>
+      <c r="O17">
+        <v>-121.292701721191</v>
+      </c>
+      <c r="P17" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>83</v>
+      </c>
+      <c r="R17" t="s">
+        <v>212</v>
+      </c>
+      <c r="S17" t="s">
+        <v>213</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17" t="s">
+        <v>214</v>
+      </c>
+      <c r="V17" t="s">
+        <v>215</v>
+      </c>
+      <c r="W17" t="s">
+        <v>216</v>
+      </c>
+      <c r="X17" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>218</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>220</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>221</v>
+      </c>
+      <c r="AO17" t="s">
+        <v>222</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>223</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>224</v>
+      </c>
+      <c r="AS17">
+        <v>0</v>
+      </c>
+      <c r="AT17">
+        <v>0</v>
+      </c>
+      <c r="AU17">
+        <v>0</v>
+      </c>
+      <c r="AV17">
+        <v>20</v>
+      </c>
+      <c r="AW17">
+        <v>20</v>
+      </c>
+      <c r="AY17" t="s">
+        <v>85</v>
+      </c>
+      <c r="AZ17" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA17" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB17" t="s">
+        <v>294</v>
+      </c>
+      <c r="BD17" t="s">
+        <v>303</v>
+      </c>
+      <c r="BE17" t="s">
+        <v>304</v>
+      </c>
+      <c r="BF17" t="s">
+        <v>155</v>
+      </c>
+      <c r="BG17" t="s">
+        <v>305</v>
+      </c>
+      <c r="BH17" t="s">
+        <v>306</v>
+      </c>
+      <c r="BJ17">
+        <v>150</v>
+      </c>
+      <c r="BK17">
+        <v>50</v>
+      </c>
+      <c r="BL17" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM17" t="s">
+        <v>307</v>
+      </c>
+      <c r="BN17" t="s">
+        <v>308</v>
+      </c>
+      <c r="BO17" t="s">
+        <v>309</v>
+      </c>
+      <c r="BP17" t="s">
+        <v>310</v>
+      </c>
+      <c r="BS17" t="s">
+        <v>355</v>
+      </c>
+      <c r="BT17" t="s">
+        <v>355</v>
+      </c>
+      <c r="BV17" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="18" spans="1:84">
+      <c r="A18">
+        <v>43382.50405092593</v>
+      </c>
+      <c r="B18">
+        <v>43382.5228125</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>225</v>
+      </c>
+      <c r="E18">
+        <v>100</v>
+      </c>
+      <c r="F18">
+        <v>1621</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>43382.52282407408</v>
+      </c>
+      <c r="I18" t="s">
         <v>226</v>
       </c>
-      <c r="BL16" t="s">
-        <v>216</v>
-      </c>
-      <c r="BM16" t="s">
+      <c r="N18">
+        <v>46.5491943359375</v>
+      </c>
+      <c r="O18">
+        <v>-121.855499267578</v>
+      </c>
+      <c r="P18" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>83</v>
+      </c>
+      <c r="R18" t="s">
         <v>227</v>
       </c>
-      <c r="BN16" t="s">
+      <c r="S18" t="s">
         <v>228</v>
       </c>
-      <c r="BP16" t="s">
+      <c r="T18">
+        <v>2</v>
+      </c>
+      <c r="U18" s="2" t="s">
         <v>229</v>
+      </c>
+      <c r="V18" t="s">
+        <v>230</v>
+      </c>
+      <c r="W18" t="s">
+        <v>231</v>
+      </c>
+      <c r="X18" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>233</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>167</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN18" t="s">
+        <v>234</v>
+      </c>
+      <c r="AO18" t="s">
+        <v>235</v>
+      </c>
+      <c r="AP18" t="s">
+        <v>235</v>
+      </c>
+      <c r="AQ18" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>236</v>
+      </c>
+      <c r="AS18">
+        <v>0</v>
+      </c>
+      <c r="AT18">
+        <v>0</v>
+      </c>
+      <c r="AU18">
+        <v>0</v>
+      </c>
+      <c r="AV18">
+        <v>2900</v>
+      </c>
+      <c r="AW18">
+        <v>2900</v>
+      </c>
+      <c r="AX18" t="s">
+        <v>311</v>
+      </c>
+      <c r="AY18" t="s">
+        <v>185</v>
+      </c>
+      <c r="AZ18" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA18" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB18" t="s">
+        <v>312</v>
+      </c>
+      <c r="BD18">
+        <v>68</v>
+      </c>
+      <c r="BE18" t="s">
+        <v>313</v>
+      </c>
+      <c r="BF18" t="s">
+        <v>287</v>
+      </c>
+      <c r="BH18" t="s">
+        <v>314</v>
+      </c>
+      <c r="BJ18">
+        <v>350</v>
+      </c>
+      <c r="BK18">
+        <v>350</v>
+      </c>
+      <c r="BL18" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM18" t="s">
+        <v>315</v>
+      </c>
+      <c r="BN18" t="s">
+        <v>316</v>
+      </c>
+      <c r="BO18" t="s">
+        <v>317</v>
+      </c>
+      <c r="BP18" t="s">
+        <v>318</v>
+      </c>
+      <c r="BQ18" t="s">
+        <v>319</v>
+      </c>
+      <c r="BR18" t="s">
+        <v>320</v>
+      </c>
+      <c r="BS18" t="s">
+        <v>357</v>
+      </c>
+      <c r="BT18" t="s">
+        <v>357</v>
+      </c>
+      <c r="BV18" t="s">
+        <v>355</v>
+      </c>
+      <c r="BW18" t="s">
+        <v>356</v>
+      </c>
+      <c r="BX18" t="s">
+        <v>357</v>
+      </c>
+      <c r="BY18" t="s">
+        <v>358</v>
+      </c>
+      <c r="BZ18" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="19" spans="1:84">
+      <c r="AN19" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AO19" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="AP19" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="AQ19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR19" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="AS19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV19" s="1">
+        <v>693</v>
+      </c>
+      <c r="AW19" s="1">
+        <v>700</v>
+      </c>
+      <c r="AX19" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AY19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AZ19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB19" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="BC19" s="1"/>
+      <c r="BD19" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="BE19" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="BF19" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="BG19" s="1"/>
+      <c r="BH19" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="BI19" s="1"/>
+      <c r="BJ19" s="1">
+        <v>200</v>
+      </c>
+      <c r="BK19" s="1">
+        <v>200</v>
+      </c>
+      <c r="BL19" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM19" s="1">
+        <v>10</v>
+      </c>
+      <c r="BN19" s="1">
+        <v>196</v>
+      </c>
+      <c r="BO19" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="BP19" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="BQ19" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="BR19" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="BS19" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="BT19" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="BU19" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="BV19" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BW19" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="BX19" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="BY19" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="BZ19" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="CA19" s="1"/>
+      <c r="CB19" s="1"/>
+      <c r="CC19" s="1"/>
+      <c r="CD19" s="1"/>
+      <c r="CE19" s="1"/>
+      <c r="CF19" s="1"/>
+    </row>
+    <row r="21" spans="1:84">
+      <c r="A21">
+        <v>43382.63195601852</v>
+      </c>
+      <c r="B21">
+        <v>43382.63358796296</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>239</v>
+      </c>
+      <c r="E21">
+        <v>100</v>
+      </c>
+      <c r="F21">
+        <v>140</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>43382.63358796296</v>
+      </c>
+      <c r="I21" t="s">
+        <v>240</v>
+      </c>
+      <c r="N21">
+        <v>44.9490051269531</v>
+      </c>
+      <c r="O21">
+        <v>-123.003997802734</v>
+      </c>
+      <c r="P21" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>83</v>
+      </c>
+      <c r="R21" t="s">
+        <v>241</v>
+      </c>
+      <c r="S21" t="s">
+        <v>242</v>
+      </c>
+      <c r="U21" t="s">
+        <v>243</v>
+      </c>
+      <c r="V21" t="s">
+        <v>244</v>
+      </c>
+      <c r="W21" t="s">
+        <v>245</v>
+      </c>
+      <c r="X21" t="s">
+        <v>246</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>247</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>248</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>249</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>250</v>
+      </c>
+      <c r="AE21">
+        <v>97383</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>252</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:84">
+      <c r="A22">
+        <v>43383.43930555556</v>
+      </c>
+      <c r="B22">
+        <v>43383.45842592593</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>253</v>
+      </c>
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>1651</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>43383.45842592593</v>
+      </c>
+      <c r="I22" t="s">
+        <v>254</v>
+      </c>
+      <c r="N22">
+        <v>45.9828033447265</v>
+      </c>
+      <c r="O22">
+        <v>-121.516296386718</v>
+      </c>
+      <c r="P22" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>83</v>
+      </c>
+      <c r="R22" t="s">
+        <v>255</v>
+      </c>
+      <c r="S22" t="s">
+        <v>256</v>
+      </c>
+      <c r="U22" t="s">
+        <v>257</v>
+      </c>
+      <c r="V22" t="s">
+        <v>258</v>
+      </c>
+      <c r="W22" t="s">
+        <v>259</v>
+      </c>
+      <c r="X22" t="s">
+        <v>260</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>261</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>262</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>263</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:84">
+      <c r="A23">
+        <v>43383.49253472222</v>
+      </c>
+      <c r="B23">
+        <v>43383.52399305555</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>265</v>
+      </c>
+      <c r="E23">
+        <v>100</v>
+      </c>
+      <c r="F23">
+        <v>2717</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>43383.52400462963</v>
+      </c>
+      <c r="I23" t="s">
+        <v>266</v>
+      </c>
+      <c r="N23">
+        <v>45.5077972412109</v>
+      </c>
+      <c r="O23">
+        <v>-122.689697265625</v>
+      </c>
+      <c r="P23" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>83</v>
+      </c>
+      <c r="R23" t="s">
+        <v>267</v>
+      </c>
+      <c r="S23" t="s">
+        <v>268</v>
+      </c>
+      <c r="T23">
+        <v>4</v>
+      </c>
+      <c r="U23" t="s">
+        <v>269</v>
+      </c>
+      <c r="V23" t="s">
+        <v>270</v>
+      </c>
+      <c r="W23" t="s">
+        <v>271</v>
+      </c>
+      <c r="X23" t="s">
+        <v>272</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>267</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>273</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>274</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>275</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>129</v>
+      </c>
+      <c r="AE23">
+        <v>97112</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>276</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>277</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL23" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN23" t="s">
+        <v>278</v>
+      </c>
+      <c r="AO23" t="s">
+        <v>279</v>
+      </c>
+      <c r="AP23" t="s">
+        <v>279</v>
+      </c>
+      <c r="AQ23" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR23" t="s">
+        <v>279</v>
+      </c>
+      <c r="AS23">
+        <v>0</v>
+      </c>
+      <c r="AT23">
+        <v>0</v>
+      </c>
+      <c r="AU23">
+        <v>0</v>
+      </c>
+      <c r="AV23">
+        <v>220</v>
+      </c>
+      <c r="AW23">
+        <v>2000</v>
+      </c>
+      <c r="AX23" t="s">
+        <v>329</v>
+      </c>
+      <c r="AY23" t="s">
+        <v>85</v>
+      </c>
+      <c r="AZ23" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA23" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB23" t="s">
+        <v>330</v>
+      </c>
+      <c r="BD23">
+        <v>790</v>
+      </c>
+      <c r="BE23" t="s">
+        <v>331</v>
+      </c>
+      <c r="BF23" t="s">
+        <v>155</v>
+      </c>
+      <c r="BG23" t="s">
+        <v>332</v>
+      </c>
+      <c r="BH23" t="s">
+        <v>314</v>
+      </c>
+      <c r="BJ23">
+        <v>600</v>
+      </c>
+      <c r="BK23">
+        <v>0</v>
+      </c>
+      <c r="BL23" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM23" t="s">
+        <v>333</v>
+      </c>
+      <c r="BN23" t="s">
+        <v>334</v>
+      </c>
+      <c r="BO23" t="s">
+        <v>335</v>
+      </c>
+      <c r="BP23" t="s">
+        <v>336</v>
+      </c>
+      <c r="BQ23" t="s">
+        <v>337</v>
+      </c>
+      <c r="BR23" t="s">
+        <v>338</v>
+      </c>
+      <c r="BS23" t="s">
+        <v>355</v>
+      </c>
+      <c r="BT23" t="s">
+        <v>355</v>
+      </c>
+      <c r="BU23" t="s">
+        <v>355</v>
+      </c>
+      <c r="BV23" t="s">
+        <v>355</v>
+      </c>
+      <c r="BW23" t="s">
+        <v>355</v>
+      </c>
+      <c r="BX23" t="s">
+        <v>355</v>
+      </c>
+      <c r="BY23" t="s">
+        <v>355</v>
+      </c>
+      <c r="BZ23" t="s">
+        <v>355</v>
+      </c>
+      <c r="CB23" t="s">
+        <v>362</v>
+      </c>
+      <c r="CD23" t="s">
+        <v>362</v>
+      </c>
+      <c r="CF23" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="24" spans="1:84">
+      <c r="AN24" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="AO24" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="AP24" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="AQ24" s="1"/>
+      <c r="AR24" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="AS24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX24" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="AY24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AZ24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB24" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="BC24" s="1"/>
+      <c r="BD24" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="BE24" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="BF24" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="BG24" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="BH24" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="BI24" s="1"/>
+      <c r="BJ24" s="1">
+        <v>257</v>
+      </c>
+      <c r="BK24" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL24" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM24" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="BN24" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="BO24" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="BP24" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="BQ24" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="BR24" s="1"/>
+      <c r="BS24" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BT24" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BU24" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BV24" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BW24" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BX24" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BY24" s="1"/>
+      <c r="BZ24" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="CA24" s="1"/>
+      <c r="CB24" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="CC24" s="1"/>
+      <c r="CD24" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="CE24" s="1"/>
+      <c r="CF24" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="25" spans="1:84">
+      <c r="AN25" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="AO25" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="AP25" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="AQ25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR25" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="AS25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX25" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="AY25" s="1"/>
+      <c r="AZ25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB25" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="BC25" s="1"/>
+      <c r="BD25" s="1">
+        <v>640</v>
+      </c>
+      <c r="BE25" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="BF25" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="BG25" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="BH25" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="BI25" s="1"/>
+      <c r="BJ25" s="1">
+        <v>60</v>
+      </c>
+      <c r="BK25" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL25" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM25" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="BN25" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="BO25" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="BP25" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="BQ25" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="BR25" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="BS25" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BT25" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BU25" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BV25" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BW25" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BX25" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BY25" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BZ25" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="CA25" s="1"/>
+      <c r="CB25" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="CC25" s="1"/>
+      <c r="CD25" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="CE25" s="1"/>
+      <c r="CF25" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="26" spans="1:84">
+      <c r="AN26" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="AO26" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="AP26" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="AQ26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR26" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="AS26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX26" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="AY26" s="1"/>
+      <c r="AZ26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB26" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="BC26" s="1"/>
+      <c r="BD26" s="1">
+        <v>640</v>
+      </c>
+      <c r="BE26" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="BF26" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="BG26" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="BH26" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="BI26" s="1"/>
+      <c r="BJ26" s="1">
+        <v>250</v>
+      </c>
+      <c r="BK26" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL26" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="BM26" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="BN26" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO26" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="BP26" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="BQ26" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="BR26" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="BS26" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BT26" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BU26" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BV26" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BW26" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BX26" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BY26" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="BZ26" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="CA26" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="CB26" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="CC26" s="1"/>
+      <c r="CD26" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="CE26" s="1"/>
+      <c r="CF26" s="1" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="U10" r:id="rId1"/>
+    <hyperlink ref="U18" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Section 8 heading added
</commit_message>
<xml_diff>
--- a/Anand_Work/FallWork2018/OUTPUT.xlsx
+++ b/Anand_Work/FallWork2018/OUTPUT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="416">
   <si>
     <t>Start Date</t>
   </si>
@@ -313,6 +313,44 @@
   </si>
   <si>
     <t>1 - Closest Medical Provider: (Name of medical provider and city.  If possible provide an estimated distance and time to medical provider.)</t>
+  </si>
+  <si>
+    <t>Indicate your outdoor school programâ€™s status in implementing each of the accommodations and _x000D_
+modifications that may be used to promote Diversity, Equity and Inclusion. - 1 - Implementing a racial equity plan</t>
+  </si>
+  <si>
+    <t>Indicate your outdoor school programâ€™s status in implementing each of the accommodations and _x000D_
+modifications that may be used to promote Diversity, Equity and Inclusion. - 1 - Adopting a DEI lens</t>
+  </si>
+  <si>
+    <t>Indicate your outdoor school programâ€™s status in implementing each of the accommodations and _x000D_
+modifications that may be used to promote Diversity, Equity and Inclusion. - 1 - Translation of Materials</t>
+  </si>
+  <si>
+    <t>Indicate your outdoor school programâ€™s status in implementing each of the accommodations and _x000D_
+modifications that may be used to promote Diversity, Equity and Inclusion. - 1 - Interpretation Services</t>
+  </si>
+  <si>
+    <t>Indicate your outdoor school programâ€™s status in implementing each of the accommodations and _x000D_
+modifications that may be used to promote Diversity, Equity and Inclusion. - 1 - Informational Sessions/Open House Night</t>
+  </si>
+  <si>
+    <t>Indicate your outdoor school programâ€™s status in implementing each of the accommodations and _x000D_
+modifications that may be used to promote Diversity, Equity and Inclusion. - 1 - Allow Families to Attend</t>
+  </si>
+  <si>
+    <t>Indicate your outdoor school programâ€™s status in implementing each of the accommodations and _x000D_
+modifications that may be used to promote Diversity, Equity and Inclusion. - 1 - Accessibility/ADA</t>
+  </si>
+  <si>
+    <t>Indicate your outdoor school programâ€™s status in implementing each of the accommodations and _x000D_
+modifications that may be used to promote Diversity, Equity and Inclusion. - 1 - Mobility Supports</t>
+  </si>
+  <si>
+    <t>1 - What support(s) do you need to further promote DEI in your outdoor school?</t>
+  </si>
+  <si>
+    <t>1 - Is there additional information that you would like to provide regarding DEI?</t>
   </si>
   <si>
     <t>Survey Preview</t>
@@ -1606,13 +1644,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU26"/>
+  <dimension ref="A1:DE26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:99">
+    <row r="1" spans="1:109">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1910,8 +1948,38 @@
       <c r="CU1" t="s">
         <v>94</v>
       </c>
+      <c r="CV1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>99</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>100</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>101</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>102</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>103</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="2" spans="1:99">
+    <row r="2" spans="1:109">
       <c r="A2">
         <v>43378.46934027778</v>
       </c>
@@ -1919,7 +1987,7 @@
         <v>43378.47023148148</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -1934,7 +2002,7 @@
         <v>43378.47024305556</v>
       </c>
       <c r="I2" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="N2">
         <v>44.5641937255859</v>
@@ -1943,13 +2011,13 @@
         <v>-123.278999328613</v>
       </c>
       <c r="P2" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="Q2" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:99">
+    <row r="3" spans="1:109">
       <c r="A3">
         <v>43378.47028935186</v>
       </c>
@@ -1957,7 +2025,7 @@
         <v>43378.47060185186</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -1972,7 +2040,7 @@
         <v>43378.47060185186</v>
       </c>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="N3">
         <v>44.5641937255859</v>
@@ -1981,22 +2049,22 @@
         <v>-123.278999328613</v>
       </c>
       <c r="P3" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="Q3" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="AH3" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AJ3" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AL3" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:99">
+    <row r="4" spans="1:109">
       <c r="A4">
         <v>43380.91150462963</v>
       </c>
@@ -2004,7 +2072,7 @@
         <v>43380.91293981481</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -2019,7 +2087,7 @@
         <v>43380.91295138889</v>
       </c>
       <c r="I4" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="N4">
         <v>44.5637969970703</v>
@@ -2028,10 +2096,10 @@
         <v>-123.2779006958</v>
       </c>
       <c r="P4" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="Q4" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="T4">
         <v>3</v>
@@ -2046,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:99">
+    <row r="5" spans="1:109">
       <c r="AN5" s="1"/>
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
@@ -2114,7 +2182,7 @@
       <c r="CT5" s="1"/>
       <c r="CU5" s="1"/>
     </row>
-    <row r="6" spans="1:99">
+    <row r="6" spans="1:109">
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
       <c r="AP6" s="1"/>
@@ -2182,7 +2250,7 @@
       <c r="CT6" s="1"/>
       <c r="CU6" s="1"/>
     </row>
-    <row r="8" spans="1:99">
+    <row r="8" spans="1:109">
       <c r="A8">
         <v>43381.70964120371</v>
       </c>
@@ -2193,7 +2261,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="E8">
         <v>100</v>
@@ -2208,7 +2276,7 @@
         <v>43381.71163194445</v>
       </c>
       <c r="I8" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="N8">
         <v>40.7180023193359</v>
@@ -2217,52 +2285,52 @@
         <v>-74.0754013061523</v>
       </c>
       <c r="P8" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q8" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="R8" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="S8" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="U8" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="V8" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="W8" t="s">
+        <v>121</v>
+      </c>
+      <c r="X8" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>125</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AJ8" t="s">
         <v>111</v>
       </c>
-      <c r="X8" t="s">
+      <c r="AL8" t="s">
         <v>112</v>
       </c>
-      <c r="Y8" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>113</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>114</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>115</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>100</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>101</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>102</v>
-      </c>
     </row>
-    <row r="9" spans="1:99">
+    <row r="9" spans="1:109">
       <c r="A9">
         <v>43381.71248842592</v>
       </c>
@@ -2273,7 +2341,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -2288,7 +2356,7 @@
         <v>43381.715</v>
       </c>
       <c r="I9" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="N9">
         <v>45.5653076171875</v>
@@ -2297,67 +2365,67 @@
         <v>-122.644798278808</v>
       </c>
       <c r="P9" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q9" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="R9" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="S9" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="U9" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="V9" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="W9" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="X9" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="Y9" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="Z9" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="AA9" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="AB9" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="AC9" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="AD9" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="AE9">
         <v>97055</v>
       </c>
       <c r="AF9" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="AG9" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="AH9" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AJ9" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AL9" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:99">
+    <row r="10" spans="1:109">
       <c r="A10">
         <v>43381.71474537037</v>
       </c>
@@ -2368,7 +2436,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="E10">
         <v>100</v>
@@ -2383,7 +2451,7 @@
         <v>43381.71667824074</v>
       </c>
       <c r="I10" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="N10">
         <v>44.0682067871093</v>
@@ -2392,67 +2460,67 @@
         <v>-123.081901550292</v>
       </c>
       <c r="P10" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q10" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="R10" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="S10" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="U10" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="V10" t="s">
+        <v>147</v>
+      </c>
+      <c r="W10" t="s">
+        <v>148</v>
+      </c>
+      <c r="X10" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA10" t="s">
         <v>136</v>
       </c>
-      <c r="V10" t="s">
-        <v>137</v>
-      </c>
-      <c r="W10" t="s">
-        <v>138</v>
-      </c>
-      <c r="X10" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>126</v>
-      </c>
       <c r="AB10" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="AC10" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="AD10" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="AE10">
         <v>97419</v>
       </c>
       <c r="AF10" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="AG10" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="AH10" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AJ10" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AL10" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:99">
+    <row r="11" spans="1:109">
       <c r="A11">
         <v>43381.71635416667</v>
       </c>
@@ -2463,7 +2531,7 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="E11">
         <v>100</v>
@@ -2478,7 +2546,7 @@
         <v>43381.72159722223</v>
       </c>
       <c r="I11" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="N11">
         <v>45.3726959228515</v>
@@ -2487,64 +2555,64 @@
         <v>-122.76309967041</v>
       </c>
       <c r="P11" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q11" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="R11" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="S11" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="U11" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="V11" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="W11" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="X11" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Y11" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="AA11" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="AB11" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="AC11" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="AD11" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="AE11">
         <v>97064</v>
       </c>
       <c r="AF11" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="AG11" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="AH11" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AJ11" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AL11" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:99">
+    <row r="12" spans="1:109">
       <c r="A12">
         <v>43381.74771990741</v>
       </c>
@@ -2555,7 +2623,7 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="E12">
         <v>100</v>
@@ -2570,7 +2638,7 @@
         <v>43381.75016203704</v>
       </c>
       <c r="I12" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="N12">
         <v>45.3493957519531</v>
@@ -2579,55 +2647,55 @@
         <v>-117.212799072265</v>
       </c>
       <c r="P12" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q12" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="R12" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="S12" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="U12" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="V12" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="W12" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="X12" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="Y12" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="Z12" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="AA12" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="AB12" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="AH12" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="AI12" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="AJ12" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AL12" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:99">
+    <row r="13" spans="1:109">
       <c r="A13">
         <v>43381.7379050926</v>
       </c>
@@ -2638,7 +2706,7 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="E13">
         <v>100</v>
@@ -2653,7 +2721,7 @@
         <v>43381.75645833334</v>
       </c>
       <c r="I13" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="N13">
         <v>38.4797058105468</v>
@@ -2662,64 +2730,64 @@
         <v>-121.443801879882</v>
       </c>
       <c r="P13" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q13" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="R13" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="S13" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="T13">
         <v>1</v>
       </c>
       <c r="U13" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="V13" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="W13" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="X13" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="Y13" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="Z13" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="AA13" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="AB13" t="s">
+        <v>192</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>110</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL13" t="s">
         <v>182</v>
       </c>
-      <c r="AH13" t="s">
-        <v>100</v>
-      </c>
-      <c r="AJ13" t="s">
-        <v>101</v>
-      </c>
-      <c r="AL13" t="s">
-        <v>172</v>
-      </c>
       <c r="AN13" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="AO13" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="AP13" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="AQ13" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AS13">
         <v>40</v>
@@ -2737,31 +2805,31 @@
         <v>1700</v>
       </c>
       <c r="AX13" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="AY13" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="AZ13" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BA13" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BB13" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="BD13" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="BE13" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="BF13" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="BH13" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="BJ13">
         <v>240</v>
@@ -2770,7 +2838,7 @@
         <v>300</v>
       </c>
       <c r="BL13" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="BM13">
         <v>5</v>
@@ -2782,76 +2850,76 @@
         <v>500</v>
       </c>
       <c r="BP13" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="BQ13" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="BR13" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
       <c r="BS13" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BT13" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="BU13" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BV13" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="BW13" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="BX13" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="BY13" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="CA13" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="CB13" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="CC13" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="CD13" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="CE13" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="CF13" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
       <c r="CG13" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CH13" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CK13" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CL13" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CM13" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CN13" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
       <c r="CO13" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
     </row>
-    <row r="14" spans="1:99">
+    <row r="14" spans="1:109">
       <c r="A14">
         <v>43381.87571759259</v>
       </c>
@@ -2862,7 +2930,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="E14">
         <v>100</v>
@@ -2877,7 +2945,7 @@
         <v>43381.88489583333</v>
       </c>
       <c r="I14" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="N14">
         <v>45.5440979003906</v>
@@ -2886,67 +2954,67 @@
         <v>-122.642303466796</v>
       </c>
       <c r="P14" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q14" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="R14" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="S14" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="U14" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="V14" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="W14" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="X14" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="Y14" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="Z14" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="AA14" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="AB14" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="AC14" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="AD14" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="AE14">
         <v>98671</v>
       </c>
       <c r="AF14" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="AG14" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="AH14" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="AJ14" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AL14" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:99">
+    <row r="15" spans="1:109">
       <c r="A15">
         <v>43382.01947916667</v>
       </c>
@@ -2957,7 +3025,7 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="E15">
         <v>100</v>
@@ -2972,7 +3040,7 @@
         <v>43382.02648148148</v>
       </c>
       <c r="I15" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="N15">
         <v>48.465103149414</v>
@@ -2981,49 +3049,49 @@
         <v>7.95590209960937</v>
       </c>
       <c r="P15" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q15" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="R15" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="S15" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="U15" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="V15" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="W15" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="X15" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="Y15" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="Z15" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="AB15" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="AH15" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AJ15" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AL15" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:99">
+    <row r="16" spans="1:109">
       <c r="A16">
         <v>43382.42454861111</v>
       </c>
@@ -3034,7 +3102,7 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="E16">
         <v>100</v>
@@ -3049,7 +3117,7 @@
         <v>43382.44296296296</v>
       </c>
       <c r="I16" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="N16">
         <v>45.0897064208984</v>
@@ -3058,79 +3126,79 @@
         <v>-123.400299072265</v>
       </c>
       <c r="P16" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q16" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="R16" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="S16" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="T16">
         <v>1</v>
       </c>
       <c r="U16" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="V16" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="W16" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="X16" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="Y16" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="Z16" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="AA16" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="AB16" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="AC16" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="AD16" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="AE16">
         <v>97367</v>
       </c>
       <c r="AF16" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="AG16" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="AH16" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AJ16" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AL16" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="AN16" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="AO16" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="AP16" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="AQ16" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AS16">
         <v>0</v>
@@ -3142,76 +3210,76 @@
         <v>0</v>
       </c>
       <c r="AX16" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
       <c r="AY16" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="AZ16" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BA16" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="BB16" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="BD16" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="BE16" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="BF16" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="BG16" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="BH16" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="BJ16">
         <v>150</v>
       </c>
       <c r="BK16" t="s">
+        <v>324</v>
+      </c>
+      <c r="BL16" t="s">
         <v>314</v>
       </c>
-      <c r="BL16" t="s">
-        <v>304</v>
-      </c>
       <c r="BM16" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="BN16" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="BP16" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="CG16" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CH16" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="CI16" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CK16" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CL16" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CM16" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="CN16" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="CO16" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:99">
@@ -3225,7 +3293,7 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="E17">
         <v>100</v>
@@ -3240,7 +3308,7 @@
         <v>43382.4516087963</v>
       </c>
       <c r="I17" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="N17">
         <v>45.222900390625</v>
@@ -3249,67 +3317,67 @@
         <v>-121.292701721191</v>
       </c>
       <c r="P17" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q17" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="R17" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="S17" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="T17">
         <v>1</v>
       </c>
       <c r="U17" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="V17" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="W17" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="X17" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="Y17" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="Z17" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="AA17" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="AB17" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="AH17" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AJ17" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AL17" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="AN17" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="AO17" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="AP17" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="AQ17" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AR17" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="AS17">
         <v>0</v>
@@ -3327,31 +3395,31 @@
         <v>20</v>
       </c>
       <c r="AY17" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AZ17" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BA17" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BB17" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="BD17" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="BE17" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="BF17" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="BG17" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="BH17" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="BJ17">
         <v>150</v>
@@ -3360,49 +3428,49 @@
         <v>50</v>
       </c>
       <c r="BL17" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="BM17" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="BN17" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="BO17" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="BP17" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="BS17" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BT17" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BV17" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="CG17" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CH17" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="CK17" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CL17" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CM17" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CN17" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="CO17" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
     </row>
     <row r="18" spans="1:99">
@@ -3416,7 +3484,7 @@
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="E18">
         <v>100</v>
@@ -3431,7 +3499,7 @@
         <v>43382.52282407408</v>
       </c>
       <c r="I18" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="N18">
         <v>46.5491943359375</v>
@@ -3440,67 +3508,67 @@
         <v>-121.855499267578</v>
       </c>
       <c r="P18" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q18" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="R18" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="S18" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="T18">
         <v>2</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="V18" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="W18" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="X18" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="Y18" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="Z18" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="AA18" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="AB18" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="AH18" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AJ18" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AL18" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="AN18" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="AO18" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="AP18" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="AQ18" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AR18" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="AS18">
         <v>0</v>
@@ -3518,31 +3586,31 @@
         <v>2900</v>
       </c>
       <c r="AX18" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="AY18" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="AZ18" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BA18" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BB18" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="BD18">
         <v>68</v>
       </c>
       <c r="BE18" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="BF18" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="BH18" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="BJ18">
         <v>350</v>
@@ -3551,93 +3619,93 @@
         <v>350</v>
       </c>
       <c r="BL18" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="BM18" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="BN18" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="BO18" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="BP18" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="BQ18" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="BR18" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="BS18" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="BT18" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="BV18" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BW18" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="BX18" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="BY18" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="BZ18" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="CG18" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CH18" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CI18" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="CJ18" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="CK18" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CL18" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CM18" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CN18" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="CO18" t="s">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="CP18" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
     </row>
     <row r="19" spans="1:99">
       <c r="AN19" s="1" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="AO19" s="1" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="AP19" s="1" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="AQ19" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AR19" s="1" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="AS19" s="1">
         <v>0</v>
@@ -3655,33 +3723,33 @@
         <v>700</v>
       </c>
       <c r="AX19" s="1" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="AY19" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AZ19" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BA19" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BB19" s="1" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="BC19" s="1"/>
       <c r="BD19" s="1" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="BE19" s="1" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="BF19" s="1" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="BG19" s="1"/>
       <c r="BH19" s="1" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="BI19" s="1"/>
       <c r="BJ19" s="1">
@@ -3691,7 +3759,7 @@
         <v>200</v>
       </c>
       <c r="BL19" s="1" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="BM19" s="1">
         <v>10</v>
@@ -3700,40 +3768,40 @@
         <v>196</v>
       </c>
       <c r="BO19" s="1" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="BP19" s="1" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="BQ19" s="1" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="BR19" s="1" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="BS19" s="1" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="BT19" s="1" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="BU19" s="1" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="BV19" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BW19" s="1" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="BX19" s="1" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="BY19" s="1" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="BZ19" s="1" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="CA19" s="1"/>
       <c r="CB19" s="1"/>
@@ -3742,39 +3810,39 @@
       <c r="CE19" s="1"/>
       <c r="CF19" s="1"/>
       <c r="CG19" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CH19" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CI19" s="1" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="CJ19" s="1" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="CK19" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CL19" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CM19" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CN19" s="1" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="CO19" s="1" t="s">
-        <v>389</v>
+        <v>399</v>
       </c>
       <c r="CP19" s="1"/>
       <c r="CQ19" s="1" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="CR19" s="1"/>
       <c r="CS19" s="1" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="CT19" s="1"/>
       <c r="CU19" s="1"/>
@@ -3790,7 +3858,7 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="E21">
         <v>100</v>
@@ -3805,7 +3873,7 @@
         <v>43382.63358796296</v>
       </c>
       <c r="I21" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="N21">
         <v>44.9490051269531</v>
@@ -3814,64 +3882,64 @@
         <v>-123.003997802734</v>
       </c>
       <c r="P21" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q21" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="R21" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="S21" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="U21" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="V21" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="W21" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="X21" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="Y21" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="Z21" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="AA21" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="AB21" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="AC21" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="AD21" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="AE21">
         <v>97383</v>
       </c>
       <c r="AF21" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="AG21" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="AH21" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AJ21" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AL21" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:99">
@@ -3885,7 +3953,7 @@
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="E22">
         <v>100</v>
@@ -3900,7 +3968,7 @@
         <v>43383.45842592593</v>
       </c>
       <c r="I22" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="N22">
         <v>45.9828033447265</v>
@@ -3909,49 +3977,49 @@
         <v>-121.516296386718</v>
       </c>
       <c r="P22" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q22" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="R22" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="S22" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="U22" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="V22" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="W22" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="X22" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="Y22" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="Z22" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="AA22" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="AB22" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="AH22" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AJ22" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AL22" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
     </row>
     <row r="23" spans="1:99">
@@ -3965,7 +4033,7 @@
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="E23">
         <v>100</v>
@@ -3980,7 +4048,7 @@
         <v>43383.52400462963</v>
       </c>
       <c r="I23" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="N23">
         <v>45.5077972412109</v>
@@ -3989,82 +4057,82 @@
         <v>-122.689697265625</v>
       </c>
       <c r="P23" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="Q23" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="R23" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
       <c r="S23" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="T23">
         <v>4</v>
       </c>
       <c r="U23" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="V23" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="W23" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="X23" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="Y23" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
       <c r="Z23" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="AA23" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="AB23" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="AC23" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="AD23" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="AE23">
         <v>97112</v>
       </c>
       <c r="AF23" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="AG23" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="AH23" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AJ23" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="AL23" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="AN23" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="AO23" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="AP23" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="AQ23" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AR23" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="AS23">
         <v>0</v>
@@ -4082,34 +4150,34 @@
         <v>2000</v>
       </c>
       <c r="AX23" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="AY23" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AZ23" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BA23" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BB23" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="BD23">
         <v>790</v>
       </c>
       <c r="BE23" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="BF23" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="BG23" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="BH23" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="BJ23">
         <v>600</v>
@@ -4118,94 +4186,94 @@
         <v>0</v>
       </c>
       <c r="BL23" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="BM23" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="BN23" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="BO23" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="BP23" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="BQ23" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="BR23" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="BS23" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BT23" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BU23" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BV23" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BW23" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BX23" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BY23" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BZ23" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="CB23" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="CD23" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="CF23" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="CG23" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CH23" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CK23" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CL23" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CM23" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CN23" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="CO23" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
     </row>
     <row r="24" spans="1:99">
       <c r="AN24" s="1" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="AO24" s="1" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="AP24" s="1" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="AQ24" s="1"/>
       <c r="AR24" s="1" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="AS24" s="1">
         <v>0</v>
@@ -4223,35 +4291,35 @@
         <v>0</v>
       </c>
       <c r="AX24" s="1" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="AY24" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AZ24" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BA24" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BB24" s="1" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="BC24" s="1"/>
       <c r="BD24" s="1" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="BE24" s="1" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="BF24" s="1" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="BG24" s="1" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="BH24" s="1" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="BI24" s="1"/>
       <c r="BJ24" s="1">
@@ -4261,109 +4329,109 @@
         <v>0</v>
       </c>
       <c r="BL24" s="1" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="BM24" s="1" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="BN24" s="1" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="BO24" s="1" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="BP24" s="1" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="BQ24" s="1" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="BR24" s="1"/>
       <c r="BS24" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BT24" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BU24" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BV24" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BW24" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BX24" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BY24" s="1"/>
       <c r="BZ24" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="CA24" s="1"/>
       <c r="CB24" s="1" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="CC24" s="1"/>
       <c r="CD24" s="1" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="CE24" s="1"/>
       <c r="CF24" s="1" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="CG24" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CH24" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CI24" s="1"/>
       <c r="CJ24" s="1"/>
       <c r="CK24" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CL24" s="1" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="CM24" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CN24" s="1" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="CO24" s="1" t="s">
-        <v>393</v>
+        <v>403</v>
       </c>
       <c r="CP24" s="1"/>
       <c r="CQ24" s="1" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="CR24" s="1"/>
       <c r="CS24" s="1" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="CT24" s="1"/>
       <c r="CU24" s="1" t="s">
-        <v>400</v>
+        <v>410</v>
       </c>
     </row>
     <row r="25" spans="1:99">
       <c r="AN25" s="1" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="AO25" s="1" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="AP25" s="1" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="AQ25" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AR25" s="1" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="AS25" s="1">
         <v>0</v>
@@ -4381,33 +4449,33 @@
         <v>0</v>
       </c>
       <c r="AX25" s="1" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="AY25" s="1"/>
       <c r="AZ25" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BA25" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BB25" s="1" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="BC25" s="1"/>
       <c r="BD25" s="1">
         <v>640</v>
       </c>
       <c r="BE25" s="1" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="BF25" s="1" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="BG25" s="1" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="BH25" s="1" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="BI25" s="1"/>
       <c r="BJ25" s="1">
@@ -4417,113 +4485,113 @@
         <v>0</v>
       </c>
       <c r="BL25" s="1" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="BM25" s="1" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="BN25" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="BO25" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="BP25" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="BQ25" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="BO25" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="BP25" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="BQ25" s="1" t="s">
-        <v>352</v>
-      </c>
       <c r="BR25" s="1" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="BS25" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BT25" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BU25" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BV25" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BW25" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BX25" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BY25" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BZ25" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="CA25" s="1"/>
       <c r="CB25" s="1" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="CC25" s="1"/>
       <c r="CD25" s="1" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="CE25" s="1"/>
       <c r="CF25" s="1" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="CG25" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CH25" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CI25" s="1"/>
       <c r="CJ25" s="1"/>
       <c r="CK25" s="1" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="CL25" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CM25" s="1" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="CN25" s="1">
         <v>1961</v>
       </c>
       <c r="CO25" s="1" t="s">
-        <v>394</v>
+        <v>404</v>
       </c>
       <c r="CP25" s="1"/>
       <c r="CQ25" s="1" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="CR25" s="1"/>
       <c r="CS25" s="1" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="CT25" s="1"/>
       <c r="CU25" s="1" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
     </row>
     <row r="26" spans="1:99">
       <c r="AN26" s="1" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="AO26" s="1" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="AP26" s="1" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="AQ26" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="AR26" s="1" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="AS26" s="1">
         <v>0</v>
@@ -4541,33 +4609,33 @@
         <v>0</v>
       </c>
       <c r="AX26" s="1" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="AY26" s="1"/>
       <c r="AZ26" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BA26" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BB26" s="1" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="BC26" s="1"/>
       <c r="BD26" s="1">
         <v>640</v>
       </c>
       <c r="BE26" s="1" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="BF26" s="1" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="BG26" s="1" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="BH26" s="1" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="BI26" s="1"/>
       <c r="BJ26" s="1">
@@ -4577,100 +4645,100 @@
         <v>0</v>
       </c>
       <c r="BL26" s="1" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="BM26" s="1" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="BN26" s="1">
         <v>0</v>
       </c>
       <c r="BO26" s="1" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="BP26" s="1" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="BQ26" s="1" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="BR26" s="1" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="BS26" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BT26" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BU26" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BV26" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BW26" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BX26" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BY26" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="BZ26" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="CA26" s="1" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="CB26" s="1" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="CC26" s="1"/>
       <c r="CD26" s="1" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="CE26" s="1"/>
       <c r="CF26" s="1" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="CG26" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CH26" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CI26" s="1"/>
       <c r="CJ26" s="1"/>
       <c r="CK26" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CL26" s="1" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="CM26" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="CN26" s="1" t="s">
-        <v>395</v>
+        <v>405</v>
       </c>
       <c r="CO26" s="1" t="s">
-        <v>396</v>
+        <v>406</v>
       </c>
       <c r="CP26" s="1"/>
       <c r="CQ26" s="1" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="CR26" s="1"/>
       <c r="CS26" s="1" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
       <c r="CT26" s="1" t="s">
-        <v>404</v>
+        <v>414</v>
       </c>
       <c r="CU26" s="1" t="s">
-        <v>405</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Section 9 added with headings
</commit_message>
<xml_diff>
--- a/Anand_Work/FallWork2018/OUTPUT.xlsx
+++ b/Anand_Work/FallWork2018/OUTPUT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="441">
   <si>
     <t>Start Date</t>
   </si>
@@ -353,6 +353,58 @@
     <t>1 - Is there additional information that you would like to provide regarding DEI?</t>
   </si>
   <si>
+    <t>Please identify the types of partners that your program works with in order to provide outdoor _x000D_
+school: - 1 - Non-Governmental Organization or community-based organizations (e.g, watershed council, non-profit)</t>
+  </si>
+  <si>
+    <t>Please identify the types of partners that your program works with in order to provide outdoor _x000D_
+school: - 1 - university/college students</t>
+  </si>
+  <si>
+    <t>Please identify the types of partners that your program works with in order to provide outdoor _x000D_
+school: - 1 - parents/community members</t>
+  </si>
+  <si>
+    <t>Please identify the types of partners that your program works with in order to provide outdoor _x000D_
+school: - 1 - government organizations (e.g. forest service, department of fisheries and wildlife)</t>
+  </si>
+  <si>
+    <t>Please identify the types of partners that your program works with in order to provide outdoor _x000D_
+school: - 1 - volunteers</t>
+  </si>
+  <si>
+    <t>Please identify the types of partners that your program works with in order to provide outdoor _x000D_
+school: - 1 - school district</t>
+  </si>
+  <si>
+    <t>Please identify the types of partners that your program works with in order to provide outdoor _x000D_
+school: - 1 - farms</t>
+  </si>
+  <si>
+    <t>Please identify the types of partners that your program works with in order to provide outdoor _x000D_
+school: - 1 - high schools</t>
+  </si>
+  <si>
+    <t>Please identify the types of partners that your program works with in order to provide outdoor _x000D_
+school: - 1 - foundations</t>
+  </si>
+  <si>
+    <t>Please identify the types of partners that your program works with in order to provide outdoor _x000D_
+school: - 1 - local businesses</t>
+  </si>
+  <si>
+    <t>Please identify the types of partners that your program works with in order to provide outdoor _x000D_
+school: - 1 - OSU Extension</t>
+  </si>
+  <si>
+    <t>Please identify the types of partners that your program works with in order to provide outdoor _x000D_
+school: - 1 - Other</t>
+  </si>
+  <si>
+    <t>Please identify the types of partners that your program works with in order to provide outdoor _x000D_
+school: - 1 - Other - Text</t>
+  </si>
+  <si>
     <t>Survey Preview</t>
   </si>
   <si>
@@ -1324,6 +1376,9 @@
   </si>
   <si>
     <t>We offer summer student leadership programs for Latino, deaf, and tribal youth</t>
+  </si>
+  <si>
+    <t>Have worked with 4H over the years as they have had retreats and camps here for years.</t>
   </si>
 </sst>
 </file>
@@ -1677,13 +1732,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DE26"/>
+  <dimension ref="A1:DV26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:109">
+    <row r="1" spans="1:126">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2011,8 +2066,59 @@
       <c r="DE1" t="s">
         <v>104</v>
       </c>
+      <c r="DF1" t="s">
+        <v>105</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>106</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>107</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>108</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>109</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>110</v>
+      </c>
+      <c r="DL1" t="s">
+        <v>111</v>
+      </c>
+      <c r="DM1" t="s">
+        <v>112</v>
+      </c>
+      <c r="DN1" t="s">
+        <v>113</v>
+      </c>
+      <c r="DO1" t="s">
+        <v>114</v>
+      </c>
+      <c r="DP1" t="s">
+        <v>115</v>
+      </c>
+      <c r="DQ1" t="s">
+        <v>116</v>
+      </c>
+      <c r="DR1" t="s">
+        <v>117</v>
+      </c>
+      <c r="DS1" t="s">
+        <v>116</v>
+      </c>
+      <c r="DT1" t="s">
+        <v>117</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>116</v>
+      </c>
+      <c r="DV1" t="s">
+        <v>117</v>
+      </c>
     </row>
-    <row r="2" spans="1:109">
+    <row r="2" spans="1:126">
       <c r="A2">
         <v>43378.46934027778</v>
       </c>
@@ -2020,7 +2126,7 @@
         <v>43378.47023148148</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -2035,7 +2141,7 @@
         <v>43378.47024305556</v>
       </c>
       <c r="I2" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="N2">
         <v>44.5641937255859</v>
@@ -2044,13 +2150,13 @@
         <v>-123.278999328613</v>
       </c>
       <c r="P2" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="Q2" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:109">
+    <row r="3" spans="1:126">
       <c r="A3">
         <v>43378.47028935186</v>
       </c>
@@ -2058,7 +2164,7 @@
         <v>43378.47060185186</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -2073,7 +2179,7 @@
         <v>43378.47060185186</v>
       </c>
       <c r="I3" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="N3">
         <v>44.5641937255859</v>
@@ -2082,22 +2188,22 @@
         <v>-123.278999328613</v>
       </c>
       <c r="P3" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="Q3" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="AH3" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AJ3" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="AL3" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:109">
+    <row r="4" spans="1:126">
       <c r="A4">
         <v>43380.91150462963</v>
       </c>
@@ -2105,7 +2211,7 @@
         <v>43380.91293981481</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -2120,7 +2226,7 @@
         <v>43380.91295138889</v>
       </c>
       <c r="I4" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="N4">
         <v>44.5637969970703</v>
@@ -2129,10 +2235,10 @@
         <v>-123.2779006958</v>
       </c>
       <c r="P4" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="Q4" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="T4">
         <v>3</v>
@@ -2147,7 +2253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:109">
+    <row r="5" spans="1:126">
       <c r="AN5" s="1"/>
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
@@ -2224,8 +2330,25 @@
       <c r="DC5" s="1"/>
       <c r="DD5" s="1"/>
       <c r="DE5" s="1"/>
+      <c r="DF5" s="1"/>
+      <c r="DG5" s="1"/>
+      <c r="DH5" s="1"/>
+      <c r="DI5" s="1"/>
+      <c r="DJ5" s="1"/>
+      <c r="DK5" s="1"/>
+      <c r="DL5" s="1"/>
+      <c r="DM5" s="1"/>
+      <c r="DN5" s="1"/>
+      <c r="DO5" s="1"/>
+      <c r="DP5" s="1"/>
+      <c r="DQ5" s="1"/>
+      <c r="DR5" s="1"/>
+      <c r="DS5" s="1"/>
+      <c r="DT5" s="1"/>
+      <c r="DU5" s="1"/>
+      <c r="DV5" s="1"/>
     </row>
-    <row r="6" spans="1:109">
+    <row r="6" spans="1:126">
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
       <c r="AP6" s="1"/>
@@ -2302,8 +2425,25 @@
       <c r="DC6" s="1"/>
       <c r="DD6" s="1"/>
       <c r="DE6" s="1"/>
+      <c r="DF6" s="1"/>
+      <c r="DG6" s="1"/>
+      <c r="DH6" s="1"/>
+      <c r="DI6" s="1"/>
+      <c r="DJ6" s="1"/>
+      <c r="DK6" s="1"/>
+      <c r="DL6" s="1"/>
+      <c r="DM6" s="1"/>
+      <c r="DN6" s="1"/>
+      <c r="DO6" s="1"/>
+      <c r="DP6" s="1"/>
+      <c r="DQ6" s="1"/>
+      <c r="DR6" s="1"/>
+      <c r="DS6" s="1"/>
+      <c r="DT6" s="1"/>
+      <c r="DU6" s="1"/>
+      <c r="DV6" s="1"/>
     </row>
-    <row r="8" spans="1:109">
+    <row r="8" spans="1:126">
       <c r="A8">
         <v>43381.70964120371</v>
       </c>
@@ -2314,7 +2454,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="E8">
         <v>100</v>
@@ -2329,7 +2469,7 @@
         <v>43381.71163194445</v>
       </c>
       <c r="I8" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="N8">
         <v>40.7180023193359</v>
@@ -2338,52 +2478,52 @@
         <v>-74.0754013061523</v>
       </c>
       <c r="P8" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="Q8" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="R8" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="S8" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="U8" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="V8" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="W8" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="X8" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="Y8" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="Z8" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="AA8" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>138</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>123</v>
+      </c>
+      <c r="AJ8" t="s">
         <v>124</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AL8" t="s">
         <v>125</v>
       </c>
-      <c r="AH8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>111</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>112</v>
-      </c>
     </row>
-    <row r="9" spans="1:109">
+    <row r="9" spans="1:126">
       <c r="A9">
         <v>43381.71248842592</v>
       </c>
@@ -2394,7 +2534,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -2409,7 +2549,7 @@
         <v>43381.715</v>
       </c>
       <c r="I9" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="N9">
         <v>45.5653076171875</v>
@@ -2418,67 +2558,67 @@
         <v>-122.644798278808</v>
       </c>
       <c r="P9" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="Q9" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="R9" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="S9" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="U9" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="V9" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="W9" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="X9" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="Y9" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="Z9" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="AA9" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="AB9" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="AC9" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="AD9" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="AE9">
         <v>97055</v>
       </c>
       <c r="AF9" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="AG9" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="AH9" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AJ9" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="AL9" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:109">
+    <row r="10" spans="1:126">
       <c r="A10">
         <v>43381.71474537037</v>
       </c>
@@ -2489,7 +2629,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="E10">
         <v>100</v>
@@ -2504,7 +2644,7 @@
         <v>43381.71667824074</v>
       </c>
       <c r="I10" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="N10">
         <v>44.0682067871093</v>
@@ -2513,67 +2653,67 @@
         <v>-123.081901550292</v>
       </c>
       <c r="P10" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="Q10" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="R10" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="S10" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="V10" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="W10" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="X10" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA10" t="s">
         <v>149</v>
       </c>
-      <c r="Y10" t="s">
-        <v>150</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>136</v>
-      </c>
       <c r="AB10" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="AC10" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="AD10" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="AE10">
         <v>97419</v>
       </c>
       <c r="AF10" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="AG10" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="AH10" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AJ10" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="AL10" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:109">
+    <row r="11" spans="1:126">
       <c r="A11">
         <v>43381.71635416667</v>
       </c>
@@ -2584,7 +2724,7 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="E11">
         <v>100</v>
@@ -2599,7 +2739,7 @@
         <v>43381.72159722223</v>
       </c>
       <c r="I11" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="N11">
         <v>45.3726959228515</v>
@@ -2608,64 +2748,64 @@
         <v>-122.76309967041</v>
       </c>
       <c r="P11" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="Q11" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="R11" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="S11" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="U11" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="V11" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="W11" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="X11" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="Y11" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="AA11" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="AB11" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="AC11" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="AD11" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="AE11">
         <v>97064</v>
       </c>
       <c r="AF11" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="AG11" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="AH11" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AJ11" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="AL11" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:109">
+    <row r="12" spans="1:126">
       <c r="A12">
         <v>43381.74771990741</v>
       </c>
@@ -2676,7 +2816,7 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="E12">
         <v>100</v>
@@ -2691,7 +2831,7 @@
         <v>43381.75016203704</v>
       </c>
       <c r="I12" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="N12">
         <v>45.3493957519531</v>
@@ -2700,55 +2840,55 @@
         <v>-117.212799072265</v>
       </c>
       <c r="P12" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="Q12" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="R12" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="S12" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="U12" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="V12" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="W12" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="X12" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="Y12" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="Z12" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="AA12" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>192</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>193</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>194</v>
+      </c>
+      <c r="AJ12" t="s">
         <v>124</v>
       </c>
-      <c r="AB12" t="s">
-        <v>179</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>180</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>181</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>111</v>
-      </c>
       <c r="AL12" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:109">
+    <row r="13" spans="1:126">
       <c r="A13">
         <v>43381.7379050926</v>
       </c>
@@ -2759,7 +2899,7 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="E13">
         <v>100</v>
@@ -2774,7 +2914,7 @@
         <v>43381.75645833334</v>
       </c>
       <c r="I13" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="N13">
         <v>38.4797058105468</v>
@@ -2783,64 +2923,64 @@
         <v>-121.443801879882</v>
       </c>
       <c r="P13" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="Q13" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="R13" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="S13" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="T13">
         <v>1</v>
       </c>
       <c r="U13" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="V13" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="W13" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="X13" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="Y13" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="Z13" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="AA13" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>205</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>123</v>
+      </c>
+      <c r="AJ13" t="s">
         <v>124</v>
       </c>
-      <c r="AB13" t="s">
-        <v>192</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ13" t="s">
-        <v>111</v>
-      </c>
       <c r="AL13" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="AN13" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="AO13" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="AP13" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="AQ13" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AS13">
         <v>40</v>
@@ -2858,31 +2998,31 @@
         <v>1700</v>
       </c>
       <c r="AX13" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="AY13" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="AZ13" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BA13" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BB13" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="BD13" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="BE13" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="BF13" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="BH13" t="s">
-        <v>313</v>
+        <v>326</v>
       </c>
       <c r="BJ13">
         <v>240</v>
@@ -2891,7 +3031,7 @@
         <v>300</v>
       </c>
       <c r="BL13" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="BM13">
         <v>5</v>
@@ -2903,115 +3043,148 @@
         <v>500</v>
       </c>
       <c r="BP13" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="BQ13" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="BR13" t="s">
-        <v>317</v>
+        <v>330</v>
       </c>
       <c r="BS13" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BT13" t="s">
-        <v>381</v>
+        <v>394</v>
       </c>
       <c r="BU13" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BV13" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="BW13" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
       <c r="BX13" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
       <c r="BY13" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="CA13" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="CB13" t="s">
-        <v>384</v>
+        <v>397</v>
       </c>
       <c r="CC13" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="CD13" t="s">
-        <v>385</v>
+        <v>398</v>
       </c>
       <c r="CE13" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="CF13" t="s">
-        <v>386</v>
+        <v>399</v>
       </c>
       <c r="CG13" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CH13" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CK13" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CL13" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CM13" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CN13" t="s">
-        <v>388</v>
+        <v>401</v>
       </c>
       <c r="CO13" t="s">
-        <v>389</v>
+        <v>402</v>
       </c>
       <c r="CQ13" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
       <c r="CS13" t="s">
-        <v>408</v>
+        <v>421</v>
       </c>
       <c r="CU13" t="s">
-        <v>409</v>
+        <v>422</v>
       </c>
       <c r="CV13" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="CW13" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="CX13" t="s">
-        <v>422</v>
+        <v>435</v>
       </c>
       <c r="CY13" t="s">
-        <v>422</v>
+        <v>435</v>
       </c>
       <c r="CZ13" t="s">
-        <v>422</v>
+        <v>435</v>
       </c>
       <c r="DA13" t="s">
-        <v>422</v>
+        <v>435</v>
       </c>
       <c r="DB13" t="s">
-        <v>422</v>
+        <v>435</v>
       </c>
       <c r="DC13" t="s">
-        <v>422</v>
+        <v>435</v>
       </c>
       <c r="DD13" t="s">
-        <v>423</v>
+        <v>436</v>
       </c>
       <c r="DE13" t="s">
-        <v>424</v>
+        <v>437</v>
+      </c>
+      <c r="DF13" t="s">
+        <v>123</v>
+      </c>
+      <c r="DG13" t="s">
+        <v>123</v>
+      </c>
+      <c r="DH13" t="s">
+        <v>123</v>
+      </c>
+      <c r="DI13" t="s">
+        <v>123</v>
+      </c>
+      <c r="DJ13" t="s">
+        <v>123</v>
+      </c>
+      <c r="DK13" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL13" t="s">
+        <v>123</v>
+      </c>
+      <c r="DM13" t="s">
+        <v>123</v>
+      </c>
+      <c r="DN13" t="s">
+        <v>123</v>
+      </c>
+      <c r="DO13" t="s">
+        <v>123</v>
+      </c>
+      <c r="DP13" t="s">
+        <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:109">
+    <row r="14" spans="1:126">
       <c r="A14">
         <v>43381.87571759259</v>
       </c>
@@ -3022,7 +3195,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="E14">
         <v>100</v>
@@ -3037,7 +3210,7 @@
         <v>43381.88489583333</v>
       </c>
       <c r="I14" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="N14">
         <v>45.5440979003906</v>
@@ -3046,67 +3219,67 @@
         <v>-122.642303466796</v>
       </c>
       <c r="P14" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="Q14" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="R14" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="S14" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="U14" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="V14" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="W14" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="X14" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="Y14" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="Z14" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="AA14" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="AB14" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="AC14" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="AD14" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="AE14">
         <v>98671</v>
       </c>
       <c r="AF14" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="AG14" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="AH14" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="AJ14" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="AL14" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:109">
+    <row r="15" spans="1:126">
       <c r="A15">
         <v>43382.01947916667</v>
       </c>
@@ -3117,7 +3290,7 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="E15">
         <v>100</v>
@@ -3132,7 +3305,7 @@
         <v>43382.02648148148</v>
       </c>
       <c r="I15" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="N15">
         <v>48.465103149414</v>
@@ -3141,49 +3314,49 @@
         <v>7.95590209960937</v>
       </c>
       <c r="P15" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="Q15" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="R15" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="S15" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="U15" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="V15" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="W15" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="X15" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="Y15" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="Z15" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="AB15" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="AH15" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AJ15" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="AL15" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
     </row>
-    <row r="16" spans="1:109">
+    <row r="16" spans="1:126">
       <c r="A16">
         <v>43382.42454861111</v>
       </c>
@@ -3194,7 +3367,7 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="E16">
         <v>100</v>
@@ -3209,7 +3382,7 @@
         <v>43382.44296296296</v>
       </c>
       <c r="I16" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="N16">
         <v>45.0897064208984</v>
@@ -3218,79 +3391,79 @@
         <v>-123.400299072265</v>
       </c>
       <c r="P16" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="Q16" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="R16" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="S16" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="T16">
         <v>1</v>
       </c>
       <c r="U16" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="V16" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="W16" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="X16" t="s">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="Y16" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="Z16" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="AA16" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="AB16" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="AC16" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="AD16" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="AE16">
         <v>97367</v>
       </c>
       <c r="AF16" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="AG16" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="AH16" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AJ16" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="AL16" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="AN16" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="AO16" t="s">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c r="AP16" t="s">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c r="AQ16" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AS16">
         <v>0</v>
@@ -3302,88 +3475,106 @@
         <v>0</v>
       </c>
       <c r="AX16" t="s">
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="AY16" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="AZ16" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BA16" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="BB16" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="BD16" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="BE16" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="BF16" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="BG16" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="BH16" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="BJ16">
         <v>150</v>
       </c>
       <c r="BK16" t="s">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="BL16" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="BM16" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="BN16" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="BP16" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="CG16" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CH16" t="s">
-        <v>390</v>
+        <v>403</v>
       </c>
       <c r="CI16" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CK16" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CL16" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CM16" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="CN16" t="s">
-        <v>391</v>
+        <v>404</v>
       </c>
       <c r="CO16" t="s">
-        <v>392</v>
+        <v>405</v>
       </c>
       <c r="CQ16" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
       <c r="CS16" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
       <c r="CU16" t="s">
-        <v>411</v>
+        <v>424</v>
+      </c>
+      <c r="DF16" t="s">
+        <v>123</v>
+      </c>
+      <c r="DH16" t="s">
+        <v>123</v>
+      </c>
+      <c r="DI16" t="s">
+        <v>123</v>
+      </c>
+      <c r="DJ16" t="s">
+        <v>123</v>
+      </c>
+      <c r="DK16" t="s">
+        <v>123</v>
+      </c>
+      <c r="DP16" t="s">
+        <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:109">
+    <row r="17" spans="1:126">
       <c r="A17">
         <v>43382.4278125</v>
       </c>
@@ -3394,7 +3585,7 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="E17">
         <v>100</v>
@@ -3409,7 +3600,7 @@
         <v>43382.4516087963</v>
       </c>
       <c r="I17" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="N17">
         <v>45.222900390625</v>
@@ -3418,67 +3609,67 @@
         <v>-121.292701721191</v>
       </c>
       <c r="P17" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="Q17" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="R17" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="S17" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="T17">
         <v>1</v>
       </c>
       <c r="U17" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="V17" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="W17" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="X17" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="Y17" t="s">
-        <v>243</v>
+        <v>256</v>
       </c>
       <c r="Z17" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="AA17" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>258</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>123</v>
+      </c>
+      <c r="AJ17" t="s">
         <v>124</v>
       </c>
-      <c r="AB17" t="s">
-        <v>245</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>111</v>
-      </c>
       <c r="AL17" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="AN17" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="AO17" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="AP17" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
       <c r="AQ17" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AR17" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="AS17">
         <v>0</v>
@@ -3496,31 +3687,31 @@
         <v>20</v>
       </c>
       <c r="AY17" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AZ17" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BA17" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BB17" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="BD17" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="BE17" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="BF17" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="BG17" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="BH17" t="s">
-        <v>331</v>
+        <v>344</v>
       </c>
       <c r="BJ17">
         <v>150</v>
@@ -3529,85 +3720,130 @@
         <v>50</v>
       </c>
       <c r="BL17" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="BM17" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
       <c r="BN17" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="BO17" t="s">
-        <v>334</v>
+        <v>347</v>
       </c>
       <c r="BP17" t="s">
-        <v>335</v>
+        <v>348</v>
       </c>
       <c r="BS17" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BT17" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BV17" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="CG17" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CH17" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="CK17" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CL17" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CM17" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CN17" t="s">
-        <v>393</v>
+        <v>406</v>
       </c>
       <c r="CO17" t="s">
-        <v>394</v>
+        <v>407</v>
       </c>
       <c r="CQ17" t="s">
-        <v>412</v>
+        <v>425</v>
       </c>
       <c r="CS17" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
       <c r="CU17" t="s">
-        <v>413</v>
+        <v>426</v>
       </c>
       <c r="CV17" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="CW17" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="CX17" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="CY17" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="CZ17" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="DA17" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="DB17" t="s">
-        <v>422</v>
+        <v>435</v>
       </c>
       <c r="DC17" t="s">
-        <v>422</v>
+        <v>435</v>
+      </c>
+      <c r="DF17" t="s">
+        <v>223</v>
+      </c>
+      <c r="DG17" t="s">
+        <v>223</v>
+      </c>
+      <c r="DH17" t="s">
+        <v>123</v>
+      </c>
+      <c r="DI17" t="s">
+        <v>223</v>
+      </c>
+      <c r="DJ17" t="s">
+        <v>123</v>
+      </c>
+      <c r="DK17" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL17" t="s">
+        <v>223</v>
+      </c>
+      <c r="DM17" t="s">
+        <v>123</v>
+      </c>
+      <c r="DN17" t="s">
+        <v>223</v>
+      </c>
+      <c r="DO17" t="s">
+        <v>223</v>
+      </c>
+      <c r="DP17" t="s">
+        <v>123</v>
+      </c>
+      <c r="DQ17" t="s">
+        <v>123</v>
+      </c>
+      <c r="DR17" t="s">
+        <v>440</v>
+      </c>
+      <c r="DS17" t="s">
+        <v>223</v>
+      </c>
+      <c r="DU17" t="s">
+        <v>223</v>
       </c>
     </row>
-    <row r="18" spans="1:109">
+    <row r="18" spans="1:126">
       <c r="A18">
         <v>43382.50405092593</v>
       </c>
@@ -3618,7 +3854,7 @@
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="E18">
         <v>100</v>
@@ -3633,7 +3869,7 @@
         <v>43382.52282407408</v>
       </c>
       <c r="I18" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="N18">
         <v>46.5491943359375</v>
@@ -3642,67 +3878,67 @@
         <v>-121.855499267578</v>
       </c>
       <c r="P18" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="Q18" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="R18" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="S18" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="T18">
         <v>2</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>254</v>
+        <v>267</v>
       </c>
       <c r="V18" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="W18" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
       <c r="X18" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="Y18" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="Z18" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="AA18" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>205</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>123</v>
+      </c>
+      <c r="AJ18" t="s">
         <v>124</v>
       </c>
-      <c r="AB18" t="s">
-        <v>192</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ18" t="s">
-        <v>111</v>
-      </c>
       <c r="AL18" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="AN18" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="AO18" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="AP18" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="AQ18" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AR18" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="AS18">
         <v>0</v>
@@ -3720,31 +3956,31 @@
         <v>2900</v>
       </c>
       <c r="AX18" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="AY18" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="AZ18" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BA18" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BB18" t="s">
-        <v>337</v>
+        <v>350</v>
       </c>
       <c r="BD18">
         <v>68</v>
       </c>
       <c r="BE18" t="s">
-        <v>338</v>
+        <v>351</v>
       </c>
       <c r="BF18" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="BH18" t="s">
-        <v>339</v>
+        <v>352</v>
       </c>
       <c r="BJ18">
         <v>350</v>
@@ -3753,129 +3989,162 @@
         <v>350</v>
       </c>
       <c r="BL18" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="BM18" t="s">
-        <v>340</v>
+        <v>353</v>
       </c>
       <c r="BN18" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="BO18" t="s">
-        <v>342</v>
+        <v>355</v>
       </c>
       <c r="BP18" t="s">
-        <v>343</v>
+        <v>356</v>
       </c>
       <c r="BQ18" t="s">
-        <v>344</v>
+        <v>357</v>
       </c>
       <c r="BR18" t="s">
-        <v>345</v>
+        <v>358</v>
       </c>
       <c r="BS18" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="BT18" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="BV18" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BW18" t="s">
-        <v>381</v>
+        <v>394</v>
       </c>
       <c r="BX18" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="BY18" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
       <c r="BZ18" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
       <c r="CG18" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CH18" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CI18" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="CJ18" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="CK18" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CL18" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CM18" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CN18" t="s">
-        <v>395</v>
+        <v>408</v>
       </c>
       <c r="CO18" t="s">
-        <v>396</v>
+        <v>409</v>
       </c>
       <c r="CP18" t="s">
-        <v>397</v>
+        <v>410</v>
       </c>
       <c r="CQ18" t="s">
-        <v>414</v>
+        <v>427</v>
       </c>
       <c r="CS18" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
       <c r="CV18" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="CW18" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="CX18" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="CY18" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="CZ18" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="DA18" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="DB18" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="DC18" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="DD18" t="s">
-        <v>425</v>
+        <v>438</v>
       </c>
       <c r="DE18" t="s">
-        <v>426</v>
+        <v>439</v>
+      </c>
+      <c r="DF18" t="s">
+        <v>123</v>
+      </c>
+      <c r="DG18" t="s">
+        <v>123</v>
+      </c>
+      <c r="DH18" t="s">
+        <v>123</v>
+      </c>
+      <c r="DI18" t="s">
+        <v>123</v>
+      </c>
+      <c r="DJ18" t="s">
+        <v>123</v>
+      </c>
+      <c r="DK18" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL18" t="s">
+        <v>223</v>
+      </c>
+      <c r="DM18" t="s">
+        <v>123</v>
+      </c>
+      <c r="DN18" t="s">
+        <v>123</v>
+      </c>
+      <c r="DO18" t="s">
+        <v>223</v>
+      </c>
+      <c r="DP18" t="s">
+        <v>223</v>
       </c>
     </row>
-    <row r="19" spans="1:109">
+    <row r="19" spans="1:126">
       <c r="AN19" s="1" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="AO19" s="1" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="AP19" s="1" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="AQ19" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AR19" s="1" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="AS19" s="1">
         <v>0</v>
@@ -3893,33 +4162,33 @@
         <v>700</v>
       </c>
       <c r="AX19" s="1" t="s">
-        <v>346</v>
+        <v>359</v>
       </c>
       <c r="AY19" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AZ19" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BA19" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BB19" s="1" t="s">
-        <v>347</v>
+        <v>360</v>
       </c>
       <c r="BC19" s="1"/>
       <c r="BD19" s="1" t="s">
-        <v>348</v>
+        <v>361</v>
       </c>
       <c r="BE19" s="1" t="s">
-        <v>349</v>
+        <v>362</v>
       </c>
       <c r="BF19" s="1" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="BG19" s="1"/>
       <c r="BH19" s="1" t="s">
-        <v>339</v>
+        <v>352</v>
       </c>
       <c r="BI19" s="1"/>
       <c r="BJ19" s="1">
@@ -3929,7 +4198,7 @@
         <v>200</v>
       </c>
       <c r="BL19" s="1" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="BM19" s="1">
         <v>10</v>
@@ -3938,40 +4207,40 @@
         <v>196</v>
       </c>
       <c r="BO19" s="1" t="s">
-        <v>350</v>
+        <v>363</v>
       </c>
       <c r="BP19" s="1" t="s">
-        <v>351</v>
+        <v>364</v>
       </c>
       <c r="BQ19" s="1" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="BR19" s="1" t="s">
-        <v>353</v>
+        <v>366</v>
       </c>
       <c r="BS19" s="1" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="BT19" s="1" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="BU19" s="1" t="s">
-        <v>381</v>
+        <v>394</v>
       </c>
       <c r="BV19" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BW19" s="1" t="s">
-        <v>381</v>
+        <v>394</v>
       </c>
       <c r="BX19" s="1" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="BY19" s="1" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
       <c r="BZ19" s="1" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
       <c r="CA19" s="1"/>
       <c r="CB19" s="1"/>
@@ -3980,74 +4249,113 @@
       <c r="CE19" s="1"/>
       <c r="CF19" s="1"/>
       <c r="CG19" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CH19" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CI19" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="CJ19" s="1" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="CK19" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CL19" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CM19" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CN19" s="1" t="s">
-        <v>398</v>
+        <v>411</v>
       </c>
       <c r="CO19" s="1" t="s">
-        <v>399</v>
+        <v>412</v>
       </c>
       <c r="CP19" s="1"/>
       <c r="CQ19" s="1" t="s">
-        <v>415</v>
+        <v>428</v>
       </c>
       <c r="CR19" s="1"/>
       <c r="CS19" s="1" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
       <c r="CT19" s="1"/>
       <c r="CU19" s="1"/>
       <c r="CV19" s="1" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="CW19" s="1" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="CX19" s="1" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="CY19" s="1" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="CZ19" s="1" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="DA19" s="1" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="DB19" s="1" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="DC19" s="1" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="DD19" s="1" t="s">
-        <v>425</v>
+        <v>438</v>
       </c>
       <c r="DE19" s="1" t="s">
-        <v>426</v>
-      </c>
+        <v>439</v>
+      </c>
+      <c r="DF19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DG19" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="DH19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DI19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DJ19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DK19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL19" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="DM19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DN19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DO19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DP19" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="DQ19" s="1"/>
+      <c r="DR19" s="1"/>
+      <c r="DS19" s="1"/>
+      <c r="DT19" s="1"/>
+      <c r="DU19" s="1"/>
+      <c r="DV19" s="1"/>
     </row>
-    <row r="21" spans="1:109">
+    <row r="21" spans="1:126">
       <c r="A21">
         <v>43382.63195601852</v>
       </c>
@@ -4058,7 +4366,7 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="E21">
         <v>100</v>
@@ -4073,7 +4381,7 @@
         <v>43382.63358796296</v>
       </c>
       <c r="I21" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="N21">
         <v>44.9490051269531</v>
@@ -4082,67 +4390,67 @@
         <v>-123.003997802734</v>
       </c>
       <c r="P21" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="Q21" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="R21" t="s">
-        <v>266</v>
+        <v>279</v>
       </c>
       <c r="S21" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="U21" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="V21" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="W21" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
       <c r="X21" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="Y21" t="s">
-        <v>266</v>
+        <v>279</v>
       </c>
       <c r="Z21" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="AA21" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="AB21" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
       <c r="AC21" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="AD21" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
       <c r="AE21">
         <v>97383</v>
       </c>
       <c r="AF21" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="AG21" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
       <c r="AH21" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AJ21" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="AL21" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:109">
+    <row r="22" spans="1:126">
       <c r="A22">
         <v>43383.43930555556</v>
       </c>
@@ -4153,7 +4461,7 @@
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="E22">
         <v>100</v>
@@ -4168,7 +4476,7 @@
         <v>43383.45842592593</v>
       </c>
       <c r="I22" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="N22">
         <v>45.9828033447265</v>
@@ -4177,52 +4485,52 @@
         <v>-121.516296386718</v>
       </c>
       <c r="P22" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="Q22" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="R22" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="S22" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="U22" t="s">
-        <v>282</v>
+        <v>295</v>
       </c>
       <c r="V22" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="W22" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="X22" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="Y22" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="Z22" t="s">
-        <v>287</v>
+        <v>300</v>
       </c>
       <c r="AA22" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>301</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>123</v>
+      </c>
+      <c r="AJ22" t="s">
         <v>124</v>
       </c>
-      <c r="AB22" t="s">
-        <v>288</v>
-      </c>
-      <c r="AH22" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ22" t="s">
-        <v>111</v>
-      </c>
       <c r="AL22" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
     </row>
-    <row r="23" spans="1:109">
+    <row r="23" spans="1:126">
       <c r="A23">
         <v>43383.49253472222</v>
       </c>
@@ -4233,7 +4541,7 @@
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="E23">
         <v>100</v>
@@ -4248,7 +4556,7 @@
         <v>43383.52400462963</v>
       </c>
       <c r="I23" t="s">
-        <v>291</v>
+        <v>304</v>
       </c>
       <c r="N23">
         <v>45.5077972412109</v>
@@ -4257,82 +4565,82 @@
         <v>-122.689697265625</v>
       </c>
       <c r="P23" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="Q23" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="R23" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="S23" t="s">
-        <v>293</v>
+        <v>306</v>
       </c>
       <c r="T23">
         <v>4</v>
       </c>
       <c r="U23" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
       <c r="V23" t="s">
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="W23" t="s">
-        <v>296</v>
+        <v>309</v>
       </c>
       <c r="X23" t="s">
-        <v>297</v>
+        <v>310</v>
       </c>
       <c r="Y23" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="Z23" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="AA23" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="AB23" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="AC23" t="s">
-        <v>300</v>
+        <v>313</v>
       </c>
       <c r="AD23" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="AE23">
         <v>97112</v>
       </c>
       <c r="AF23" t="s">
-        <v>301</v>
+        <v>314</v>
       </c>
       <c r="AG23" t="s">
-        <v>302</v>
+        <v>315</v>
       </c>
       <c r="AH23" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AJ23" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="AL23" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="AN23" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="AO23" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="AP23" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="AQ23" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AR23" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="AS23">
         <v>0</v>
@@ -4350,34 +4658,34 @@
         <v>2000</v>
       </c>
       <c r="AX23" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
       <c r="AY23" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AZ23" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BA23" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BB23" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
       <c r="BD23">
         <v>790</v>
       </c>
       <c r="BE23" t="s">
-        <v>356</v>
+        <v>369</v>
       </c>
       <c r="BF23" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="BG23" t="s">
-        <v>357</v>
+        <v>370</v>
       </c>
       <c r="BH23" t="s">
-        <v>339</v>
+        <v>352</v>
       </c>
       <c r="BJ23">
         <v>600</v>
@@ -4386,103 +4694,118 @@
         <v>0</v>
       </c>
       <c r="BL23" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="BM23" t="s">
-        <v>358</v>
+        <v>371</v>
       </c>
       <c r="BN23" t="s">
-        <v>359</v>
+        <v>372</v>
       </c>
       <c r="BO23" t="s">
-        <v>360</v>
+        <v>373</v>
       </c>
       <c r="BP23" t="s">
-        <v>361</v>
+        <v>374</v>
       </c>
       <c r="BQ23" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="BR23" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="BS23" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BT23" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BU23" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BV23" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BW23" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BX23" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BY23" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BZ23" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="CB23" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="CD23" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="CF23" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="CG23" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CH23" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CK23" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CL23" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CM23" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CN23" t="s">
-        <v>400</v>
+        <v>413</v>
       </c>
       <c r="CO23" t="s">
-        <v>401</v>
+        <v>414</v>
       </c>
       <c r="CQ23" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
       <c r="CS23" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
       <c r="CU23" t="s">
-        <v>416</v>
+        <v>429</v>
+      </c>
+      <c r="DF23" t="s">
+        <v>123</v>
+      </c>
+      <c r="DG23" t="s">
+        <v>123</v>
+      </c>
+      <c r="DH23" t="s">
+        <v>123</v>
+      </c>
+      <c r="DI23" t="s">
+        <v>123</v>
+      </c>
+      <c r="DK23" t="s">
+        <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:109">
+    <row r="24" spans="1:126">
       <c r="AN24" s="1" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
       <c r="AO24" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="AP24" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="AQ24" s="1"/>
       <c r="AR24" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="AS24" s="1">
         <v>0</v>
@@ -4500,35 +4823,35 @@
         <v>0</v>
       </c>
       <c r="AX24" s="1" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="AY24" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AZ24" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BA24" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BB24" s="1" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
       <c r="BC24" s="1"/>
       <c r="BD24" s="1" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="BE24" s="1" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="BF24" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="BG24" s="1" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="BH24" s="1" t="s">
-        <v>365</v>
+        <v>378</v>
       </c>
       <c r="BI24" s="1"/>
       <c r="BJ24" s="1">
@@ -4538,92 +4861,92 @@
         <v>0</v>
       </c>
       <c r="BL24" s="1" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="BM24" s="1" t="s">
-        <v>366</v>
+        <v>379</v>
       </c>
       <c r="BN24" s="1" t="s">
-        <v>367</v>
+        <v>380</v>
       </c>
       <c r="BO24" s="1" t="s">
-        <v>368</v>
+        <v>381</v>
       </c>
       <c r="BP24" s="1" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="BQ24" s="1" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="BR24" s="1"/>
       <c r="BS24" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BT24" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BU24" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BV24" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BW24" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BX24" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BY24" s="1"/>
       <c r="BZ24" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="CA24" s="1"/>
       <c r="CB24" s="1" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="CC24" s="1"/>
       <c r="CD24" s="1" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="CE24" s="1"/>
       <c r="CF24" s="1" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="CG24" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CH24" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CI24" s="1"/>
       <c r="CJ24" s="1"/>
       <c r="CK24" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CL24" s="1" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="CM24" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CN24" s="1" t="s">
-        <v>402</v>
+        <v>415</v>
       </c>
       <c r="CO24" s="1" t="s">
-        <v>403</v>
+        <v>416</v>
       </c>
       <c r="CP24" s="1"/>
       <c r="CQ24" s="1" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
       <c r="CR24" s="1"/>
       <c r="CS24" s="1" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
       <c r="CT24" s="1"/>
       <c r="CU24" s="1" t="s">
-        <v>416</v>
+        <v>429</v>
       </c>
       <c r="CV24" s="1"/>
       <c r="CW24" s="1"/>
@@ -4635,22 +4958,45 @@
       <c r="DC24" s="1"/>
       <c r="DD24" s="1"/>
       <c r="DE24" s="1"/>
+      <c r="DF24" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DG24" s="1"/>
+      <c r="DH24" s="1"/>
+      <c r="DI24" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DJ24" s="1"/>
+      <c r="DK24" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL24" s="1"/>
+      <c r="DM24" s="1"/>
+      <c r="DN24" s="1"/>
+      <c r="DO24" s="1"/>
+      <c r="DP24" s="1"/>
+      <c r="DQ24" s="1"/>
+      <c r="DR24" s="1"/>
+      <c r="DS24" s="1"/>
+      <c r="DT24" s="1"/>
+      <c r="DU24" s="1"/>
+      <c r="DV24" s="1"/>
     </row>
-    <row r="25" spans="1:109">
+    <row r="25" spans="1:126">
       <c r="AN25" s="1" t="s">
-        <v>306</v>
+        <v>319</v>
       </c>
       <c r="AO25" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="AP25" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="AQ25" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AR25" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="AS25" s="1">
         <v>0</v>
@@ -4668,33 +5014,33 @@
         <v>0</v>
       </c>
       <c r="AX25" s="1" t="s">
-        <v>369</v>
+        <v>382</v>
       </c>
       <c r="AY25" s="1"/>
       <c r="AZ25" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BA25" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BB25" s="1" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
       <c r="BC25" s="1"/>
       <c r="BD25" s="1">
         <v>640</v>
       </c>
       <c r="BE25" s="1" t="s">
-        <v>370</v>
+        <v>383</v>
       </c>
       <c r="BF25" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="BG25" s="1" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="BH25" s="1" t="s">
-        <v>339</v>
+        <v>352</v>
       </c>
       <c r="BI25" s="1"/>
       <c r="BJ25" s="1">
@@ -4704,96 +5050,96 @@
         <v>0</v>
       </c>
       <c r="BL25" s="1" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="BM25" s="1" t="s">
-        <v>371</v>
+        <v>384</v>
       </c>
       <c r="BN25" s="1" t="s">
-        <v>372</v>
+        <v>385</v>
       </c>
       <c r="BO25" s="1" t="s">
-        <v>373</v>
+        <v>386</v>
       </c>
       <c r="BP25" s="1" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="BQ25" s="1" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="BR25" s="1" t="s">
-        <v>374</v>
+        <v>387</v>
       </c>
       <c r="BS25" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BT25" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BU25" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BV25" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BW25" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BX25" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BY25" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BZ25" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="CA25" s="1"/>
       <c r="CB25" s="1" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="CC25" s="1"/>
       <c r="CD25" s="1" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="CE25" s="1"/>
       <c r="CF25" s="1" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="CG25" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CH25" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CI25" s="1"/>
       <c r="CJ25" s="1"/>
       <c r="CK25" s="1" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="CL25" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CM25" s="1" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="CN25" s="1">
         <v>1961</v>
       </c>
       <c r="CO25" s="1" t="s">
-        <v>404</v>
+        <v>417</v>
       </c>
       <c r="CP25" s="1"/>
       <c r="CQ25" s="1" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
       <c r="CR25" s="1"/>
       <c r="CS25" s="1" t="s">
-        <v>408</v>
+        <v>421</v>
       </c>
       <c r="CT25" s="1"/>
       <c r="CU25" s="1" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="CV25" s="1"/>
       <c r="CW25" s="1"/>
@@ -4805,22 +5151,45 @@
       <c r="DC25" s="1"/>
       <c r="DD25" s="1"/>
       <c r="DE25" s="1"/>
+      <c r="DF25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DG25" s="1"/>
+      <c r="DH25" s="1"/>
+      <c r="DI25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DJ25" s="1"/>
+      <c r="DK25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL25" s="1"/>
+      <c r="DM25" s="1"/>
+      <c r="DN25" s="1"/>
+      <c r="DO25" s="1"/>
+      <c r="DP25" s="1"/>
+      <c r="DQ25" s="1"/>
+      <c r="DR25" s="1"/>
+      <c r="DS25" s="1"/>
+      <c r="DT25" s="1"/>
+      <c r="DU25" s="1"/>
+      <c r="DV25" s="1"/>
     </row>
-    <row r="26" spans="1:109">
+    <row r="26" spans="1:126">
       <c r="AN26" s="1" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="AO26" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="AP26" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="AQ26" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="AR26" s="1" t="s">
-        <v>304</v>
+        <v>317</v>
       </c>
       <c r="AS26" s="1">
         <v>0</v>
@@ -4838,33 +5207,33 @@
         <v>0</v>
       </c>
       <c r="AX26" s="1" t="s">
-        <v>375</v>
+        <v>388</v>
       </c>
       <c r="AY26" s="1"/>
       <c r="AZ26" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BA26" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="BB26" s="1" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
       <c r="BC26" s="1"/>
       <c r="BD26" s="1">
         <v>640</v>
       </c>
       <c r="BE26" s="1" t="s">
-        <v>376</v>
+        <v>389</v>
       </c>
       <c r="BF26" s="1" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="BG26" s="1" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="BH26" s="1" t="s">
-        <v>339</v>
+        <v>352</v>
       </c>
       <c r="BI26" s="1"/>
       <c r="BJ26" s="1">
@@ -4874,100 +5243,100 @@
         <v>0</v>
       </c>
       <c r="BL26" s="1" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="BM26" s="1" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="BN26" s="1">
         <v>0</v>
       </c>
       <c r="BO26" s="1" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
       <c r="BP26" s="1" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="BQ26" s="1" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="BR26" s="1" t="s">
-        <v>379</v>
+        <v>392</v>
       </c>
       <c r="BS26" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BT26" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BU26" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BV26" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BW26" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BX26" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BY26" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="BZ26" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="CA26" s="1" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="CB26" s="1" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="CC26" s="1"/>
       <c r="CD26" s="1" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="CE26" s="1"/>
       <c r="CF26" s="1" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="CG26" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CH26" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CI26" s="1"/>
       <c r="CJ26" s="1"/>
       <c r="CK26" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CL26" s="1" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="CM26" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="CN26" s="1" t="s">
-        <v>405</v>
+        <v>418</v>
       </c>
       <c r="CO26" s="1" t="s">
-        <v>406</v>
+        <v>419</v>
       </c>
       <c r="CP26" s="1"/>
       <c r="CQ26" s="1" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
       <c r="CR26" s="1"/>
       <c r="CS26" s="1" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="CT26" s="1" t="s">
-        <v>419</v>
+        <v>432</v>
       </c>
       <c r="CU26" s="1" t="s">
-        <v>420</v>
+        <v>433</v>
       </c>
       <c r="CV26" s="1"/>
       <c r="CW26" s="1"/>
@@ -4979,6 +5348,29 @@
       <c r="DC26" s="1"/>
       <c r="DD26" s="1"/>
       <c r="DE26" s="1"/>
+      <c r="DF26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DG26" s="1"/>
+      <c r="DH26" s="1"/>
+      <c r="DI26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DJ26" s="1"/>
+      <c r="DK26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DL26" s="1"/>
+      <c r="DM26" s="1"/>
+      <c r="DN26" s="1"/>
+      <c r="DO26" s="1"/>
+      <c r="DP26" s="1"/>
+      <c r="DQ26" s="1"/>
+      <c r="DR26" s="1"/>
+      <c r="DS26" s="1"/>
+      <c r="DT26" s="1"/>
+      <c r="DU26" s="1"/>
+      <c r="DV26" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Completed Last Section 10
</commit_message>
<xml_diff>
--- a/Anand_Work/FallWork2018/OUTPUT.xlsx
+++ b/Anand_Work/FallWork2018/OUTPUT.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\GitHub\qualtrics_data_py\Anand_Work\FallWork2018\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Provider Suvery Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="454">
   <si>
     <t>Start Date</t>
   </si>
@@ -405,6 +410,15 @@
 school: - 1 - Other - Text</t>
   </si>
   <si>
+    <t>1 - What kind of professional development do you and/or your staff recieve?</t>
+  </si>
+  <si>
+    <t>1 - Who conducts professional development for you and/or your staff?</t>
+  </si>
+  <si>
+    <t>1 - What are your greatest professional development needs? (e.g. field study, strategies for engaging students, etc.)</t>
+  </si>
+  <si>
     <t>Survey Preview</t>
   </si>
   <si>
@@ -1379,13 +1393,43 @@
   </si>
   <si>
     <t>Have worked with 4H over the years as they have had retreats and camps here for years.</t>
+  </si>
+  <si>
+    <t>We have over 40 years of outdoor school experience between 3 staff, but we could always use more training. We do trainings on everything from abuse to diversity.</t>
+  </si>
+  <si>
+    <t>I do, executive director of Grove Camp and we try to attend training elsewhere when available.</t>
+  </si>
+  <si>
+    <t>Strategies</t>
+  </si>
+  <si>
+    <t>I take classes through ONREP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our staff is small. Essentially we are only capable of providing a facility. We do not have adequate staffing to provide instruction. </t>
+  </si>
+  <si>
+    <t>Attend a camp conference on an annual basis including workshops and teaching.</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>1st aid training, job related seminars off site</t>
+  </si>
+  <si>
+    <t>local and state professionals</t>
+  </si>
+  <si>
+    <t>sound business practices</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1444,6 +1488,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1490,7 +1542,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1522,9 +1574,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1556,6 +1609,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1731,14 +1785,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DV26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:DY26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="DJ10" workbookViewId="0">
+      <selection activeCell="DQ20" sqref="DQ20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:126">
+    <row r="1" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2117,16 +2173,25 @@
       <c r="DV1" t="s">
         <v>117</v>
       </c>
+      <c r="DW1" t="s">
+        <v>118</v>
+      </c>
+      <c r="DX1" t="s">
+        <v>119</v>
+      </c>
+      <c r="DY1" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="2" spans="1:126">
+    <row r="2" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>43378.46934027778</v>
+        <v>43378.469340277778</v>
       </c>
       <c r="B2">
-        <v>43378.47023148148</v>
+        <v>43378.470231481479</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -2138,33 +2203,33 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>43378.47024305556</v>
+        <v>43378.470243055563</v>
       </c>
       <c r="I2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="N2">
-        <v>44.5641937255859</v>
+        <v>44.564193725585902</v>
       </c>
       <c r="O2">
         <v>-123.278999328613</v>
       </c>
       <c r="P2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="Q2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:129" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>43378.470289351862</v>
+      </c>
+      <c r="B3">
+        <v>43378.470601851863</v>
+      </c>
+      <c r="C3" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:126">
-      <c r="A3">
-        <v>43378.47028935186</v>
-      </c>
-      <c r="B3">
-        <v>43378.47060185186</v>
-      </c>
-      <c r="C3" t="s">
-        <v>118</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -2176,42 +2241,42 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>43378.47060185186</v>
+        <v>43378.470601851863</v>
       </c>
       <c r="I3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="N3">
-        <v>44.5641937255859</v>
+        <v>44.564193725585902</v>
       </c>
       <c r="O3">
         <v>-123.278999328613</v>
       </c>
       <c r="P3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="Q3" t="s">
+        <v>124</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:129" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>43380.911504629628</v>
+      </c>
+      <c r="B4">
+        <v>43380.912939814807</v>
+      </c>
+      <c r="C4" t="s">
         <v>121</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>123</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>124</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:126">
-      <c r="A4">
-        <v>43380.91150462963</v>
-      </c>
-      <c r="B4">
-        <v>43380.91293981481</v>
-      </c>
-      <c r="C4" t="s">
-        <v>118</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -2223,22 +2288,22 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>43380.91295138889</v>
+        <v>43380.912951388891</v>
       </c>
       <c r="I4" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="N4">
-        <v>44.5637969970703</v>
+        <v>44.563796997070298</v>
       </c>
       <c r="O4">
         <v>-123.2779006958</v>
       </c>
       <c r="P4" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="Q4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="T4">
         <v>3</v>
@@ -2253,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:126">
+    <row r="5" spans="1:129" x14ac:dyDescent="0.25">
       <c r="AN5" s="1"/>
       <c r="AO5" s="1"/>
       <c r="AP5" s="1"/>
@@ -2347,8 +2412,11 @@
       <c r="DT5" s="1"/>
       <c r="DU5" s="1"/>
       <c r="DV5" s="1"/>
+      <c r="DW5" s="1"/>
+      <c r="DX5" s="1"/>
+      <c r="DY5" s="1"/>
     </row>
-    <row r="6" spans="1:126">
+    <row r="6" spans="1:129" x14ac:dyDescent="0.25">
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
       <c r="AP6" s="1"/>
@@ -2442,10 +2510,13 @@
       <c r="DT6" s="1"/>
       <c r="DU6" s="1"/>
       <c r="DV6" s="1"/>
+      <c r="DW6" s="1"/>
+      <c r="DX6" s="1"/>
+      <c r="DY6" s="1"/>
     </row>
-    <row r="8" spans="1:126">
+    <row r="8" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>43381.70964120371</v>
+        <v>43381.709641203714</v>
       </c>
       <c r="B8">
         <v>43381.71162037037</v>
@@ -2454,7 +2525,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E8">
         <v>100</v>
@@ -2466,75 +2537,75 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>43381.71163194445</v>
+        <v>43381.711631944447</v>
       </c>
       <c r="I8" t="s">
+        <v>131</v>
+      </c>
+      <c r="N8">
+        <v>40.718002319335902</v>
+      </c>
+      <c r="O8">
+        <v>-74.075401306152301</v>
+      </c>
+      <c r="P8" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>124</v>
+      </c>
+      <c r="R8" t="s">
+        <v>133</v>
+      </c>
+      <c r="S8" t="s">
+        <v>134</v>
+      </c>
+      <c r="U8" t="s">
+        <v>135</v>
+      </c>
+      <c r="V8" t="s">
+        <v>136</v>
+      </c>
+      <c r="W8" t="s">
+        <v>137</v>
+      </c>
+      <c r="X8" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL8" t="s">
         <v>128</v>
       </c>
-      <c r="N8">
-        <v>40.7180023193359</v>
-      </c>
-      <c r="O8">
-        <v>-74.0754013061523</v>
-      </c>
-      <c r="P8" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>121</v>
-      </c>
-      <c r="R8" t="s">
-        <v>130</v>
-      </c>
-      <c r="S8" t="s">
-        <v>131</v>
-      </c>
-      <c r="U8" t="s">
-        <v>132</v>
-      </c>
-      <c r="V8" t="s">
-        <v>133</v>
-      </c>
-      <c r="W8" t="s">
-        <v>134</v>
-      </c>
-      <c r="X8" t="s">
-        <v>135</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>130</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>136</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>138</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>123</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>124</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>125</v>
-      </c>
     </row>
-    <row r="9" spans="1:126">
+    <row r="9" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>43381.71248842592</v>
+        <v>43381.712488425917</v>
       </c>
       <c r="B9">
-        <v>43381.715</v>
+        <v>43381.714999999997</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -2546,10 +2617,10 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>43381.715</v>
+        <v>43381.714999999997</v>
       </c>
       <c r="I9" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N9">
         <v>45.5653076171875</v>
@@ -2558,78 +2629,78 @@
         <v>-122.644798278808</v>
       </c>
       <c r="P9" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="Q9" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R9" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="S9" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="U9" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="V9" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="W9" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="X9" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="Y9" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="Z9" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AA9" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AB9" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AC9" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="AD9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="AE9">
         <v>97055</v>
       </c>
       <c r="AF9" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="AG9" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="AH9" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AJ9" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL9" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:126">
+    <row r="10" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>43381.71474537037</v>
+        <v>43381.714745370373</v>
       </c>
       <c r="B10">
-        <v>43381.71667824074</v>
+        <v>43381.716678240737</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E10">
         <v>100</v>
@@ -2641,90 +2712,90 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>43381.71667824074</v>
+        <v>43381.716678240737</v>
       </c>
       <c r="I10" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N10">
-        <v>44.0682067871093</v>
+        <v>44.068206787109297</v>
       </c>
       <c r="O10">
         <v>-123.081901550292</v>
       </c>
       <c r="P10" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="Q10" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R10" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="S10" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="V10" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="W10" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="X10" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="Y10" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="Z10" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="AA10" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AB10" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="AC10" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="AD10" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="AE10">
         <v>97419</v>
       </c>
       <c r="AF10" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="AG10" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="AH10" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AJ10" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL10" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:126">
+    <row r="11" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>43381.71635416667</v>
+        <v>43381.716354166667</v>
       </c>
       <c r="B11">
-        <v>43381.72159722223</v>
+        <v>43381.721597222233</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E11">
         <v>100</v>
@@ -2736,87 +2807,87 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>43381.72159722223</v>
+        <v>43381.721597222233</v>
       </c>
       <c r="I11" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="N11">
-        <v>45.3726959228515</v>
+        <v>45.372695922851499</v>
       </c>
       <c r="O11">
         <v>-122.76309967041</v>
       </c>
       <c r="P11" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="Q11" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R11" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="S11" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="U11" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="V11" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="W11" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="X11" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="Y11" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="AA11" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AB11" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="AC11" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="AD11" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="AE11">
         <v>97064</v>
       </c>
       <c r="AF11" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="AG11" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="AH11" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AJ11" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL11" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:126">
+    <row r="12" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>43381.74771990741</v>
+        <v>43381.747719907413</v>
       </c>
       <c r="B12">
-        <v>43381.75016203704</v>
+        <v>43381.750162037039</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E12">
         <v>100</v>
@@ -2828,78 +2899,78 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>43381.75016203704</v>
+        <v>43381.750162037039</v>
       </c>
       <c r="I12" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="N12">
-        <v>45.3493957519531</v>
+        <v>45.349395751953097</v>
       </c>
       <c r="O12">
         <v>-117.212799072265</v>
       </c>
       <c r="P12" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="Q12" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R12" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="S12" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="U12" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="V12" t="s">
+        <v>191</v>
+      </c>
+      <c r="W12" t="s">
+        <v>192</v>
+      </c>
+      <c r="X12" t="s">
+        <v>193</v>
+      </c>
+      <c r="Y12" t="s">
         <v>188</v>
       </c>
-      <c r="W12" t="s">
-        <v>189</v>
-      </c>
-      <c r="X12" t="s">
-        <v>190</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>185</v>
-      </c>
       <c r="Z12" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AA12" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AB12" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="AH12" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="AI12" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="AJ12" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL12" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:126">
+    <row r="13" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>43381.7379050926</v>
+        <v>43381.737905092603</v>
       </c>
       <c r="B13">
-        <v>43381.75645833334</v>
+        <v>43381.756458333337</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E13">
         <v>100</v>
@@ -2911,76 +2982,76 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>43381.75645833334</v>
+        <v>43381.756458333337</v>
       </c>
       <c r="I13" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="N13">
-        <v>38.4797058105468</v>
+        <v>38.479705810546797</v>
       </c>
       <c r="O13">
         <v>-121.443801879882</v>
       </c>
       <c r="P13" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="Q13" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R13" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="S13" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="T13">
         <v>1</v>
       </c>
       <c r="U13" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="V13" t="s">
+        <v>204</v>
+      </c>
+      <c r="W13" t="s">
+        <v>205</v>
+      </c>
+      <c r="X13" t="s">
+        <v>206</v>
+      </c>
+      <c r="Y13" t="s">
         <v>201</v>
       </c>
-      <c r="W13" t="s">
-        <v>202</v>
-      </c>
-      <c r="X13" t="s">
-        <v>203</v>
-      </c>
-      <c r="Y13" t="s">
+      <c r="Z13" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>208</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL13" t="s">
         <v>198</v>
       </c>
-      <c r="Z13" t="s">
-        <v>204</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>205</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AJ13" t="s">
-        <v>124</v>
-      </c>
-      <c r="AL13" t="s">
-        <v>195</v>
-      </c>
       <c r="AN13" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AO13" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AP13" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="AQ13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AS13">
         <v>40</v>
@@ -2998,31 +3069,31 @@
         <v>1700</v>
       </c>
       <c r="AX13" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="AY13" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="AZ13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BA13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BB13" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="BD13" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="BE13" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="BF13" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="BH13" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="BJ13">
         <v>240</v>
@@ -3031,7 +3102,7 @@
         <v>300</v>
       </c>
       <c r="BL13" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="BM13">
         <v>5</v>
@@ -3043,159 +3114,168 @@
         <v>500</v>
       </c>
       <c r="BP13" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="BQ13" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="BR13" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="BS13" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BT13" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="BU13" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BV13" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="BW13" t="s">
+        <v>399</v>
+      </c>
+      <c r="BX13" t="s">
+        <v>399</v>
+      </c>
+      <c r="BY13" t="s">
+        <v>398</v>
+      </c>
+      <c r="CA13" t="s">
         <v>396</v>
       </c>
-      <c r="BX13" t="s">
+      <c r="CB13" t="s">
+        <v>400</v>
+      </c>
+      <c r="CC13" t="s">
         <v>396</v>
       </c>
-      <c r="BY13" t="s">
-        <v>395</v>
-      </c>
-      <c r="CA13" t="s">
-        <v>393</v>
-      </c>
-      <c r="CB13" t="s">
-        <v>397</v>
-      </c>
-      <c r="CC13" t="s">
-        <v>393</v>
-      </c>
       <c r="CD13" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="CE13" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="CF13" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="CG13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CH13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CK13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CL13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CM13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CN13" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="CO13" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="CQ13" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="CS13" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="CU13" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="CV13" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="CW13" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="CX13" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="CY13" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="CZ13" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="DA13" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="DB13" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="DC13" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="DD13" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="DE13" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="DF13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DG13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DH13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DI13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DJ13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DK13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DL13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DM13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DN13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DO13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DP13" t="s">
-        <v>123</v>
+        <v>126</v>
+      </c>
+      <c r="DW13" t="s">
+        <v>444</v>
+      </c>
+      <c r="DX13" t="s">
+        <v>445</v>
+      </c>
+      <c r="DY13" t="s">
+        <v>446</v>
       </c>
     </row>
-    <row r="14" spans="1:126">
+    <row r="14" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>43381.87571759259</v>
+        <v>43381.875717592593</v>
       </c>
       <c r="B14">
-        <v>43381.88489583333</v>
+        <v>43381.884895833333</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E14">
         <v>100</v>
@@ -3207,81 +3287,81 @@
         <v>1</v>
       </c>
       <c r="H14">
-        <v>43381.88489583333</v>
+        <v>43381.884895833333</v>
       </c>
       <c r="I14" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="N14">
-        <v>45.5440979003906</v>
+        <v>45.544097900390597</v>
       </c>
       <c r="O14">
-        <v>-122.642303466796</v>
+        <v>-122.64230346679599</v>
       </c>
       <c r="P14" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="Q14" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R14" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="S14" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="U14" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="V14" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="W14" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="X14" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="Y14" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="Z14" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="AA14" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AB14" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="AC14" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="AD14" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="AE14">
         <v>98671</v>
       </c>
       <c r="AF14" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="AG14" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="AH14" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="AJ14" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL14" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:126">
+    <row r="15" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>43382.01947916667</v>
+        <v>43382.019479166673</v>
       </c>
       <c r="B15">
         <v>43382.02648148148</v>
@@ -3290,7 +3370,7 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E15">
         <v>100</v>
@@ -3305,58 +3385,58 @@
         <v>43382.02648148148</v>
       </c>
       <c r="I15" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="N15">
-        <v>48.465103149414</v>
+        <v>48.465103149413999</v>
       </c>
       <c r="O15">
-        <v>7.95590209960937</v>
+        <v>7.9559020996093697</v>
       </c>
       <c r="P15" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="Q15" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R15" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="S15" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="U15" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="V15" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="W15" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="X15" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="Y15" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="Z15" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="AB15" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="AH15" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AJ15" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL15" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:126">
+    <row r="16" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>43382.42454861111</v>
       </c>
@@ -3367,7 +3447,7 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="E16">
         <v>100</v>
@@ -3379,91 +3459,91 @@
         <v>1</v>
       </c>
       <c r="H16">
-        <v>43382.44296296296</v>
+        <v>43382.442962962959</v>
       </c>
       <c r="I16" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="N16">
-        <v>45.0897064208984</v>
+        <v>45.089706420898402</v>
       </c>
       <c r="O16">
         <v>-123.400299072265</v>
       </c>
       <c r="P16" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="Q16" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R16" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="S16" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="T16">
         <v>1</v>
       </c>
       <c r="U16" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="V16" t="s">
+        <v>243</v>
+      </c>
+      <c r="W16" t="s">
+        <v>244</v>
+      </c>
+      <c r="X16" t="s">
+        <v>245</v>
+      </c>
+      <c r="Y16" t="s">
         <v>240</v>
       </c>
-      <c r="W16" t="s">
-        <v>241</v>
-      </c>
-      <c r="X16" t="s">
-        <v>242</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>237</v>
-      </c>
       <c r="Z16" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="AA16" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AB16" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="AC16" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="AD16" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="AE16">
         <v>97367</v>
       </c>
       <c r="AF16" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="AG16" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="AH16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AJ16" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL16" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="AN16" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="AO16" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="AP16" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="AQ16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AS16">
         <v>0</v>
@@ -3475,117 +3555,123 @@
         <v>0</v>
       </c>
       <c r="AX16" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="AY16" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="AZ16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BA16" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="BB16" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="BD16" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="BE16" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="BF16" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="BG16" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="BH16" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="BJ16">
         <v>150</v>
       </c>
       <c r="BK16" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="BL16" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="BM16" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="BN16" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="BP16" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="CG16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CH16" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="CI16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CK16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CL16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CM16" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="CN16" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="CO16" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="CQ16" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="CS16" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="CU16" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="DF16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DH16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DI16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DJ16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DK16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DP16" t="s">
-        <v>123</v>
+        <v>126</v>
+      </c>
+      <c r="DW16" t="s">
+        <v>447</v>
+      </c>
+      <c r="DY16" t="s">
+        <v>448</v>
       </c>
     </row>
-    <row r="17" spans="1:126">
+    <row r="17" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>43382.4278125</v>
+        <v>43382.427812499998</v>
       </c>
       <c r="B17">
-        <v>43382.45159722222</v>
+        <v>43382.451597222222</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E17">
         <v>100</v>
@@ -3597,79 +3683,79 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>43382.4516087963</v>
+        <v>43382.451608796298</v>
       </c>
       <c r="I17" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="N17">
         <v>45.222900390625</v>
       </c>
       <c r="O17">
-        <v>-121.292701721191</v>
+        <v>-121.29270172119099</v>
       </c>
       <c r="P17" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="Q17" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R17" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="S17" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="T17">
         <v>1</v>
       </c>
       <c r="U17" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="V17" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="W17" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="X17" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="Y17" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="Z17" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="AA17" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AB17" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="AH17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AJ17" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL17" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="AN17" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="AO17" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="AP17" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="AQ17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AR17" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="AS17">
         <v>0</v>
@@ -3687,31 +3773,31 @@
         <v>20</v>
       </c>
       <c r="AY17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AZ17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BA17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BB17" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="BD17" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="BE17" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="BF17" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="BG17" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="BH17" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="BJ17">
         <v>150</v>
@@ -3720,141 +3806,147 @@
         <v>50</v>
       </c>
       <c r="BL17" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="BM17" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="BN17" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="BO17" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="BP17" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="BS17" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BT17" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BV17" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="CG17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CH17" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="CK17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CL17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CM17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CN17" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="CO17" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="CQ17" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="CS17" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="CU17" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="CV17" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="CW17" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="CX17" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="CY17" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="CZ17" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="DA17" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="DB17" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="DC17" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="DF17" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="DG17" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="DH17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DI17" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="DJ17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DK17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DL17" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="DM17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DN17" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="DO17" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="DP17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DQ17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DR17" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="DS17" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="DU17" t="s">
-        <v>223</v>
+        <v>226</v>
+      </c>
+      <c r="DW17" t="s">
+        <v>449</v>
+      </c>
+      <c r="DX17" t="s">
+        <v>450</v>
       </c>
     </row>
-    <row r="18" spans="1:126">
+    <row r="18" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>43382.50405092593</v>
+        <v>43382.504050925927</v>
       </c>
       <c r="B18">
-        <v>43382.5228125</v>
+        <v>43382.522812499999</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="E18">
         <v>100</v>
@@ -3866,10 +3958,10 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>43382.52282407408</v>
+        <v>43382.522824074083</v>
       </c>
       <c r="I18" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="N18">
         <v>46.5491943359375</v>
@@ -3878,67 +3970,67 @@
         <v>-121.855499267578</v>
       </c>
       <c r="P18" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="Q18" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R18" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="S18" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="T18">
         <v>2</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="V18" t="s">
+        <v>271</v>
+      </c>
+      <c r="W18" t="s">
+        <v>272</v>
+      </c>
+      <c r="X18" t="s">
+        <v>273</v>
+      </c>
+      <c r="Y18" t="s">
         <v>268</v>
       </c>
-      <c r="W18" t="s">
-        <v>269</v>
-      </c>
-      <c r="X18" t="s">
-        <v>270</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>265</v>
-      </c>
       <c r="Z18" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="AA18" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AB18" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="AH18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AJ18" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL18" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="AN18" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="AO18" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AP18" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AQ18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AR18" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="AS18">
         <v>0</v>
@@ -3956,31 +4048,31 @@
         <v>2900</v>
       </c>
       <c r="AX18" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="AY18" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="AZ18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BA18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BB18" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="BD18">
         <v>68</v>
       </c>
       <c r="BE18" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="BF18" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="BH18" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="BJ18">
         <v>350</v>
@@ -3989,162 +4081,171 @@
         <v>350</v>
       </c>
       <c r="BL18" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="BM18" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="BN18" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="BO18" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="BP18" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="BQ18" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="BR18" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="BS18" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="BT18" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="BV18" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BW18" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="BX18" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="BY18" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="BZ18" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="CG18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CH18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CI18" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="CJ18" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="CK18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CL18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CM18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CN18" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="CO18" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="CP18" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="CQ18" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="CS18" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="CV18" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="CW18" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="CX18" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="CY18" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="CZ18" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="DA18" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="DB18" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="DC18" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="DD18" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="DE18" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="DF18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DG18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DH18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DI18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DJ18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DK18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DL18" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="DM18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DN18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DO18" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="DP18" t="s">
-        <v>223</v>
+        <v>226</v>
+      </c>
+      <c r="DW18" t="s">
+        <v>451</v>
+      </c>
+      <c r="DX18" t="s">
+        <v>452</v>
+      </c>
+      <c r="DY18" t="s">
+        <v>453</v>
       </c>
     </row>
-    <row r="19" spans="1:126">
+    <row r="19" spans="1:129" x14ac:dyDescent="0.25">
       <c r="AN19" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="AO19" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AP19" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AQ19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AR19" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="AS19" s="1">
         <v>0</v>
@@ -4162,33 +4263,33 @@
         <v>700</v>
       </c>
       <c r="AX19" s="1" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="AY19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AZ19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BA19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BB19" s="1" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="BC19" s="1"/>
       <c r="BD19" s="1" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="BE19" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="BF19" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="BG19" s="1"/>
       <c r="BH19" s="1" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="BI19" s="1"/>
       <c r="BJ19" s="1">
@@ -4198,7 +4299,7 @@
         <v>200</v>
       </c>
       <c r="BL19" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="BM19" s="1">
         <v>10</v>
@@ -4207,40 +4308,40 @@
         <v>196</v>
       </c>
       <c r="BO19" s="1" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="BP19" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="BQ19" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="BR19" s="1" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="BS19" s="1" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="BT19" s="1" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="BU19" s="1" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="BV19" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BW19" s="1" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="BX19" s="1" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="BY19" s="1" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="BZ19" s="1" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="CA19" s="1"/>
       <c r="CB19" s="1"/>
@@ -4249,104 +4350,104 @@
       <c r="CE19" s="1"/>
       <c r="CF19" s="1"/>
       <c r="CG19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CH19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CI19" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="CJ19" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="CK19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CL19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CM19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CN19" s="1" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="CO19" s="1" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="CP19" s="1"/>
       <c r="CQ19" s="1" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="CR19" s="1"/>
       <c r="CS19" s="1" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="CT19" s="1"/>
       <c r="CU19" s="1"/>
       <c r="CV19" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="CW19" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="CX19" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="CY19" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="CZ19" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="DA19" s="1" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="DB19" s="1" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="DC19" s="1" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="DD19" s="1" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="DE19" s="1" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="DF19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DG19" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="DH19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DI19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DJ19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DK19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DL19" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="DM19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DN19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DO19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DP19" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="DQ19" s="1"/>
       <c r="DR19" s="1"/>
@@ -4354,19 +4455,28 @@
       <c r="DT19" s="1"/>
       <c r="DU19" s="1"/>
       <c r="DV19" s="1"/>
+      <c r="DW19" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="DX19" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="DY19" s="1" t="s">
+        <v>453</v>
+      </c>
     </row>
-    <row r="21" spans="1:126">
+    <row r="21" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>43382.63195601852</v>
+        <v>43382.631956018522</v>
       </c>
       <c r="B21">
-        <v>43382.63358796296</v>
+        <v>43382.633587962962</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E21">
         <v>100</v>
@@ -4378,90 +4488,90 @@
         <v>1</v>
       </c>
       <c r="H21">
-        <v>43382.63358796296</v>
+        <v>43382.633587962962</v>
       </c>
       <c r="I21" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="N21">
-        <v>44.9490051269531</v>
+        <v>44.949005126953097</v>
       </c>
       <c r="O21">
-        <v>-123.003997802734</v>
+        <v>-123.00399780273401</v>
       </c>
       <c r="P21" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="Q21" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R21" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="S21" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="U21" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="V21" t="s">
+        <v>285</v>
+      </c>
+      <c r="W21" t="s">
+        <v>286</v>
+      </c>
+      <c r="X21" t="s">
+        <v>287</v>
+      </c>
+      <c r="Y21" t="s">
         <v>282</v>
       </c>
-      <c r="W21" t="s">
-        <v>283</v>
-      </c>
-      <c r="X21" t="s">
-        <v>284</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>279</v>
-      </c>
       <c r="Z21" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="AA21" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AB21" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="AC21" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="AD21" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="AE21">
         <v>97383</v>
       </c>
       <c r="AF21" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="AG21" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="AH21" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AJ21" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL21" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:126">
+    <row r="22" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>43383.43930555556</v>
+        <v>43383.439305555563</v>
       </c>
       <c r="B22">
-        <v>43383.45842592593</v>
+        <v>43383.458425925928</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="E22">
         <v>100</v>
@@ -4473,75 +4583,75 @@
         <v>1</v>
       </c>
       <c r="H22">
-        <v>43383.45842592593</v>
+        <v>43383.458425925928</v>
       </c>
       <c r="I22" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="N22">
-        <v>45.9828033447265</v>
+        <v>45.982803344726499</v>
       </c>
       <c r="O22">
         <v>-121.516296386718</v>
       </c>
       <c r="P22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="Q22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R22" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="S22" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="U22" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="V22" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="W22" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="X22" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="Y22" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="Z22" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="AA22" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AB22" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="AH22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AJ22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL22" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
-    <row r="23" spans="1:126">
+    <row r="23" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>43383.49253472222</v>
+        <v>43383.492534722223</v>
       </c>
       <c r="B23">
-        <v>43383.52399305555</v>
+        <v>43383.523993055547</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="E23">
         <v>100</v>
@@ -4553,94 +4663,94 @@
         <v>1</v>
       </c>
       <c r="H23">
-        <v>43383.52400462963</v>
+        <v>43383.524004629631</v>
       </c>
       <c r="I23" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="N23">
-        <v>45.5077972412109</v>
+        <v>45.507797241210902</v>
       </c>
       <c r="O23">
         <v>-122.689697265625</v>
       </c>
       <c r="P23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="Q23" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R23" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="S23" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="T23">
         <v>4</v>
       </c>
       <c r="U23" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="V23" t="s">
+        <v>311</v>
+      </c>
+      <c r="W23" t="s">
+        <v>312</v>
+      </c>
+      <c r="X23" t="s">
+        <v>313</v>
+      </c>
+      <c r="Y23" t="s">
         <v>308</v>
       </c>
-      <c r="W23" t="s">
-        <v>309</v>
-      </c>
-      <c r="X23" t="s">
-        <v>310</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>305</v>
-      </c>
       <c r="Z23" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="AA23" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AB23" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="AC23" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="AD23" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="AE23">
         <v>97112</v>
       </c>
       <c r="AF23" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="AG23" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="AH23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AJ23" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AL23" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="AN23" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="AO23" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="AP23" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="AQ23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AR23" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="AS23">
         <v>0</v>
@@ -4658,34 +4768,34 @@
         <v>2000</v>
       </c>
       <c r="AX23" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="AY23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AZ23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BA23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BB23" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="BD23">
         <v>790</v>
       </c>
       <c r="BE23" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="BF23" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="BG23" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="BH23" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="BJ23">
         <v>600</v>
@@ -4694,118 +4804,118 @@
         <v>0</v>
       </c>
       <c r="BL23" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="BM23" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="BN23" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="BO23" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="BP23" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="BQ23" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="BR23" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="BS23" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BT23" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BU23" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BV23" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BW23" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BX23" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BY23" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BZ23" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="CB23" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="CD23" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="CF23" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="CG23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CH23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CK23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CL23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CM23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CN23" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="CO23" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="CQ23" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="CS23" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="CU23" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="DF23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DG23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DH23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DI23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DK23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:126">
+    <row r="24" spans="1:129" x14ac:dyDescent="0.25">
       <c r="AN24" s="1" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="AO24" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="AP24" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="AQ24" s="1"/>
       <c r="AR24" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="AS24" s="1">
         <v>0</v>
@@ -4823,35 +4933,35 @@
         <v>0</v>
       </c>
       <c r="AX24" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="AY24" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AZ24" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BA24" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BB24" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="BC24" s="1"/>
       <c r="BD24" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="BE24" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="BF24" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="BG24" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="BH24" s="1" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="BI24" s="1"/>
       <c r="BJ24" s="1">
@@ -4861,92 +4971,92 @@
         <v>0</v>
       </c>
       <c r="BL24" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="BM24" s="1" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="BN24" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="BO24" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="BP24" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="BO24" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="BP24" s="1" t="s">
-        <v>377</v>
-      </c>
       <c r="BQ24" s="1" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="BR24" s="1"/>
       <c r="BS24" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BT24" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BU24" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BV24" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BW24" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BX24" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BY24" s="1"/>
       <c r="BZ24" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="CA24" s="1"/>
       <c r="CB24" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="CC24" s="1"/>
       <c r="CD24" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="CE24" s="1"/>
       <c r="CF24" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="CG24" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CH24" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CI24" s="1"/>
       <c r="CJ24" s="1"/>
       <c r="CK24" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CL24" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="CM24" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CN24" s="1" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="CO24" s="1" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="CP24" s="1"/>
       <c r="CQ24" s="1" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="CR24" s="1"/>
       <c r="CS24" s="1" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="CT24" s="1"/>
       <c r="CU24" s="1" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="CV24" s="1"/>
       <c r="CW24" s="1"/>
@@ -4959,16 +5069,16 @@
       <c r="DD24" s="1"/>
       <c r="DE24" s="1"/>
       <c r="DF24" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DG24" s="1"/>
       <c r="DH24" s="1"/>
       <c r="DI24" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DJ24" s="1"/>
       <c r="DK24" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DL24" s="1"/>
       <c r="DM24" s="1"/>
@@ -4981,22 +5091,25 @@
       <c r="DT24" s="1"/>
       <c r="DU24" s="1"/>
       <c r="DV24" s="1"/>
+      <c r="DW24" s="1"/>
+      <c r="DX24" s="1"/>
+      <c r="DY24" s="1"/>
     </row>
-    <row r="25" spans="1:126">
+    <row r="25" spans="1:129" x14ac:dyDescent="0.25">
       <c r="AN25" s="1" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="AO25" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="AP25" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="AQ25" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AR25" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="AS25" s="1">
         <v>0</v>
@@ -5014,33 +5127,33 @@
         <v>0</v>
       </c>
       <c r="AX25" s="1" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="AY25" s="1"/>
       <c r="AZ25" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BA25" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BB25" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="BC25" s="1"/>
       <c r="BD25" s="1">
         <v>640</v>
       </c>
       <c r="BE25" s="1" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="BF25" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="BG25" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="BH25" s="1" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="BI25" s="1"/>
       <c r="BJ25" s="1">
@@ -5050,96 +5163,96 @@
         <v>0</v>
       </c>
       <c r="BL25" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="BM25" s="1" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="BN25" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="BO25" s="1" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="BP25" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="BQ25" s="1" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="BR25" s="1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="BS25" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BT25" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BU25" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BV25" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BW25" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BX25" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BY25" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BZ25" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="CA25" s="1"/>
       <c r="CB25" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="CC25" s="1"/>
       <c r="CD25" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="CE25" s="1"/>
       <c r="CF25" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="CG25" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CH25" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CI25" s="1"/>
       <c r="CJ25" s="1"/>
       <c r="CK25" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="CL25" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CM25" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="CN25" s="1">
         <v>1961</v>
       </c>
       <c r="CO25" s="1" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="CP25" s="1"/>
       <c r="CQ25" s="1" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="CR25" s="1"/>
       <c r="CS25" s="1" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="CT25" s="1"/>
       <c r="CU25" s="1" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="CV25" s="1"/>
       <c r="CW25" s="1"/>
@@ -5152,16 +5265,16 @@
       <c r="DD25" s="1"/>
       <c r="DE25" s="1"/>
       <c r="DF25" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DG25" s="1"/>
       <c r="DH25" s="1"/>
       <c r="DI25" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DJ25" s="1"/>
       <c r="DK25" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DL25" s="1"/>
       <c r="DM25" s="1"/>
@@ -5174,22 +5287,25 @@
       <c r="DT25" s="1"/>
       <c r="DU25" s="1"/>
       <c r="DV25" s="1"/>
+      <c r="DW25" s="1"/>
+      <c r="DX25" s="1"/>
+      <c r="DY25" s="1"/>
     </row>
-    <row r="26" spans="1:126">
+    <row r="26" spans="1:129" x14ac:dyDescent="0.25">
       <c r="AN26" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="AO26" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="AO26" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="AP26" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="AQ26" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AR26" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="AS26" s="1">
         <v>0</v>
@@ -5207,33 +5323,33 @@
         <v>0</v>
       </c>
       <c r="AX26" s="1" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="AY26" s="1"/>
       <c r="AZ26" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BA26" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BB26" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="BC26" s="1"/>
       <c r="BD26" s="1">
         <v>640</v>
       </c>
       <c r="BE26" s="1" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="BF26" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="BG26" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="BH26" s="1" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="BI26" s="1"/>
       <c r="BJ26" s="1">
@@ -5243,100 +5359,100 @@
         <v>0</v>
       </c>
       <c r="BL26" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="BM26" s="1" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="BN26" s="1">
         <v>0</v>
       </c>
       <c r="BO26" s="1" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="BP26" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="BQ26" s="1" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="BR26" s="1" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="BS26" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BT26" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BU26" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BV26" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BW26" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BX26" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BY26" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="BZ26" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="CA26" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="CB26" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="CC26" s="1"/>
       <c r="CD26" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="CE26" s="1"/>
       <c r="CF26" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="CG26" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CH26" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CI26" s="1"/>
       <c r="CJ26" s="1"/>
       <c r="CK26" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CL26" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="CM26" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="CN26" s="1" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="CO26" s="1" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="CP26" s="1"/>
       <c r="CQ26" s="1" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="CR26" s="1"/>
       <c r="CS26" s="1" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="CT26" s="1" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="CU26" s="1" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="CV26" s="1"/>
       <c r="CW26" s="1"/>
@@ -5349,16 +5465,16 @@
       <c r="DD26" s="1"/>
       <c r="DE26" s="1"/>
       <c r="DF26" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DG26" s="1"/>
       <c r="DH26" s="1"/>
       <c r="DI26" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DJ26" s="1"/>
       <c r="DK26" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="DL26" s="1"/>
       <c r="DM26" s="1"/>
@@ -5371,6 +5487,9 @@
       <c r="DT26" s="1"/>
       <c r="DU26" s="1"/>
       <c r="DV26" s="1"/>
+      <c r="DW26" s="1"/>
+      <c r="DX26" s="1"/>
+      <c r="DY26" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added final comments and changed Q4 to intergers
</commit_message>
<xml_diff>
--- a/Anand_Work/FallWork2018/OUTPUT.xlsx
+++ b/Anand_Work/FallWork2018/OUTPUT.xlsx
@@ -4972,10 +4972,10 @@
     </row>
     <row r="2" spans="1:129">
       <c r="A2">
-        <v>43378.46934027778</v>
+        <v>43378.46875</v>
       </c>
       <c r="B2">
-        <v>43378.47023148148</v>
+        <v>43378.47013888889</v>
       </c>
       <c r="C2" t="s">
         <v>121</v>
@@ -4990,16 +4990,16 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>43378.47024305556</v>
+        <v>43378.47013888889</v>
       </c>
       <c r="I2" t="s">
         <v>122</v>
       </c>
       <c r="N2">
-        <v>44.5641937255859</v>
+        <v>44.56419373</v>
       </c>
       <c r="O2">
-        <v>-123.278999328613</v>
+        <v>-123.2789993</v>
       </c>
       <c r="P2" t="s">
         <v>123</v>
@@ -5010,10 +5010,10 @@
     </row>
     <row r="3" spans="1:129">
       <c r="A3">
-        <v>43378.47028935186</v>
+        <v>43378.47013888889</v>
       </c>
       <c r="B3">
-        <v>43378.47060185186</v>
+        <v>43378.47013888889</v>
       </c>
       <c r="C3" t="s">
         <v>121</v>
@@ -5028,16 +5028,16 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>43378.47060185186</v>
+        <v>43378.47013888889</v>
       </c>
       <c r="I3" t="s">
         <v>125</v>
       </c>
       <c r="N3">
-        <v>44.5641937255859</v>
+        <v>44.56419373</v>
       </c>
       <c r="O3">
-        <v>-123.278999328613</v>
+        <v>-123.2789993</v>
       </c>
       <c r="P3" t="s">
         <v>123</v>
@@ -5057,10 +5057,10 @@
     </row>
     <row r="4" spans="1:129">
       <c r="A4">
-        <v>43380.91150462963</v>
+        <v>43380.91111111111</v>
       </c>
       <c r="B4">
-        <v>43380.91293981481</v>
+        <v>43380.9125</v>
       </c>
       <c r="C4" t="s">
         <v>121</v>
@@ -5075,16 +5075,16 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>43380.91295138889</v>
+        <v>43380.9125</v>
       </c>
       <c r="I4" t="s">
         <v>129</v>
       </c>
       <c r="N4">
-        <v>44.5637969970703</v>
+        <v>44.563797</v>
       </c>
       <c r="O4">
-        <v>-123.2779006958</v>
+        <v>-123.2779007</v>
       </c>
       <c r="P4" t="s">
         <v>123</v>
@@ -5129,10 +5129,10 @@
     </row>
     <row r="8" spans="1:129">
       <c r="A8">
-        <v>43381.70964120371</v>
+        <v>43381.70902777778</v>
       </c>
       <c r="B8">
-        <v>43381.71162037037</v>
+        <v>43381.71111111111</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -5150,16 +5150,16 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>43381.71163194445</v>
+        <v>43381.71111111111</v>
       </c>
       <c r="I8" t="s">
         <v>131</v>
       </c>
       <c r="N8">
-        <v>40.7180023193359</v>
+        <v>40.71800232</v>
       </c>
       <c r="O8">
-        <v>-74.0754013061523</v>
+        <v>-74.07540131</v>
       </c>
       <c r="P8" t="s">
         <v>132</v>
@@ -5209,10 +5209,10 @@
     </row>
     <row r="9" spans="1:129">
       <c r="A9">
-        <v>43381.71248842592</v>
+        <v>43381.71180555555</v>
       </c>
       <c r="B9">
-        <v>43381.715</v>
+        <v>43381.71458333333</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -5230,16 +5230,16 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>43381.715</v>
+        <v>43381.71458333333</v>
       </c>
       <c r="I9" t="s">
         <v>143</v>
       </c>
       <c r="N9">
-        <v>45.5653076171875</v>
+        <v>45.56530762</v>
       </c>
       <c r="O9">
-        <v>-122.644798278808</v>
+        <v>-122.6447983</v>
       </c>
       <c r="P9" t="s">
         <v>132</v>
@@ -5304,10 +5304,10 @@
     </row>
     <row r="10" spans="1:129">
       <c r="A10">
-        <v>43381.71474537037</v>
+        <v>43381.71458333333</v>
       </c>
       <c r="B10">
-        <v>43381.71667824074</v>
+        <v>43381.71666666667</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -5325,16 +5325,16 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>43381.71667824074</v>
+        <v>43381.71666666667</v>
       </c>
       <c r="I10" t="s">
         <v>159</v>
       </c>
       <c r="N10">
-        <v>44.0682067871093</v>
+        <v>44.06820679</v>
       </c>
       <c r="O10">
-        <v>-123.081901550292</v>
+        <v>-123.0819016</v>
       </c>
       <c r="P10" t="s">
         <v>132</v>
@@ -5399,10 +5399,10 @@
     </row>
     <row r="11" spans="1:129">
       <c r="A11">
-        <v>43381.71635416667</v>
+        <v>43381.71597222222</v>
       </c>
       <c r="B11">
-        <v>43381.72159722223</v>
+        <v>43381.72152777778</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -5420,16 +5420,16 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>43381.72159722223</v>
+        <v>43381.72152777778</v>
       </c>
       <c r="I11" t="s">
         <v>175</v>
       </c>
       <c r="N11">
-        <v>45.3726959228515</v>
+        <v>45.37269592</v>
       </c>
       <c r="O11">
-        <v>-122.76309967041</v>
+        <v>-122.7630997</v>
       </c>
       <c r="P11" t="s">
         <v>132</v>
@@ -5491,10 +5491,10 @@
     </row>
     <row r="12" spans="1:129">
       <c r="A12">
-        <v>43381.74771990741</v>
+        <v>43381.74722222222</v>
       </c>
       <c r="B12">
-        <v>43381.75016203704</v>
+        <v>43381.75</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
@@ -5512,16 +5512,16 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>43381.75016203704</v>
+        <v>43381.75</v>
       </c>
       <c r="I12" t="s">
         <v>187</v>
       </c>
       <c r="N12">
-        <v>45.3493957519531</v>
+        <v>45.34939575</v>
       </c>
       <c r="O12">
-        <v>-117.212799072265</v>
+        <v>-117.2127991</v>
       </c>
       <c r="P12" t="s">
         <v>132</v>
@@ -5574,10 +5574,10 @@
     </row>
     <row r="13" spans="1:129">
       <c r="A13">
-        <v>43381.7379050926</v>
+        <v>43381.7375</v>
       </c>
       <c r="B13">
-        <v>43381.75645833334</v>
+        <v>43381.75625</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
@@ -5595,16 +5595,16 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>43381.75645833334</v>
+        <v>43381.75625</v>
       </c>
       <c r="I13" t="s">
         <v>200</v>
       </c>
       <c r="N13">
-        <v>38.4797058105468</v>
+        <v>38.47970581</v>
       </c>
       <c r="O13">
-        <v>-121.443801879882</v>
+        <v>-121.4438019</v>
       </c>
       <c r="P13" t="s">
         <v>132</v>
@@ -5879,10 +5879,10 @@
     </row>
     <row r="14" spans="1:129">
       <c r="A14">
-        <v>43381.87571759259</v>
+        <v>43381.87569444445</v>
       </c>
       <c r="B14">
-        <v>43381.88489583333</v>
+        <v>43381.88472222222</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -5900,16 +5900,16 @@
         <v>1</v>
       </c>
       <c r="H14">
-        <v>43381.88489583333</v>
+        <v>43381.88472222222</v>
       </c>
       <c r="I14" t="s">
         <v>213</v>
       </c>
       <c r="N14">
-        <v>45.5440979003906</v>
+        <v>45.5440979</v>
       </c>
       <c r="O14">
-        <v>-122.642303466796</v>
+        <v>-122.6423035</v>
       </c>
       <c r="P14" t="s">
         <v>132</v>
@@ -5974,10 +5974,10 @@
     </row>
     <row r="15" spans="1:129">
       <c r="A15">
-        <v>43382.01947916667</v>
+        <v>43382.01944444444</v>
       </c>
       <c r="B15">
-        <v>43382.02648148148</v>
+        <v>43382.02638888889</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -5995,16 +5995,16 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>43382.02648148148</v>
+        <v>43382.02638888889</v>
       </c>
       <c r="I15" t="s">
         <v>228</v>
       </c>
       <c r="N15">
-        <v>48.465103149414</v>
+        <v>48.46510315</v>
       </c>
       <c r="O15">
-        <v>7.95590209960937</v>
+        <v>7.9559021</v>
       </c>
       <c r="P15" t="s">
         <v>132</v>
@@ -6051,10 +6051,10 @@
     </row>
     <row r="16" spans="1:129">
       <c r="A16">
-        <v>43382.42454861111</v>
+        <v>43382.42430555556</v>
       </c>
       <c r="B16">
-        <v>43382.44295138889</v>
+        <v>43382.44236111111</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -6072,16 +6072,16 @@
         <v>1</v>
       </c>
       <c r="H16">
-        <v>43382.44296296296</v>
+        <v>43382.44236111111</v>
       </c>
       <c r="I16" t="s">
         <v>239</v>
       </c>
       <c r="N16">
-        <v>45.0897064208984</v>
+        <v>45.08970642</v>
       </c>
       <c r="O16">
-        <v>-123.400299072265</v>
+        <v>-123.4002991</v>
       </c>
       <c r="P16" t="s">
         <v>132</v>
@@ -6275,10 +6275,10 @@
     </row>
     <row r="17" spans="1:129">
       <c r="A17">
-        <v>43382.4278125</v>
+        <v>43382.42777777778</v>
       </c>
       <c r="B17">
-        <v>43382.45159722222</v>
+        <v>43382.45138888889</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
@@ -6296,16 +6296,16 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>43382.4516087963</v>
+        <v>43382.45138888889</v>
       </c>
       <c r="I17" t="s">
         <v>252</v>
       </c>
       <c r="N17">
-        <v>45.222900390625</v>
+        <v>45.22290039</v>
       </c>
       <c r="O17">
-        <v>-121.292701721191</v>
+        <v>-121.2927017</v>
       </c>
       <c r="P17" t="s">
         <v>132</v>
@@ -6550,10 +6550,10 @@
     </row>
     <row r="18" spans="1:129">
       <c r="A18">
-        <v>43382.50405092593</v>
+        <v>43382.50347222222</v>
       </c>
       <c r="B18">
-        <v>43382.5228125</v>
+        <v>43382.52222222222</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -6571,16 +6571,16 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>43382.52282407408</v>
+        <v>43382.52222222222</v>
       </c>
       <c r="I18" t="s">
         <v>267</v>
       </c>
       <c r="N18">
-        <v>46.5491943359375</v>
+        <v>46.54919434</v>
       </c>
       <c r="O18">
-        <v>-121.855499267578</v>
+        <v>-121.8554993</v>
       </c>
       <c r="P18" t="s">
         <v>132</v>
@@ -7061,10 +7061,10 @@
     </row>
     <row r="21" spans="1:129">
       <c r="A21">
-        <v>43382.63195601852</v>
+        <v>43382.63194444445</v>
       </c>
       <c r="B21">
-        <v>43382.63358796296</v>
+        <v>43382.63333333333</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
@@ -7082,16 +7082,16 @@
         <v>1</v>
       </c>
       <c r="H21">
-        <v>43382.63358796296</v>
+        <v>43382.63333333333</v>
       </c>
       <c r="I21" t="s">
         <v>281</v>
       </c>
       <c r="N21">
-        <v>44.9490051269531</v>
+        <v>44.94900513</v>
       </c>
       <c r="O21">
-        <v>-123.003997802734</v>
+        <v>-123.0039978</v>
       </c>
       <c r="P21" t="s">
         <v>132</v>
@@ -7156,10 +7156,10 @@
     </row>
     <row r="22" spans="1:129">
       <c r="A22">
-        <v>43383.43930555556</v>
+        <v>43383.43888888889</v>
       </c>
       <c r="B22">
-        <v>43383.45842592593</v>
+        <v>43383.45833333334</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
@@ -7177,16 +7177,16 @@
         <v>1</v>
       </c>
       <c r="H22">
-        <v>43383.45842592593</v>
+        <v>43383.45833333334</v>
       </c>
       <c r="I22" t="s">
         <v>295</v>
       </c>
       <c r="N22">
-        <v>45.9828033447265</v>
+        <v>45.98280334</v>
       </c>
       <c r="O22">
-        <v>-121.516296386718</v>
+        <v>-121.5162964</v>
       </c>
       <c r="P22" t="s">
         <v>132</v>
@@ -7236,10 +7236,10 @@
     </row>
     <row r="23" spans="1:129">
       <c r="A23">
-        <v>43383.49253472222</v>
+        <v>43383.49236111111</v>
       </c>
       <c r="B23">
-        <v>43383.52399305555</v>
+        <v>43383.52361111111</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
@@ -7257,16 +7257,16 @@
         <v>1</v>
       </c>
       <c r="H23">
-        <v>43383.52400462963</v>
+        <v>43383.52361111111</v>
       </c>
       <c r="I23" t="s">
         <v>307</v>
       </c>
       <c r="N23">
-        <v>45.5077972412109</v>
+        <v>45.50779724</v>
       </c>
       <c r="O23">
-        <v>-122.689697265625</v>
+        <v>-122.6896973</v>
       </c>
       <c r="P23" t="s">
         <v>132</v>
@@ -7973,10 +7973,10 @@
     </row>
     <row r="28" spans="1:129">
       <c r="A28">
-        <v>43383.66971064815</v>
+        <v>43383.66944444444</v>
       </c>
       <c r="B28">
-        <v>43383.6724537037</v>
+        <v>43383.67222222222</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
@@ -7994,16 +7994,16 @@
         <v>1</v>
       </c>
       <c r="H28">
-        <v>43383.6724537037</v>
+        <v>43383.67222222222</v>
       </c>
       <c r="I28" t="s">
         <v>325</v>
       </c>
       <c r="N28">
-        <v>44.0184936523437</v>
+        <v>44.01849365</v>
       </c>
       <c r="O28">
-        <v>-123.099800109863</v>
+        <v>-123.0998001</v>
       </c>
       <c r="P28" t="s">
         <v>132</v>
@@ -8068,10 +8068,10 @@
     </row>
     <row r="29" spans="1:129">
       <c r="A29">
-        <v>43383.67261574074</v>
+        <v>43383.67222222222</v>
       </c>
       <c r="B29">
-        <v>43383.67402777778</v>
+        <v>43383.67361111111</v>
       </c>
       <c r="C29" t="s">
         <v>3</v>
@@ -8089,16 +8089,16 @@
         <v>1</v>
       </c>
       <c r="H29">
-        <v>43383.67402777778</v>
+        <v>43383.67361111111</v>
       </c>
       <c r="I29" t="s">
         <v>337</v>
       </c>
       <c r="N29">
-        <v>44.0184936523437</v>
+        <v>44.01849365</v>
       </c>
       <c r="O29">
-        <v>-123.099800109863</v>
+        <v>-123.0998001</v>
       </c>
       <c r="P29" t="s">
         <v>132</v>
@@ -8163,10 +8163,10 @@
     </row>
     <row r="30" spans="1:129">
       <c r="A30">
-        <v>43384.42884259259</v>
+        <v>43384.42847222222</v>
       </c>
       <c r="B30">
-        <v>43384.43192129629</v>
+        <v>43384.43125</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>
@@ -8184,16 +8184,16 @@
         <v>1</v>
       </c>
       <c r="H30">
-        <v>43384.43193287037</v>
+        <v>43384.43125</v>
       </c>
       <c r="I30" t="s">
         <v>339</v>
       </c>
       <c r="N30">
-        <v>44.0928039550781</v>
+        <v>44.09280396</v>
       </c>
       <c r="O30">
-        <v>-121.293594360351</v>
+        <v>-121.2935944</v>
       </c>
       <c r="P30" t="s">
         <v>132</v>
@@ -8258,10 +8258,10 @@
     </row>
     <row r="31" spans="1:129">
       <c r="A31">
-        <v>43385.60166666667</v>
+        <v>43385.60138888889</v>
       </c>
       <c r="B31">
-        <v>43385.60575231481</v>
+        <v>43385.60555555556</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
@@ -8279,16 +8279,16 @@
         <v>1</v>
       </c>
       <c r="H31">
-        <v>43385.60575231481</v>
+        <v>43385.60555555556</v>
       </c>
       <c r="I31" t="s">
         <v>352</v>
       </c>
       <c r="N31">
-        <v>45.5440979003906</v>
+        <v>45.5440979</v>
       </c>
       <c r="O31">
-        <v>-122.642303466796</v>
+        <v>-122.6423035</v>
       </c>
       <c r="P31" t="s">
         <v>132</v>
@@ -8353,10 +8353,10 @@
     </row>
     <row r="32" spans="1:129">
       <c r="A32">
-        <v>43388.43461805556</v>
+        <v>43388.43402777778</v>
       </c>
       <c r="B32">
-        <v>43388.46619212963</v>
+        <v>43388.46597222222</v>
       </c>
       <c r="C32" t="s">
         <v>3</v>
@@ -8374,16 +8374,16 @@
         <v>1</v>
       </c>
       <c r="H32">
-        <v>43388.46620370371</v>
+        <v>43388.46597222222</v>
       </c>
       <c r="I32" t="s">
         <v>357</v>
       </c>
       <c r="N32">
-        <v>45.3303985595703</v>
+        <v>45.33039856</v>
       </c>
       <c r="O32">
-        <v>-118.085205078125</v>
+        <v>-118.0852051</v>
       </c>
       <c r="P32" t="s">
         <v>132</v>
@@ -8652,10 +8652,10 @@
     </row>
     <row r="33" spans="1:129">
       <c r="A33">
-        <v>43388.55427083333</v>
+        <v>43388.55416666667</v>
       </c>
       <c r="B33">
-        <v>43388.56155092592</v>
+        <v>43388.56111111111</v>
       </c>
       <c r="C33" t="s">
         <v>3</v>
@@ -8673,16 +8673,16 @@
         <v>1</v>
       </c>
       <c r="H33">
-        <v>43388.56155092592</v>
+        <v>43388.56111111111</v>
       </c>
       <c r="I33" t="s">
         <v>370</v>
       </c>
       <c r="N33">
-        <v>45.1446075439453</v>
+        <v>45.14460754</v>
       </c>
       <c r="O33">
-        <v>-122.858299255371</v>
+        <v>-122.8582993</v>
       </c>
       <c r="P33" t="s">
         <v>132</v>
@@ -8822,10 +8822,10 @@
     </row>
     <row r="34" spans="1:129">
       <c r="A34">
-        <v>43383.45908564814</v>
+        <v>43383.45902777778</v>
       </c>
       <c r="B34">
-        <v>43388.65328703704</v>
+        <v>43388.65277777778</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
@@ -8843,16 +8843,16 @@
         <v>1</v>
       </c>
       <c r="H34">
-        <v>43388.65329861111</v>
+        <v>43388.65277777778</v>
       </c>
       <c r="I34" t="s">
         <v>380</v>
       </c>
       <c r="N34">
-        <v>45.7550964355468</v>
+        <v>45.75509644</v>
       </c>
       <c r="O34">
-        <v>-121.479499816894</v>
+        <v>-121.4794998</v>
       </c>
       <c r="P34" t="s">
         <v>132</v>
@@ -9133,10 +9133,10 @@
     </row>
     <row r="35" spans="1:129">
       <c r="A35">
-        <v>43388.67149305555</v>
+        <v>43388.67083333333</v>
       </c>
       <c r="B35">
-        <v>43388.67907407408</v>
+        <v>43388.67847222222</v>
       </c>
       <c r="C35" t="s">
         <v>3</v>
@@ -9154,16 +9154,16 @@
         <v>1</v>
       </c>
       <c r="H35">
-        <v>43388.67907407408</v>
+        <v>43388.67847222222</v>
       </c>
       <c r="I35" t="s">
         <v>386</v>
       </c>
       <c r="N35">
-        <v>42.19189453125</v>
+        <v>42.19189453</v>
       </c>
       <c r="O35">
-        <v>-121.724098205566</v>
+        <v>-121.7240982</v>
       </c>
       <c r="P35" t="s">
         <v>132</v>
@@ -9414,10 +9414,10 @@
     </row>
     <row r="36" spans="1:129">
       <c r="A36">
-        <v>43388.64784722222</v>
+        <v>43388.64722222222</v>
       </c>
       <c r="B36">
-        <v>43388.68721064815</v>
+        <v>43388.68680555555</v>
       </c>
       <c r="C36" t="s">
         <v>3</v>
@@ -9435,16 +9435,16 @@
         <v>1</v>
       </c>
       <c r="H36">
-        <v>43388.68721064815</v>
+        <v>43388.68680555555</v>
       </c>
       <c r="I36" t="s">
         <v>399</v>
       </c>
       <c r="N36">
-        <v>44.5637969970703</v>
+        <v>44.563797</v>
       </c>
       <c r="O36">
-        <v>-123.2779006958</v>
+        <v>-123.2779007</v>
       </c>
       <c r="P36" t="s">
         <v>132</v>
@@ -10106,10 +10106,10 @@
     </row>
     <row r="41" spans="1:129">
       <c r="A41">
-        <v>43388.69503472222</v>
+        <v>43388.69444444445</v>
       </c>
       <c r="B41">
-        <v>43388.73453703704</v>
+        <v>43388.73402777778</v>
       </c>
       <c r="C41" t="s">
         <v>3</v>
@@ -10127,16 +10127,16 @@
         <v>1</v>
       </c>
       <c r="H41">
-        <v>43388.73454861111</v>
+        <v>43388.73402777778</v>
       </c>
       <c r="I41" t="s">
         <v>416</v>
       </c>
       <c r="N41">
-        <v>44.5316009521484</v>
+        <v>44.53160095</v>
       </c>
       <c r="O41">
-        <v>-122.882095336914</v>
+        <v>-122.8820953</v>
       </c>
       <c r="P41" t="s">
         <v>132</v>
@@ -10408,10 +10408,10 @@
     </row>
     <row r="42" spans="1:129">
       <c r="A42">
-        <v>43389.65561342592</v>
+        <v>43389.65555555555</v>
       </c>
       <c r="B42">
-        <v>43389.65578703704</v>
+        <v>43389.65555555555</v>
       </c>
       <c r="C42" t="s">
         <v>121</v>
@@ -10426,16 +10426,16 @@
         <v>1</v>
       </c>
       <c r="H42">
-        <v>43389.65578703704</v>
+        <v>43389.65555555555</v>
       </c>
       <c r="I42" t="s">
         <v>429</v>
       </c>
       <c r="N42">
-        <v>44.5637969970703</v>
+        <v>44.563797</v>
       </c>
       <c r="O42">
-        <v>-123.2779006958</v>
+        <v>-123.2779007</v>
       </c>
       <c r="P42" t="s">
         <v>123</v>
@@ -10446,10 +10446,10 @@
     </row>
     <row r="43" spans="1:129">
       <c r="A43">
-        <v>43389.65587962963</v>
+        <v>43389.65555555555</v>
       </c>
       <c r="B43">
-        <v>43389.65600694445</v>
+        <v>43389.65555555555</v>
       </c>
       <c r="C43" t="s">
         <v>121</v>
@@ -10464,16 +10464,16 @@
         <v>1</v>
       </c>
       <c r="H43">
-        <v>43389.65600694445</v>
+        <v>43389.65555555555</v>
       </c>
       <c r="I43" t="s">
         <v>430</v>
       </c>
       <c r="N43">
-        <v>44.5637969970703</v>
+        <v>44.563797</v>
       </c>
       <c r="O43">
-        <v>-123.2779006958</v>
+        <v>-123.2779007</v>
       </c>
       <c r="P43" t="s">
         <v>123</v>
@@ -10484,10 +10484,10 @@
     </row>
     <row r="44" spans="1:129">
       <c r="A44">
-        <v>43389.6575</v>
+        <v>43389.65694444445</v>
       </c>
       <c r="B44">
-        <v>43389.65795138889</v>
+        <v>43389.65763888889</v>
       </c>
       <c r="C44" t="s">
         <v>121</v>
@@ -10502,16 +10502,16 @@
         <v>1</v>
       </c>
       <c r="H44">
-        <v>43389.65796296296</v>
+        <v>43389.65763888889</v>
       </c>
       <c r="I44" t="s">
         <v>431</v>
       </c>
       <c r="N44">
-        <v>44.5637969970703</v>
+        <v>44.563797</v>
       </c>
       <c r="O44">
-        <v>-123.2779006958</v>
+        <v>-123.2779007</v>
       </c>
       <c r="P44" t="s">
         <v>123</v>
@@ -10534,10 +10534,10 @@
     </row>
     <row r="45" spans="1:129">
       <c r="A45">
-        <v>43390.46107638889</v>
+        <v>43390.46041666667</v>
       </c>
       <c r="B45">
-        <v>43390.47539351852</v>
+        <v>43390.475</v>
       </c>
       <c r="C45" t="s">
         <v>3</v>
@@ -10555,16 +10555,16 @@
         <v>1</v>
       </c>
       <c r="H45">
-        <v>43390.47540509259</v>
+        <v>43390.475</v>
       </c>
       <c r="I45" t="s">
         <v>433</v>
       </c>
       <c r="N45">
-        <v>44.5903930664062</v>
+        <v>44.59039307</v>
       </c>
       <c r="O45">
-        <v>-123.272201538085</v>
+        <v>-123.2722015</v>
       </c>
       <c r="P45" t="s">
         <v>132</v>
@@ -10773,10 +10773,10 @@
     </row>
     <row r="46" spans="1:129">
       <c r="A46">
-        <v>43384.48550925926</v>
+        <v>43384.48541666667</v>
       </c>
       <c r="B46">
-        <v>43390.71734953704</v>
+        <v>43390.71666666667</v>
       </c>
       <c r="C46" t="s">
         <v>3</v>
@@ -10800,10 +10800,10 @@
         <v>449</v>
       </c>
       <c r="N46">
-        <v>45.4839935302734</v>
+        <v>45.48399353</v>
       </c>
       <c r="O46">
-        <v>-122.636505126953</v>
+        <v>-122.6365051</v>
       </c>
       <c r="P46" t="s">
         <v>132</v>
@@ -11370,10 +11370,10 @@
     </row>
     <row r="50" spans="1:129">
       <c r="A50">
-        <v>43391.50622685185</v>
+        <v>43391.50555555556</v>
       </c>
       <c r="B50">
-        <v>43391.54001157408</v>
+        <v>43391.53958333333</v>
       </c>
       <c r="C50" t="s">
         <v>3</v>
@@ -11391,16 +11391,16 @@
         <v>1</v>
       </c>
       <c r="H50">
-        <v>43391.54002314815</v>
+        <v>43391.53958333333</v>
       </c>
       <c r="I50" t="s">
         <v>469</v>
       </c>
       <c r="N50">
-        <v>47.6380004882812</v>
+        <v>47.63800049</v>
       </c>
       <c r="O50">
-        <v>-121.911102294921</v>
+        <v>-121.9111023</v>
       </c>
       <c r="P50" t="s">
         <v>132</v>
@@ -11582,10 +11582,10 @@
     </row>
     <row r="51" spans="1:129">
       <c r="A51">
-        <v>43392.47368055556</v>
+        <v>43392.47361111111</v>
       </c>
       <c r="B51">
-        <v>43392.50403935185</v>
+        <v>43392.50347222222</v>
       </c>
       <c r="C51" t="s">
         <v>3</v>
@@ -11603,16 +11603,16 @@
         <v>1</v>
       </c>
       <c r="H51">
-        <v>43392.50405092593</v>
+        <v>43392.50347222222</v>
       </c>
       <c r="I51" t="s">
         <v>482</v>
       </c>
       <c r="N51">
-        <v>47.4185943603515</v>
+        <v>47.41859436</v>
       </c>
       <c r="O51">
-        <v>-120.27310180664</v>
+        <v>-120.2731018</v>
       </c>
       <c r="P51" t="s">
         <v>132</v>
@@ -11848,10 +11848,10 @@
     </row>
     <row r="52" spans="1:129">
       <c r="A52">
-        <v>43395.42516203703</v>
+        <v>43395.425</v>
       </c>
       <c r="B52">
-        <v>43395.51697916666</v>
+        <v>43395.51666666667</v>
       </c>
       <c r="C52" t="s">
         <v>3</v>
@@ -11869,16 +11869,16 @@
         <v>1</v>
       </c>
       <c r="H52">
-        <v>43395.51699074074</v>
+        <v>43395.51666666667</v>
       </c>
       <c r="I52" t="s">
         <v>494</v>
       </c>
       <c r="N52">
-        <v>45.5269927978515</v>
+        <v>45.5269928</v>
       </c>
       <c r="O52">
-        <v>-122.685394287109</v>
+        <v>-122.6853943</v>
       </c>
       <c r="P52" t="s">
         <v>132</v>
@@ -12108,10 +12108,10 @@
     </row>
     <row r="53" spans="1:129">
       <c r="A53">
-        <v>43396.65813657407</v>
+        <v>43396.65763888889</v>
       </c>
       <c r="B53">
-        <v>43396.66050925926</v>
+        <v>43396.66041666667</v>
       </c>
       <c r="C53" t="s">
         <v>121</v>
@@ -12126,16 +12126,16 @@
         <v>1</v>
       </c>
       <c r="H53">
-        <v>43396.66052083333</v>
+        <v>43396.66041666667</v>
       </c>
       <c r="I53" t="s">
         <v>510</v>
       </c>
       <c r="N53">
-        <v>44.5637969970703</v>
+        <v>44.563797</v>
       </c>
       <c r="O53">
-        <v>-123.2779006958</v>
+        <v>-123.2779007</v>
       </c>
       <c r="P53" t="s">
         <v>123</v>
@@ -12266,10 +12266,10 @@
     </row>
     <row r="54" spans="1:129">
       <c r="A54">
-        <v>43396.76164351852</v>
+        <v>43396.76111111111</v>
       </c>
       <c r="B54">
-        <v>43396.76456018518</v>
+        <v>43396.76388888889</v>
       </c>
       <c r="C54" t="s">
         <v>3</v>
@@ -12287,16 +12287,16 @@
         <v>1</v>
       </c>
       <c r="H54">
-        <v>43396.76456018518</v>
+        <v>43396.76388888889</v>
       </c>
       <c r="I54" t="s">
         <v>523</v>
       </c>
       <c r="N54">
-        <v>44.3981018066406</v>
+        <v>44.39810181</v>
       </c>
       <c r="O54">
-        <v>-122.728599548339</v>
+        <v>-122.7285995</v>
       </c>
       <c r="P54" t="s">
         <v>132</v>
@@ -12355,10 +12355,10 @@
     </row>
     <row r="55" spans="1:129">
       <c r="A55">
-        <v>43396.74315972222</v>
+        <v>43396.74305555555</v>
       </c>
       <c r="B55">
-        <v>43396.76746527778</v>
+        <v>43396.76736111111</v>
       </c>
       <c r="C55" t="s">
         <v>3</v>
@@ -12376,16 +12376,16 @@
         <v>1</v>
       </c>
       <c r="H55">
-        <v>43396.76746527778</v>
+        <v>43396.76736111111</v>
       </c>
       <c r="I55" t="s">
         <v>531</v>
       </c>
       <c r="N55">
-        <v>45.5411071777343</v>
+        <v>45.54110718</v>
       </c>
       <c r="O55">
-        <v>-122.556594848632</v>
+        <v>-122.5565948</v>
       </c>
       <c r="P55" t="s">
         <v>132</v>
@@ -12633,10 +12633,10 @@
     </row>
     <row r="56" spans="1:129">
       <c r="A56">
-        <v>43396.76329861111</v>
+        <v>43396.76319444444</v>
       </c>
       <c r="B56">
-        <v>43396.76888888889</v>
+        <v>43396.76875</v>
       </c>
       <c r="C56" t="s">
         <v>3</v>
@@ -12654,16 +12654,16 @@
         <v>1</v>
       </c>
       <c r="H56">
-        <v>43396.76890046296</v>
+        <v>43396.76875</v>
       </c>
       <c r="I56" t="s">
         <v>546</v>
       </c>
       <c r="N56">
-        <v>46.252197265625</v>
+        <v>46.25219727</v>
       </c>
       <c r="O56">
-        <v>-119.287994384765</v>
+        <v>-119.2879944</v>
       </c>
       <c r="P56" t="s">
         <v>132</v>
@@ -12845,10 +12845,10 @@
     </row>
     <row r="57" spans="1:129">
       <c r="A57">
-        <v>43397.59631944444</v>
+        <v>43397.59583333333</v>
       </c>
       <c r="B57">
-        <v>43397.61958333333</v>
+        <v>43397.61944444444</v>
       </c>
       <c r="C57" t="s">
         <v>3</v>
@@ -12866,16 +12866,16 @@
         <v>1</v>
       </c>
       <c r="H57">
-        <v>43397.61959490741</v>
+        <v>43397.61944444444</v>
       </c>
       <c r="I57" t="s">
         <v>563</v>
       </c>
       <c r="N57">
-        <v>45.3789978027343</v>
+        <v>45.3789978</v>
       </c>
       <c r="O57">
-        <v>-122.222999572753</v>
+        <v>-122.2229996</v>
       </c>
       <c r="P57" t="s">
         <v>132</v>
@@ -13030,10 +13030,10 @@
     </row>
     <row r="58" spans="1:129">
       <c r="A58">
-        <v>43397.69358796296</v>
+        <v>43397.69305555556</v>
       </c>
       <c r="B58">
-        <v>43397.6965162037</v>
+        <v>43397.69583333333</v>
       </c>
       <c r="C58" t="s">
         <v>3</v>
@@ -13051,16 +13051,16 @@
         <v>1</v>
       </c>
       <c r="H58">
-        <v>43397.6965162037</v>
+        <v>43397.69583333333</v>
       </c>
       <c r="I58" t="s">
         <v>576</v>
       </c>
       <c r="N58">
-        <v>45.5234069824218</v>
+        <v>45.52340698</v>
       </c>
       <c r="O58">
-        <v>-122.676200866699</v>
+        <v>-122.6762009</v>
       </c>
       <c r="P58" t="s">
         <v>132</v>
@@ -13113,10 +13113,10 @@
     </row>
     <row r="59" spans="1:129">
       <c r="A59">
-        <v>43398.42032407408</v>
+        <v>43398.42013888889</v>
       </c>
       <c r="B59">
-        <v>43398.42452546296</v>
+        <v>43398.42430555556</v>
       </c>
       <c r="C59" t="s">
         <v>3</v>
@@ -13134,16 +13134,16 @@
         <v>1</v>
       </c>
       <c r="H59">
-        <v>43398.42453703703</v>
+        <v>43398.42430555556</v>
       </c>
       <c r="I59" t="s">
         <v>586</v>
       </c>
       <c r="N59">
-        <v>44.5903930664062</v>
+        <v>44.59039307</v>
       </c>
       <c r="O59">
-        <v>-123.272201538085</v>
+        <v>-123.2722015</v>
       </c>
       <c r="P59" t="s">
         <v>132</v>
@@ -13158,7 +13158,7 @@
         <v>588</v>
       </c>
       <c r="T59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U59" t="s">
         <v>589</v>
@@ -13196,10 +13196,10 @@
     </row>
     <row r="60" spans="1:129">
       <c r="A60">
-        <v>43399.73417824074</v>
+        <v>43399.73402777778</v>
       </c>
       <c r="B60">
-        <v>43399.7675</v>
+        <v>43399.76736111111</v>
       </c>
       <c r="C60" t="s">
         <v>3</v>
@@ -13217,16 +13217,16 @@
         <v>1</v>
       </c>
       <c r="H60">
-        <v>43399.7675</v>
+        <v>43399.76736111111</v>
       </c>
       <c r="I60" t="s">
         <v>597</v>
       </c>
       <c r="N60">
-        <v>45.5440979003906</v>
+        <v>45.5440979</v>
       </c>
       <c r="O60">
-        <v>-122.642303466796</v>
+        <v>-122.6423035</v>
       </c>
       <c r="P60" t="s">
         <v>132</v>
@@ -13501,10 +13501,10 @@
     </row>
     <row r="61" spans="1:129">
       <c r="A61">
-        <v>43399.62726851852</v>
+        <v>43399.62708333333</v>
       </c>
       <c r="B61">
-        <v>43399.8755787037</v>
+        <v>43399.875</v>
       </c>
       <c r="C61" t="s">
         <v>3</v>
@@ -13522,16 +13522,16 @@
         <v>1</v>
       </c>
       <c r="H61">
-        <v>43399.87559027778</v>
+        <v>43399.875</v>
       </c>
       <c r="I61" t="s">
         <v>603</v>
       </c>
       <c r="N61">
-        <v>37.7509002685546</v>
+        <v>37.75090027</v>
       </c>
       <c r="O61">
-        <v>-122.415298461914</v>
+        <v>-122.4152985</v>
       </c>
       <c r="P61" t="s">
         <v>132</v>
@@ -13779,7 +13779,7 @@
         <v>43399.86319444444</v>
       </c>
       <c r="B62">
-        <v>43399.90440972222</v>
+        <v>43399.90416666667</v>
       </c>
       <c r="C62" t="s">
         <v>3</v>
@@ -13797,16 +13797,16 @@
         <v>1</v>
       </c>
       <c r="H62">
-        <v>43399.9044212963</v>
+        <v>43399.90416666667</v>
       </c>
       <c r="I62" t="s">
         <v>609</v>
       </c>
       <c r="N62">
-        <v>42.5296936035156</v>
+        <v>42.5296936</v>
       </c>
       <c r="O62">
-        <v>-123.439300537109</v>
+        <v>-123.4393005</v>
       </c>
       <c r="P62" t="s">
         <v>132</v>
@@ -14072,10 +14072,10 @@
     </row>
     <row r="63" spans="1:129">
       <c r="A63">
-        <v>43402.50016203704</v>
+        <v>43402.5</v>
       </c>
       <c r="B63">
-        <v>43402.50239583333</v>
+        <v>43402.50208333333</v>
       </c>
       <c r="C63" t="s">
         <v>3</v>
@@ -14093,16 +14093,16 @@
         <v>1</v>
       </c>
       <c r="H63">
-        <v>43402.50239583333</v>
+        <v>43402.50208333333</v>
       </c>
       <c r="I63" t="s">
         <v>623</v>
       </c>
       <c r="N63">
-        <v>44.5637969970703</v>
+        <v>44.563797</v>
       </c>
       <c r="O63">
-        <v>-123.2779006958</v>
+        <v>-123.2779007</v>
       </c>
       <c r="P63" t="s">
         <v>132</v>
@@ -14389,10 +14389,10 @@
     </row>
     <row r="64" spans="1:129">
       <c r="A64">
-        <v>43382.66173611111</v>
+        <v>43382.66111111111</v>
       </c>
       <c r="B64">
-        <v>43402.53230324074</v>
+        <v>43402.53194444445</v>
       </c>
       <c r="C64" t="s">
         <v>3</v>
@@ -14410,16 +14410,16 @@
         <v>1</v>
       </c>
       <c r="H64">
-        <v>43402.53232638889</v>
+        <v>43402.53194444445</v>
       </c>
       <c r="I64" t="s">
         <v>638</v>
       </c>
       <c r="N64">
-        <v>44.9225006103515</v>
+        <v>44.92250061</v>
       </c>
       <c r="O64">
-        <v>-123.319999694824</v>
+        <v>-123.3199997</v>
       </c>
       <c r="P64" t="s">
         <v>132</v>
@@ -14679,10 +14679,10 @@
     </row>
     <row r="65" spans="1:129">
       <c r="A65">
-        <v>43402.61456018518</v>
+        <v>43402.61388888889</v>
       </c>
       <c r="B65">
-        <v>43402.61547453704</v>
+        <v>43402.61527777778</v>
       </c>
       <c r="C65" t="s">
         <v>121</v>
@@ -14697,16 +14697,16 @@
         <v>1</v>
       </c>
       <c r="H65">
-        <v>43402.61548611111</v>
+        <v>43402.61527777778</v>
       </c>
       <c r="I65" t="s">
         <v>653</v>
       </c>
       <c r="N65">
-        <v>44.0184936523437</v>
+        <v>44.01849365</v>
       </c>
       <c r="O65">
-        <v>-123.099800109863</v>
+        <v>-123.0998001</v>
       </c>
       <c r="P65" t="s">
         <v>123</v>
@@ -14717,10 +14717,10 @@
     </row>
     <row r="66" spans="1:129">
       <c r="A66">
-        <v>43402.7240625</v>
+        <v>43402.72361111111</v>
       </c>
       <c r="B66">
-        <v>43402.7294675926</v>
+        <v>43402.72916666666</v>
       </c>
       <c r="C66" t="s">
         <v>3</v>
@@ -14738,16 +14738,16 @@
         <v>1</v>
       </c>
       <c r="H66">
-        <v>43402.72947916666</v>
+        <v>43402.72916666666</v>
       </c>
       <c r="I66" t="s">
         <v>655</v>
       </c>
       <c r="N66">
-        <v>37.7510070800781</v>
+        <v>37.75100708</v>
       </c>
       <c r="O66">
-        <v>-97.82199859619141</v>
+        <v>-97.8219986</v>
       </c>
       <c r="P66" t="s">
         <v>132</v>
@@ -14800,10 +14800,10 @@
     </row>
     <row r="67" spans="1:129">
       <c r="A67">
-        <v>43402.72006944445</v>
+        <v>43402.71944444445</v>
       </c>
       <c r="B67">
-        <v>43402.74366898148</v>
+        <v>43402.74305555555</v>
       </c>
       <c r="C67" t="s">
         <v>3</v>
@@ -14821,16 +14821,16 @@
         <v>1</v>
       </c>
       <c r="H67">
-        <v>43402.74368055556</v>
+        <v>43402.74305555555</v>
       </c>
       <c r="I67" t="s">
         <v>665</v>
       </c>
       <c r="N67">
-        <v>44.5316009521484</v>
+        <v>44.53160095</v>
       </c>
       <c r="O67">
-        <v>-122.882095336914</v>
+        <v>-122.8820953</v>
       </c>
       <c r="P67" t="s">
         <v>132</v>
@@ -15078,7 +15078,7 @@
     </row>
     <row r="68" spans="1:129">
       <c r="A68">
-        <v>43402.73627314815</v>
+        <v>43402.73611111111</v>
       </c>
       <c r="B68">
         <v>43402.75763888889</v>
@@ -15105,10 +15105,10 @@
         <v>680</v>
       </c>
       <c r="N68">
-        <v>42.3363037109375</v>
+        <v>42.33630371</v>
       </c>
       <c r="O68">
-        <v>-122.839797973632</v>
+        <v>-122.839798</v>
       </c>
       <c r="P68" t="s">
         <v>132</v>
@@ -15383,10 +15383,10 @@
     </row>
     <row r="69" spans="1:129">
       <c r="A69">
-        <v>43402.98583333333</v>
+        <v>43402.98541666667</v>
       </c>
       <c r="B69">
-        <v>43402.98880787037</v>
+        <v>43402.98819444444</v>
       </c>
       <c r="C69" t="s">
         <v>3</v>
@@ -15404,16 +15404,16 @@
         <v>1</v>
       </c>
       <c r="H69">
-        <v>43402.98880787037</v>
+        <v>43402.98819444444</v>
       </c>
       <c r="I69" t="s">
         <v>689</v>
       </c>
       <c r="N69">
-        <v>45.3377075195312</v>
+        <v>45.33770752</v>
       </c>
       <c r="O69">
-        <v>-122.569999694824</v>
+        <v>-122.5699997</v>
       </c>
       <c r="P69" t="s">
         <v>132</v>
@@ -15466,10 +15466,10 @@
     </row>
     <row r="70" spans="1:129">
       <c r="A70">
-        <v>43403.45685185185</v>
+        <v>43403.45625</v>
       </c>
       <c r="B70">
-        <v>43403.50322916666</v>
+        <v>43403.50277777778</v>
       </c>
       <c r="C70" t="s">
         <v>3</v>
@@ -15487,16 +15487,16 @@
         <v>1</v>
       </c>
       <c r="H70">
-        <v>43403.50324074074</v>
+        <v>43403.50277777778</v>
       </c>
       <c r="I70" t="s">
         <v>699</v>
       </c>
       <c r="N70">
-        <v>45.8450012207031</v>
+        <v>45.84500122</v>
       </c>
       <c r="O70">
-        <v>-119.284896850585</v>
+        <v>-119.2848969</v>
       </c>
       <c r="P70" t="s">
         <v>132</v>
@@ -15753,10 +15753,10 @@
     </row>
     <row r="71" spans="1:129">
       <c r="A71">
-        <v>43403.46539351852</v>
+        <v>43403.46527777778</v>
       </c>
       <c r="B71">
-        <v>43403.50910879629</v>
+        <v>43403.50902777778</v>
       </c>
       <c r="C71" t="s">
         <v>3</v>
@@ -15774,16 +15774,16 @@
         <v>1</v>
       </c>
       <c r="H71">
-        <v>43403.50912037037</v>
+        <v>43403.50902777778</v>
       </c>
       <c r="I71" t="s">
         <v>714</v>
       </c>
       <c r="N71">
-        <v>45.2872009277343</v>
+        <v>45.28720093</v>
       </c>
       <c r="O71">
-        <v>-122.325897216796</v>
+        <v>-122.3258972</v>
       </c>
       <c r="P71" t="s">
         <v>132</v>
@@ -16019,10 +16019,10 @@
     </row>
     <row r="72" spans="1:129">
       <c r="A72">
-        <v>43403.53085648148</v>
+        <v>43403.53055555555</v>
       </c>
       <c r="B72">
-        <v>43403.53268518519</v>
+        <v>43403.53263888889</v>
       </c>
       <c r="C72" t="s">
         <v>3</v>
@@ -16040,16 +16040,16 @@
         <v>1</v>
       </c>
       <c r="H72">
-        <v>43403.53269675926</v>
+        <v>43403.53263888889</v>
       </c>
       <c r="I72" t="s">
         <v>723</v>
       </c>
       <c r="N72">
-        <v>44.0682067871093</v>
+        <v>44.06820679</v>
       </c>
       <c r="O72">
-        <v>-123.081901550292</v>
+        <v>-123.0819016</v>
       </c>
       <c r="P72" t="s">
         <v>132</v>
@@ -16114,10 +16114,10 @@
     </row>
     <row r="73" spans="1:129">
       <c r="A73">
-        <v>43403.59113425926</v>
+        <v>43403.59097222222</v>
       </c>
       <c r="B73">
-        <v>43403.62091435185</v>
+        <v>43403.62083333333</v>
       </c>
       <c r="C73" t="s">
         <v>3</v>
@@ -16135,16 +16135,16 @@
         <v>1</v>
       </c>
       <c r="H73">
-        <v>43403.62092592593</v>
+        <v>43403.62083333333</v>
       </c>
       <c r="I73" t="s">
         <v>731</v>
       </c>
       <c r="N73">
-        <v>44.9089050292968</v>
+        <v>44.90890503</v>
       </c>
       <c r="O73">
-        <v>-123.988800048828</v>
+        <v>-123.9888</v>
       </c>
       <c r="P73" t="s">
         <v>132</v>
@@ -16332,10 +16332,10 @@
     </row>
     <row r="74" spans="1:129">
       <c r="A74">
-        <v>43404.65027777778</v>
+        <v>43404.65</v>
       </c>
       <c r="B74">
-        <v>43404.67226851852</v>
+        <v>43404.67222222222</v>
       </c>
       <c r="C74" t="s">
         <v>3</v>
@@ -16353,16 +16353,16 @@
         <v>1</v>
       </c>
       <c r="H74">
-        <v>43404.67228009259</v>
+        <v>43404.67222222222</v>
       </c>
       <c r="I74" t="s">
         <v>742</v>
       </c>
       <c r="N74">
-        <v>44.0682067871093</v>
+        <v>44.06820679</v>
       </c>
       <c r="O74">
-        <v>-123.081901550292</v>
+        <v>-123.0819016</v>
       </c>
       <c r="P74" t="s">
         <v>132</v>
@@ -16643,10 +16643,10 @@
     </row>
     <row r="75" spans="1:129">
       <c r="A75">
-        <v>43404.63613425926</v>
+        <v>43404.63611111111</v>
       </c>
       <c r="B75">
-        <v>43404.70621527778</v>
+        <v>43404.70555555556</v>
       </c>
       <c r="C75" t="s">
         <v>3</v>
@@ -16664,16 +16664,16 @@
         <v>1</v>
       </c>
       <c r="H75">
-        <v>43404.70622685185</v>
+        <v>43404.70555555556</v>
       </c>
       <c r="I75" t="s">
         <v>755</v>
       </c>
       <c r="N75">
-        <v>44.0612030029296</v>
+        <v>44.061203</v>
       </c>
       <c r="O75">
-        <v>-123.155502319335</v>
+        <v>-123.1555023</v>
       </c>
       <c r="P75" t="s">
         <v>132</v>
@@ -16933,10 +16933,10 @@
     </row>
     <row r="76" spans="1:129">
       <c r="A76">
-        <v>43405.44184027778</v>
+        <v>43405.44166666667</v>
       </c>
       <c r="B76">
-        <v>43405.60787037037</v>
+        <v>43405.60763888889</v>
       </c>
       <c r="C76" t="s">
         <v>3</v>
@@ -16954,16 +16954,16 @@
         <v>1</v>
       </c>
       <c r="H76">
-        <v>43405.60787037037</v>
+        <v>43405.60763888889</v>
       </c>
       <c r="I76" t="s">
         <v>769</v>
       </c>
       <c r="N76">
-        <v>44.0682067871093</v>
+        <v>44.06820679</v>
       </c>
       <c r="O76">
-        <v>-123.081901550292</v>
+        <v>-123.0819016</v>
       </c>
       <c r="P76" t="s">
         <v>132</v>
@@ -17013,10 +17013,10 @@
     </row>
     <row r="77" spans="1:129">
       <c r="A77">
-        <v>43410.53413194444</v>
+        <v>43410.53402777778</v>
       </c>
       <c r="B77">
-        <v>43410.53725694444</v>
+        <v>43410.53680555556</v>
       </c>
       <c r="C77" t="s">
         <v>3</v>
@@ -17034,16 +17034,16 @@
         <v>1</v>
       </c>
       <c r="H77">
-        <v>43410.53725694444</v>
+        <v>43410.53680555556</v>
       </c>
       <c r="I77" t="s">
         <v>778</v>
       </c>
       <c r="N77">
-        <v>43.2297058105468</v>
+        <v>43.22970581</v>
       </c>
       <c r="O77">
-        <v>-123.234298706054</v>
+        <v>-123.2342987</v>
       </c>
       <c r="P77" t="s">
         <v>132</v>

</xml_diff>